<commit_message>
Andrew | Added 3 more states for licensing.
</commit_message>
<xml_diff>
--- a/compliance/State Compliance Analysis.xlsx
+++ b/compliance/State Compliance Analysis.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/andrewhetzler/Documents/Documents - Andrew’s Money Maker/School/DISSERTATION/GitHub/dissertation/compliance/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F9619B52-A097-CC47-916B-55985AE40E0C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F1915C8D-00DA-4847-8D09-806972B0BA5D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="40960" windowHeight="24400" activeTab="1" xr2:uid="{FEE3D6CA-2CD0-2B4F-9478-6397B247951E}"/>
   </bookViews>
@@ -17,6 +17,11 @@
     <sheet name="Driver License" sheetId="2" r:id="rId2"/>
     <sheet name="Registration" sheetId="3" r:id="rId3"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'Driver License'!$A$1:$A$110</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Insurance!$A$1:$A$51</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">Registration!$A$1:$A$51</definedName>
+  </definedNames>
   <calcPr calcId="181029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -38,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="679" uniqueCount="182">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="865" uniqueCount="211">
   <si>
     <t>STATE</t>
   </si>
@@ -911,12 +916,162 @@
   <si>
     <t>Optional (RS 32:401(7)(C )(1)(a)</t>
   </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Required (63-1-35(1)) </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>NOTE</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>: It's named driver license #</t>
+    </r>
+  </si>
+  <si>
+    <t>Required (63-1-35(1))</t>
+  </si>
+  <si>
+    <t>Optional--only required if sex offender (63-1-35(3))</t>
+  </si>
+  <si>
+    <t>Optoinal (63-1-35(4))</t>
+  </si>
+  <si>
+    <t>Required (63-1-39)</t>
+  </si>
+  <si>
+    <t>Required (20-7(n)(1)</t>
+  </si>
+  <si>
+    <t>Required (20-7(n)(2)</t>
+  </si>
+  <si>
+    <t>Required (20-7(n)(3)</t>
+  </si>
+  <si>
+    <t>Required (20-7(n)(4)</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Required (20-7(n)(5) </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Aptos Narrow"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>NOTE:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Aptos Narrow"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> must include sex, height, eye color, and hair color</t>
+    </r>
+  </si>
+  <si>
+    <t>Required (20-7(n)(6)</t>
+  </si>
+  <si>
+    <t>Required (20-7(n)(7)</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Required (20-7(n)(8) </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Aptos Narrow"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Note:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Aptos Narrow"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> may contain multiple classes</t>
+    </r>
+  </si>
+  <si>
+    <t>Required (20-7(n)(9)</t>
+  </si>
+  <si>
+    <t>Required (20-7(n)(10)</t>
+  </si>
+  <si>
+    <t>Optional--only required if under 21 (20-7(n)</t>
+  </si>
+  <si>
+    <t>RACE</t>
+  </si>
+  <si>
+    <t>Optional (20-7(n)</t>
+  </si>
+  <si>
+    <t>ACTIVE DUTY DISTINCTION</t>
+  </si>
+  <si>
+    <t>Optional (20-7(q))</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Optional (20-7(q)(1))</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Optional (20-7(q)(2))</t>
+  </si>
+  <si>
+    <t>Required (39-06-14(1))</t>
+  </si>
+  <si>
+    <t>Required (39-06-14(3))</t>
+  </si>
+  <si>
+    <t>Required (39-06-14(2))</t>
+  </si>
+  <si>
+    <t>Required (39-06-14(4))</t>
+  </si>
+  <si>
+    <t>ALIEN DISTINCTION</t>
+  </si>
+  <si>
+    <t>Optional--only required if alien  (39-06-14(5))</t>
+  </si>
+  <si>
+    <t>Optional (39-06-14(6))</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -942,6 +1097,19 @@
       <color rgb="FF000000"/>
       <name val="Aptos Narrow"/>
       <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Aptos Narrow"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Aptos Narrow"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -1319,7 +1487,8 @@
   <dimension ref="A1:A51"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:A51"/>
+      <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" sqref="A1:A1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1580,16 +1749,19 @@
       </c>
     </row>
   </sheetData>
+  <autoFilter ref="A1:A51" xr:uid="{4E61F571-54A4-994C-A02B-889943573726}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7F37C204-69FB-8946-B201-7E43976BBF53}">
-  <dimension ref="A1:AY110"/>
+  <sheetPr filterMode="1"/>
+  <dimension ref="A1:AZ110"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AJ1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="AX19" sqref="AX19"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <pane xSplit="1" topLeftCell="AM1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="AZ35" sqref="AZ2:AZ35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1642,9 +1814,11 @@
     <col min="47" max="47" width="26.1640625" customWidth="1"/>
     <col min="48" max="48" width="20.6640625" customWidth="1"/>
     <col min="49" max="49" width="15.33203125" customWidth="1"/>
+    <col min="50" max="51" width="24" customWidth="1"/>
+    <col min="52" max="52" width="23.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:51" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:52" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1792,8 +1966,17 @@
       <c r="AW1" s="1" t="s">
         <v>180</v>
       </c>
-    </row>
-    <row r="2" spans="1:51" ht="51" x14ac:dyDescent="0.2">
+      <c r="AX1" s="1" t="s">
+        <v>198</v>
+      </c>
+      <c r="AY1" s="1" t="s">
+        <v>200</v>
+      </c>
+      <c r="AZ1" s="1" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="2" spans="1:52" ht="51" x14ac:dyDescent="0.2">
       <c r="A2" s="3" t="s">
         <v>9</v>
       </c>
@@ -1941,10 +2124,17 @@
       <c r="AW2" s="2" t="s">
         <v>80</v>
       </c>
-      <c r="AX2" s="2"/>
-      <c r="AY2" s="2"/>
-    </row>
-    <row r="3" spans="1:51" x14ac:dyDescent="0.2">
+      <c r="AX2" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="AY2" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="AZ2" s="2" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="3" spans="1:52" hidden="1" x14ac:dyDescent="0.2">
       <c r="A3" s="3" t="s">
         <v>10</v>
       </c>
@@ -1999,7 +2189,7 @@
       <c r="AX3" s="2"/>
       <c r="AY3" s="2"/>
     </row>
-    <row r="4" spans="1:51" ht="51" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:52" ht="51" x14ac:dyDescent="0.2">
       <c r="A4" s="3" t="s">
         <v>11</v>
       </c>
@@ -2147,10 +2337,17 @@
       <c r="AW4" s="2" t="s">
         <v>80</v>
       </c>
-      <c r="AX4" s="2"/>
-      <c r="AY4" s="2"/>
-    </row>
-    <row r="5" spans="1:51" ht="68" x14ac:dyDescent="0.2">
+      <c r="AX4" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="AY4" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="AZ4" s="2" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="5" spans="1:52" ht="68" x14ac:dyDescent="0.2">
       <c r="A5" s="3" t="s">
         <v>12</v>
       </c>
@@ -2294,10 +2491,17 @@
       <c r="AW5" s="2" t="s">
         <v>80</v>
       </c>
-      <c r="AX5" s="2"/>
-      <c r="AY5" s="2"/>
-    </row>
-    <row r="6" spans="1:51" ht="68" x14ac:dyDescent="0.2">
+      <c r="AX5" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="AY5" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="AZ5" s="2" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="6" spans="1:52" ht="68" x14ac:dyDescent="0.2">
       <c r="A6" s="3" t="s">
         <v>13</v>
       </c>
@@ -2445,10 +2649,17 @@
       <c r="AW6" s="2" t="s">
         <v>80</v>
       </c>
-      <c r="AX6" s="2"/>
-      <c r="AY6" s="2"/>
-    </row>
-    <row r="7" spans="1:51" x14ac:dyDescent="0.2">
+      <c r="AX6" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="AY6" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="AZ6" s="2" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="7" spans="1:52" hidden="1" x14ac:dyDescent="0.2">
       <c r="A7" s="3" t="s">
         <v>14</v>
       </c>
@@ -2503,7 +2714,7 @@
       <c r="AX7" s="2"/>
       <c r="AY7" s="2"/>
     </row>
-    <row r="8" spans="1:51" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:52" hidden="1" x14ac:dyDescent="0.2">
       <c r="A8" s="3" t="s">
         <v>58</v>
       </c>
@@ -2558,7 +2769,7 @@
       <c r="AX8" s="2"/>
       <c r="AY8" s="2"/>
     </row>
-    <row r="9" spans="1:51" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:52" hidden="1" x14ac:dyDescent="0.2">
       <c r="A9" s="3" t="s">
         <v>15</v>
       </c>
@@ -2613,7 +2824,7 @@
       <c r="AX9" s="2"/>
       <c r="AY9" s="2"/>
     </row>
-    <row r="10" spans="1:51" ht="85" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:52" ht="85" x14ac:dyDescent="0.2">
       <c r="A10" s="3" t="s">
         <v>16</v>
       </c>
@@ -2761,10 +2972,17 @@
       <c r="AW10" s="2" t="s">
         <v>80</v>
       </c>
-      <c r="AX10" s="2"/>
-      <c r="AY10" s="2"/>
-    </row>
-    <row r="11" spans="1:51" ht="68" x14ac:dyDescent="0.2">
+      <c r="AX10" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="AY10" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="AZ10" s="2" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="11" spans="1:52" ht="68" x14ac:dyDescent="0.2">
       <c r="A11" s="3" t="s">
         <v>17</v>
       </c>
@@ -2912,10 +3130,17 @@
       <c r="AW11" s="2" t="s">
         <v>80</v>
       </c>
-      <c r="AX11" s="2"/>
-      <c r="AY11" s="2"/>
-    </row>
-    <row r="12" spans="1:51" x14ac:dyDescent="0.2">
+      <c r="AX11" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="AY11" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="AZ11" s="2" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="12" spans="1:52" hidden="1" x14ac:dyDescent="0.2">
       <c r="A12" s="3" t="s">
         <v>18</v>
       </c>
@@ -2970,7 +3195,7 @@
       <c r="AX12" s="2"/>
       <c r="AY12" s="2"/>
     </row>
-    <row r="13" spans="1:51" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:52" hidden="1" x14ac:dyDescent="0.2">
       <c r="A13" s="3" t="s">
         <v>21</v>
       </c>
@@ -3025,7 +3250,7 @@
       <c r="AX13" s="2"/>
       <c r="AY13" s="2"/>
     </row>
-    <row r="14" spans="1:51" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:52" hidden="1" x14ac:dyDescent="0.2">
       <c r="A14" s="3" t="s">
         <v>19</v>
       </c>
@@ -3080,7 +3305,7 @@
       <c r="AX14" s="2"/>
       <c r="AY14" s="2"/>
     </row>
-    <row r="15" spans="1:51" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:52" hidden="1" x14ac:dyDescent="0.2">
       <c r="A15" s="3" t="s">
         <v>20</v>
       </c>
@@ -3135,7 +3360,7 @@
       <c r="AX15" s="2"/>
       <c r="AY15" s="2"/>
     </row>
-    <row r="16" spans="1:51" ht="68" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:52" ht="68" x14ac:dyDescent="0.2">
       <c r="A16" s="3" t="s">
         <v>22</v>
       </c>
@@ -3283,10 +3508,17 @@
       <c r="AW16" s="2" t="s">
         <v>80</v>
       </c>
-      <c r="AX16" s="2"/>
-      <c r="AY16" s="2"/>
-    </row>
-    <row r="17" spans="1:51" ht="68" x14ac:dyDescent="0.2">
+      <c r="AX16" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="AY16" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="AZ16" s="2" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="17" spans="1:52" ht="68" x14ac:dyDescent="0.2">
       <c r="A17" s="3" t="s">
         <v>23</v>
       </c>
@@ -3434,10 +3666,17 @@
       <c r="AW17" s="2" t="s">
         <v>80</v>
       </c>
-      <c r="AX17" s="2"/>
-      <c r="AY17" s="2"/>
-    </row>
-    <row r="18" spans="1:51" ht="119" x14ac:dyDescent="0.2">
+      <c r="AX17" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="AY17" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="AZ17" s="2" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="18" spans="1:52" ht="119" x14ac:dyDescent="0.2">
       <c r="A18" s="3" t="s">
         <v>24</v>
       </c>
@@ -3585,10 +3824,17 @@
       <c r="AW18" s="2" t="s">
         <v>80</v>
       </c>
-      <c r="AX18" s="2"/>
-      <c r="AY18" s="2"/>
-    </row>
-    <row r="19" spans="1:51" ht="51" x14ac:dyDescent="0.2">
+      <c r="AX18" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="AY18" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="AZ18" s="2" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="19" spans="1:52" ht="51" x14ac:dyDescent="0.2">
       <c r="A19" s="3" t="s">
         <v>25</v>
       </c>
@@ -3736,10 +3982,17 @@
       <c r="AW19" s="2" t="s">
         <v>181</v>
       </c>
-      <c r="AX19" s="2"/>
-      <c r="AY19" s="2"/>
-    </row>
-    <row r="20" spans="1:51" x14ac:dyDescent="0.2">
+      <c r="AX19" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="AY19" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="AZ19" s="2" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="20" spans="1:52" hidden="1" x14ac:dyDescent="0.2">
       <c r="A20" s="3" t="s">
         <v>26</v>
       </c>
@@ -3794,7 +4047,7 @@
       <c r="AX20" s="2"/>
       <c r="AY20" s="2"/>
     </row>
-    <row r="21" spans="1:51" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:52" hidden="1" x14ac:dyDescent="0.2">
       <c r="A21" s="3" t="s">
         <v>27</v>
       </c>
@@ -3849,7 +4102,7 @@
       <c r="AX21" s="2"/>
       <c r="AY21" s="2"/>
     </row>
-    <row r="22" spans="1:51" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:52" hidden="1" x14ac:dyDescent="0.2">
       <c r="A22" s="3" t="s">
         <v>28</v>
       </c>
@@ -3904,7 +4157,7 @@
       <c r="AX22" s="2"/>
       <c r="AY22" s="2"/>
     </row>
-    <row r="23" spans="1:51" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:52" hidden="1" x14ac:dyDescent="0.2">
       <c r="A23" s="3" t="s">
         <v>29</v>
       </c>
@@ -3959,7 +4212,7 @@
       <c r="AX23" s="2"/>
       <c r="AY23" s="2"/>
     </row>
-    <row r="24" spans="1:51" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:52" hidden="1" x14ac:dyDescent="0.2">
       <c r="A24" s="3" t="s">
         <v>30</v>
       </c>
@@ -4014,62 +4267,165 @@
       <c r="AX24" s="2"/>
       <c r="AY24" s="2"/>
     </row>
-    <row r="25" spans="1:51" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:52" ht="34" x14ac:dyDescent="0.2">
       <c r="A25" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="B25" s="2"/>
-      <c r="C25" s="2"/>
-      <c r="D25" s="2"/>
-      <c r="E25" s="2"/>
-      <c r="F25" s="2"/>
-      <c r="G25" s="2"/>
-      <c r="H25" s="2"/>
-      <c r="I25" s="2"/>
-      <c r="J25" s="2"/>
-      <c r="K25" s="2"/>
-      <c r="L25" s="2"/>
-      <c r="M25" s="2"/>
-      <c r="N25" s="2"/>
-      <c r="O25" s="2"/>
-      <c r="P25" s="2"/>
-      <c r="Q25" s="2"/>
-      <c r="R25" s="2"/>
-      <c r="S25" s="2"/>
-      <c r="T25" s="2"/>
-      <c r="U25" s="2"/>
-      <c r="V25" s="2"/>
-      <c r="W25" s="2"/>
-      <c r="X25" s="2"/>
-      <c r="Y25" s="2"/>
-      <c r="Z25" s="2"/>
-      <c r="AA25" s="2"/>
-      <c r="AB25" s="2"/>
-      <c r="AC25" s="2"/>
-      <c r="AD25" s="2"/>
-      <c r="AE25" s="2"/>
-      <c r="AF25" s="2"/>
-      <c r="AG25" s="2"/>
-      <c r="AH25" s="2"/>
-      <c r="AI25" s="2"/>
-      <c r="AJ25" s="2"/>
-      <c r="AK25" s="2"/>
-      <c r="AL25" s="2"/>
-      <c r="AM25" s="2"/>
-      <c r="AN25" s="2"/>
-      <c r="AO25" s="2"/>
-      <c r="AP25" s="2"/>
-      <c r="AQ25" s="2"/>
-      <c r="AR25" s="2"/>
-      <c r="AS25" s="2"/>
-      <c r="AT25" s="2"/>
-      <c r="AU25" s="2"/>
-      <c r="AV25" s="2"/>
-      <c r="AW25" s="2"/>
-      <c r="AX25" s="2"/>
-      <c r="AY25" s="2"/>
-    </row>
-    <row r="26" spans="1:51" x14ac:dyDescent="0.2">
+      <c r="B25" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="C25" s="2" t="s">
+        <v>182</v>
+      </c>
+      <c r="D25" s="2" t="s">
+        <v>183</v>
+      </c>
+      <c r="E25" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="F25" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="G25" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="H25" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="I25" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="J25" s="2" t="s">
+        <v>186</v>
+      </c>
+      <c r="K25" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="L25" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="M25" s="2" t="s">
+        <v>185</v>
+      </c>
+      <c r="N25" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="O25" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="P25" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="Q25" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="R25" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="S25" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="T25" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="U25" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="V25" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="W25" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="X25" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="Y25" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="Z25" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="AA25" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="AB25" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="AC25" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="AD25" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="AE25" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="AF25" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="AG25" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="AH25" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="AI25" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="AJ25" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="AK25" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="AL25" s="2" t="s">
+        <v>184</v>
+      </c>
+      <c r="AM25" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="AN25" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="AO25" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="AP25" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="AQ25" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="AR25" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="AS25" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="AT25" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="AU25" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="AV25" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="AW25" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="AX25" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="AY25" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="AZ25" s="2" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="26" spans="1:52" hidden="1" x14ac:dyDescent="0.2">
       <c r="A26" s="3" t="s">
         <v>32</v>
       </c>
@@ -4124,7 +4480,7 @@
       <c r="AX26" s="2"/>
       <c r="AY26" s="2"/>
     </row>
-    <row r="27" spans="1:51" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:52" hidden="1" x14ac:dyDescent="0.2">
       <c r="A27" s="3" t="s">
         <v>33</v>
       </c>
@@ -4179,7 +4535,7 @@
       <c r="AX27" s="2"/>
       <c r="AY27" s="2"/>
     </row>
-    <row r="28" spans="1:51" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:52" hidden="1" x14ac:dyDescent="0.2">
       <c r="A28" s="3" t="s">
         <v>34</v>
       </c>
@@ -4234,7 +4590,7 @@
       <c r="AX28" s="2"/>
       <c r="AY28" s="2"/>
     </row>
-    <row r="29" spans="1:51" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:52" hidden="1" x14ac:dyDescent="0.2">
       <c r="A29" s="3" t="s">
         <v>35</v>
       </c>
@@ -4289,7 +4645,7 @@
       <c r="AX29" s="2"/>
       <c r="AY29" s="2"/>
     </row>
-    <row r="30" spans="1:51" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:52" hidden="1" x14ac:dyDescent="0.2">
       <c r="A30" s="3" t="s">
         <v>36</v>
       </c>
@@ -4344,7 +4700,7 @@
       <c r="AX30" s="2"/>
       <c r="AY30" s="2"/>
     </row>
-    <row r="31" spans="1:51" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:52" hidden="1" x14ac:dyDescent="0.2">
       <c r="A31" s="3" t="s">
         <v>37</v>
       </c>
@@ -4399,7 +4755,7 @@
       <c r="AX31" s="2"/>
       <c r="AY31" s="2"/>
     </row>
-    <row r="32" spans="1:51" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:52" hidden="1" x14ac:dyDescent="0.2">
       <c r="A32" s="3" t="s">
         <v>38</v>
       </c>
@@ -4454,7 +4810,7 @@
       <c r="AX32" s="2"/>
       <c r="AY32" s="2"/>
     </row>
-    <row r="33" spans="1:51" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:52" hidden="1" x14ac:dyDescent="0.2">
       <c r="A33" s="3" t="s">
         <v>39</v>
       </c>
@@ -4509,117 +4865,323 @@
       <c r="AX33" s="2"/>
       <c r="AY33" s="2"/>
     </row>
-    <row r="34" spans="1:51" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:52" ht="51" x14ac:dyDescent="0.2">
       <c r="A34" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="B34" s="2"/>
-      <c r="C34" s="2"/>
-      <c r="D34" s="2"/>
-      <c r="E34" s="2"/>
-      <c r="F34" s="2"/>
-      <c r="G34" s="2"/>
-      <c r="H34" s="2"/>
-      <c r="I34" s="2"/>
-      <c r="J34" s="2"/>
-      <c r="K34" s="2"/>
-      <c r="L34" s="2"/>
-      <c r="M34" s="2"/>
-      <c r="N34" s="2"/>
-      <c r="O34" s="2"/>
-      <c r="P34" s="2"/>
-      <c r="Q34" s="2"/>
-      <c r="R34" s="2"/>
-      <c r="S34" s="2"/>
-      <c r="T34" s="2"/>
-      <c r="U34" s="2"/>
-      <c r="V34" s="2"/>
-      <c r="W34" s="2"/>
-      <c r="X34" s="2"/>
-      <c r="Y34" s="2"/>
-      <c r="Z34" s="2"/>
-      <c r="AA34" s="2"/>
-      <c r="AB34" s="2"/>
-      <c r="AC34" s="2"/>
-      <c r="AD34" s="2"/>
-      <c r="AE34" s="2"/>
-      <c r="AF34" s="2"/>
-      <c r="AG34" s="2"/>
-      <c r="AH34" s="2"/>
-      <c r="AI34" s="2"/>
-      <c r="AJ34" s="2"/>
-      <c r="AK34" s="2"/>
-      <c r="AL34" s="2"/>
-      <c r="AM34" s="2"/>
-      <c r="AN34" s="2"/>
-      <c r="AO34" s="2"/>
-      <c r="AP34" s="2"/>
-      <c r="AQ34" s="2"/>
-      <c r="AR34" s="2"/>
-      <c r="AS34" s="2"/>
-      <c r="AT34" s="2"/>
-      <c r="AU34" s="2"/>
-      <c r="AV34" s="2"/>
-      <c r="AW34" s="2"/>
-      <c r="AX34" s="2"/>
-      <c r="AY34" s="2"/>
-    </row>
-    <row r="35" spans="1:51" x14ac:dyDescent="0.2">
+      <c r="B34" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="C34" s="2" t="s">
+        <v>193</v>
+      </c>
+      <c r="D34" s="4" t="s">
+        <v>190</v>
+      </c>
+      <c r="E34" s="2" t="s">
+        <v>188</v>
+      </c>
+      <c r="F34" s="4" t="s">
+        <v>192</v>
+      </c>
+      <c r="G34" s="2" t="s">
+        <v>189</v>
+      </c>
+      <c r="H34" s="4" t="s">
+        <v>191</v>
+      </c>
+      <c r="I34" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="J34" s="4" t="s">
+        <v>195</v>
+      </c>
+      <c r="K34" s="4" t="s">
+        <v>194</v>
+      </c>
+      <c r="L34" s="4" t="s">
+        <v>194</v>
+      </c>
+      <c r="M34" s="2" t="s">
+        <v>202</v>
+      </c>
+      <c r="N34" s="2" t="s">
+        <v>197</v>
+      </c>
+      <c r="O34" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="P34" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="Q34" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="R34" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="S34" s="2" t="s">
+        <v>196</v>
+      </c>
+      <c r="T34" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="U34" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="V34" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="W34" s="4" t="s">
+        <v>187</v>
+      </c>
+      <c r="X34" s="2" t="s">
+        <v>196</v>
+      </c>
+      <c r="Y34" s="2" t="s">
+        <v>203</v>
+      </c>
+      <c r="Z34" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="AA34" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="AB34" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="AC34" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="AD34" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="AE34" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="AF34" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="AG34" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="AH34" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="AI34" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="AJ34" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="AK34" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="AL34" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="AM34" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="AN34" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="AO34" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="AP34" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="AQ34" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="AR34" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="AS34" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="AT34" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="AU34" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="AV34" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="AW34" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="AX34" s="2" t="s">
+        <v>199</v>
+      </c>
+      <c r="AY34" s="2" t="s">
+        <v>201</v>
+      </c>
+      <c r="AZ34" s="2" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="35" spans="1:52" ht="34" x14ac:dyDescent="0.2">
       <c r="A35" s="3" t="s">
         <v>41</v>
       </c>
-      <c r="B35" s="2"/>
-      <c r="C35" s="2"/>
-      <c r="D35" s="2"/>
-      <c r="E35" s="2"/>
-      <c r="F35" s="2"/>
-      <c r="G35" s="2"/>
-      <c r="H35" s="2"/>
-      <c r="I35" s="2"/>
-      <c r="J35" s="2"/>
-      <c r="K35" s="2"/>
-      <c r="L35" s="2"/>
-      <c r="M35" s="2"/>
-      <c r="N35" s="2"/>
-      <c r="O35" s="2"/>
-      <c r="P35" s="2"/>
-      <c r="Q35" s="2"/>
-      <c r="R35" s="2"/>
-      <c r="S35" s="2"/>
-      <c r="T35" s="2"/>
-      <c r="U35" s="2"/>
-      <c r="V35" s="2"/>
-      <c r="W35" s="2"/>
-      <c r="X35" s="2"/>
-      <c r="Y35" s="2"/>
-      <c r="Z35" s="2"/>
-      <c r="AA35" s="2"/>
-      <c r="AB35" s="2"/>
-      <c r="AC35" s="2"/>
-      <c r="AD35" s="2"/>
-      <c r="AE35" s="2"/>
-      <c r="AF35" s="2"/>
-      <c r="AG35" s="2"/>
-      <c r="AH35" s="2"/>
-      <c r="AI35" s="2"/>
-      <c r="AJ35" s="2"/>
-      <c r="AK35" s="2"/>
-      <c r="AL35" s="2"/>
-      <c r="AM35" s="2"/>
-      <c r="AN35" s="2"/>
-      <c r="AO35" s="2"/>
-      <c r="AP35" s="2"/>
-      <c r="AQ35" s="2"/>
-      <c r="AR35" s="2"/>
-      <c r="AS35" s="2"/>
-      <c r="AT35" s="2"/>
-      <c r="AU35" s="2"/>
-      <c r="AV35" s="2"/>
-      <c r="AW35" s="2"/>
-      <c r="AX35" s="2"/>
-      <c r="AY35" s="2"/>
-    </row>
-    <row r="36" spans="1:51" x14ac:dyDescent="0.2">
+      <c r="B35" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="C35" s="2" t="s">
+        <v>205</v>
+      </c>
+      <c r="D35" s="2" t="s">
+        <v>207</v>
+      </c>
+      <c r="E35" s="2" t="s">
+        <v>204</v>
+      </c>
+      <c r="F35" s="2" t="s">
+        <v>204</v>
+      </c>
+      <c r="G35" s="2" t="s">
+        <v>204</v>
+      </c>
+      <c r="H35" s="2" t="s">
+        <v>204</v>
+      </c>
+      <c r="I35" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="J35" s="2" t="s">
+        <v>206</v>
+      </c>
+      <c r="K35" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="L35" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="M35" s="2" t="s">
+        <v>210</v>
+      </c>
+      <c r="N35" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="O35" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="P35" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="Q35" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="R35" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="S35" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="T35" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="U35" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="V35" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="W35" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="X35" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="Y35" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="Z35" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="AA35" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="AB35" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="AC35" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="AD35" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="AE35" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="AF35" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="AG35" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="AH35" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="AI35" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="AJ35" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="AK35" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="AL35" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="AM35" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="AN35" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="AO35" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="AP35" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="AQ35" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="AR35" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="AS35" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="AT35" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="AU35" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="AV35" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="AW35" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="AX35" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="AY35" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="AZ35" s="3" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="36" spans="1:52" hidden="1" x14ac:dyDescent="0.2">
       <c r="A36" s="3" t="s">
         <v>42</v>
       </c>
@@ -4674,7 +5236,7 @@
       <c r="AX36" s="2"/>
       <c r="AY36" s="2"/>
     </row>
-    <row r="37" spans="1:51" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:52" x14ac:dyDescent="0.2">
       <c r="A37" s="3" t="s">
         <v>43</v>
       </c>
@@ -4728,8 +5290,9 @@
       <c r="AW37" s="2"/>
       <c r="AX37" s="2"/>
       <c r="AY37" s="2"/>
-    </row>
-    <row r="38" spans="1:51" x14ac:dyDescent="0.2">
+      <c r="AZ37" s="3"/>
+    </row>
+    <row r="38" spans="1:52" hidden="1" x14ac:dyDescent="0.2">
       <c r="A38" s="3" t="s">
         <v>44</v>
       </c>
@@ -4784,7 +5347,7 @@
       <c r="AX38" s="2"/>
       <c r="AY38" s="2"/>
     </row>
-    <row r="39" spans="1:51" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:52" x14ac:dyDescent="0.2">
       <c r="A39" s="3" t="s">
         <v>45</v>
       </c>
@@ -4838,8 +5401,9 @@
       <c r="AW39" s="2"/>
       <c r="AX39" s="2"/>
       <c r="AY39" s="2"/>
-    </row>
-    <row r="40" spans="1:51" x14ac:dyDescent="0.2">
+      <c r="AZ39" s="3"/>
+    </row>
+    <row r="40" spans="1:52" hidden="1" x14ac:dyDescent="0.2">
       <c r="A40" s="3" t="s">
         <v>46</v>
       </c>
@@ -4894,7 +5458,7 @@
       <c r="AX40" s="2"/>
       <c r="AY40" s="2"/>
     </row>
-    <row r="41" spans="1:51" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:52" hidden="1" x14ac:dyDescent="0.2">
       <c r="A41" s="3" t="s">
         <v>47</v>
       </c>
@@ -4949,7 +5513,7 @@
       <c r="AX41" s="2"/>
       <c r="AY41" s="2"/>
     </row>
-    <row r="42" spans="1:51" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:52" x14ac:dyDescent="0.2">
       <c r="A42" s="3" t="s">
         <v>48</v>
       </c>
@@ -5003,8 +5567,9 @@
       <c r="AW42" s="2"/>
       <c r="AX42" s="2"/>
       <c r="AY42" s="2"/>
-    </row>
-    <row r="43" spans="1:51" x14ac:dyDescent="0.2">
+      <c r="AZ42" s="3"/>
+    </row>
+    <row r="43" spans="1:52" hidden="1" x14ac:dyDescent="0.2">
       <c r="A43" s="3" t="s">
         <v>49</v>
       </c>
@@ -5059,7 +5624,7 @@
       <c r="AX43" s="2"/>
       <c r="AY43" s="2"/>
     </row>
-    <row r="44" spans="1:51" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:52" x14ac:dyDescent="0.2">
       <c r="A44" s="3" t="s">
         <v>50</v>
       </c>
@@ -5113,8 +5678,9 @@
       <c r="AW44" s="2"/>
       <c r="AX44" s="2"/>
       <c r="AY44" s="2"/>
-    </row>
-    <row r="45" spans="1:51" x14ac:dyDescent="0.2">
+      <c r="AZ44" s="3"/>
+    </row>
+    <row r="45" spans="1:52" x14ac:dyDescent="0.2">
       <c r="A45" s="3" t="s">
         <v>51</v>
       </c>
@@ -5168,8 +5734,9 @@
       <c r="AW45" s="2"/>
       <c r="AX45" s="2"/>
       <c r="AY45" s="2"/>
-    </row>
-    <row r="46" spans="1:51" x14ac:dyDescent="0.2">
+      <c r="AZ45" s="3"/>
+    </row>
+    <row r="46" spans="1:52" x14ac:dyDescent="0.2">
       <c r="A46" s="3" t="s">
         <v>52</v>
       </c>
@@ -5223,8 +5790,9 @@
       <c r="AW46" s="2"/>
       <c r="AX46" s="2"/>
       <c r="AY46" s="2"/>
-    </row>
-    <row r="47" spans="1:51" x14ac:dyDescent="0.2">
+      <c r="AZ46" s="3"/>
+    </row>
+    <row r="47" spans="1:52" hidden="1" x14ac:dyDescent="0.2">
       <c r="A47" s="3" t="s">
         <v>53</v>
       </c>
@@ -5279,7 +5847,7 @@
       <c r="AX47" s="2"/>
       <c r="AY47" s="2"/>
     </row>
-    <row r="48" spans="1:51" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:52" hidden="1" x14ac:dyDescent="0.2">
       <c r="A48" s="3" t="s">
         <v>54</v>
       </c>
@@ -5334,7 +5902,7 @@
       <c r="AX48" s="2"/>
       <c r="AY48" s="2"/>
     </row>
-    <row r="49" spans="1:51" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:52" x14ac:dyDescent="0.2">
       <c r="A49" s="3" t="s">
         <v>55</v>
       </c>
@@ -5388,8 +5956,9 @@
       <c r="AW49" s="2"/>
       <c r="AX49" s="2"/>
       <c r="AY49" s="2"/>
-    </row>
-    <row r="50" spans="1:51" x14ac:dyDescent="0.2">
+      <c r="AZ49" s="3"/>
+    </row>
+    <row r="50" spans="1:52" hidden="1" x14ac:dyDescent="0.2">
       <c r="A50" s="3" t="s">
         <v>57</v>
       </c>
@@ -5444,7 +6013,7 @@
       <c r="AX50" s="2"/>
       <c r="AY50" s="2"/>
     </row>
-    <row r="51" spans="1:51" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:52" hidden="1" x14ac:dyDescent="0.2">
       <c r="A51" s="3" t="s">
         <v>56</v>
       </c>
@@ -5499,7 +6068,7 @@
       <c r="AX51" s="2"/>
       <c r="AY51" s="2"/>
     </row>
-    <row r="52" spans="1:51" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:52" x14ac:dyDescent="0.2">
       <c r="B52" s="2"/>
       <c r="C52" s="2"/>
       <c r="D52" s="2"/>
@@ -5550,8 +6119,9 @@
       <c r="AW52" s="2"/>
       <c r="AX52" s="2"/>
       <c r="AY52" s="2"/>
-    </row>
-    <row r="53" spans="1:51" x14ac:dyDescent="0.2">
+      <c r="AZ52" s="3"/>
+    </row>
+    <row r="53" spans="1:52" x14ac:dyDescent="0.2">
       <c r="B53" s="2"/>
       <c r="C53" s="2"/>
       <c r="D53" s="2"/>
@@ -5602,8 +6172,9 @@
       <c r="AW53" s="2"/>
       <c r="AX53" s="2"/>
       <c r="AY53" s="2"/>
-    </row>
-    <row r="54" spans="1:51" x14ac:dyDescent="0.2">
+      <c r="AZ53" s="3"/>
+    </row>
+    <row r="54" spans="1:52" x14ac:dyDescent="0.2">
       <c r="B54" s="2"/>
       <c r="C54" s="2"/>
       <c r="D54" s="2"/>
@@ -5654,8 +6225,9 @@
       <c r="AW54" s="2"/>
       <c r="AX54" s="2"/>
       <c r="AY54" s="2"/>
-    </row>
-    <row r="55" spans="1:51" x14ac:dyDescent="0.2">
+      <c r="AZ54" s="3"/>
+    </row>
+    <row r="55" spans="1:52" x14ac:dyDescent="0.2">
       <c r="B55" s="2"/>
       <c r="C55" s="2"/>
       <c r="D55" s="2"/>
@@ -5706,8 +6278,9 @@
       <c r="AW55" s="2"/>
       <c r="AX55" s="2"/>
       <c r="AY55" s="2"/>
-    </row>
-    <row r="56" spans="1:51" x14ac:dyDescent="0.2">
+      <c r="AZ55" s="3"/>
+    </row>
+    <row r="56" spans="1:52" x14ac:dyDescent="0.2">
       <c r="B56" s="2"/>
       <c r="C56" s="2"/>
       <c r="D56" s="2"/>
@@ -5758,8 +6331,9 @@
       <c r="AW56" s="2"/>
       <c r="AX56" s="2"/>
       <c r="AY56" s="2"/>
-    </row>
-    <row r="57" spans="1:51" x14ac:dyDescent="0.2">
+      <c r="AZ56" s="3"/>
+    </row>
+    <row r="57" spans="1:52" x14ac:dyDescent="0.2">
       <c r="B57" s="2"/>
       <c r="C57" s="2"/>
       <c r="D57" s="2"/>
@@ -5810,8 +6384,9 @@
       <c r="AW57" s="2"/>
       <c r="AX57" s="2"/>
       <c r="AY57" s="2"/>
-    </row>
-    <row r="58" spans="1:51" x14ac:dyDescent="0.2">
+      <c r="AZ57" s="3"/>
+    </row>
+    <row r="58" spans="1:52" x14ac:dyDescent="0.2">
       <c r="B58" s="2"/>
       <c r="C58" s="2"/>
       <c r="D58" s="2"/>
@@ -5862,8 +6437,9 @@
       <c r="AW58" s="2"/>
       <c r="AX58" s="2"/>
       <c r="AY58" s="2"/>
-    </row>
-    <row r="59" spans="1:51" x14ac:dyDescent="0.2">
+      <c r="AZ58" s="3"/>
+    </row>
+    <row r="59" spans="1:52" x14ac:dyDescent="0.2">
       <c r="B59" s="2"/>
       <c r="C59" s="2"/>
       <c r="D59" s="2"/>
@@ -5914,8 +6490,9 @@
       <c r="AW59" s="2"/>
       <c r="AX59" s="2"/>
       <c r="AY59" s="2"/>
-    </row>
-    <row r="60" spans="1:51" x14ac:dyDescent="0.2">
+      <c r="AZ59" s="3"/>
+    </row>
+    <row r="60" spans="1:52" x14ac:dyDescent="0.2">
       <c r="B60" s="2"/>
       <c r="C60" s="2"/>
       <c r="D60" s="2"/>
@@ -5966,8 +6543,9 @@
       <c r="AW60" s="2"/>
       <c r="AX60" s="2"/>
       <c r="AY60" s="2"/>
-    </row>
-    <row r="61" spans="1:51" x14ac:dyDescent="0.2">
+      <c r="AZ60" s="3"/>
+    </row>
+    <row r="61" spans="1:52" x14ac:dyDescent="0.2">
       <c r="B61" s="2"/>
       <c r="C61" s="2"/>
       <c r="D61" s="2"/>
@@ -6018,119 +6596,140 @@
       <c r="AW61" s="2"/>
       <c r="AX61" s="2"/>
       <c r="AY61" s="2"/>
-    </row>
-    <row r="62" spans="1:51" x14ac:dyDescent="0.2">
+      <c r="AZ61" s="3"/>
+    </row>
+    <row r="62" spans="1:52" x14ac:dyDescent="0.2">
       <c r="I62" s="3"/>
       <c r="AG62" s="3"/>
-    </row>
-    <row r="63" spans="1:51" x14ac:dyDescent="0.2">
+      <c r="AZ62" s="3"/>
+    </row>
+    <row r="63" spans="1:52" x14ac:dyDescent="0.2">
       <c r="I63" s="3"/>
       <c r="AG63" s="3"/>
-    </row>
-    <row r="64" spans="1:51" x14ac:dyDescent="0.2">
+      <c r="AZ63" s="3"/>
+    </row>
+    <row r="64" spans="1:52" x14ac:dyDescent="0.2">
       <c r="I64" s="3"/>
       <c r="AG64" s="3"/>
-    </row>
-    <row r="65" spans="9:33" x14ac:dyDescent="0.2">
+      <c r="AZ64" s="3"/>
+    </row>
+    <row r="65" spans="9:52" x14ac:dyDescent="0.2">
       <c r="I65" s="3"/>
       <c r="AG65" s="3"/>
-    </row>
-    <row r="66" spans="9:33" x14ac:dyDescent="0.2">
+      <c r="AZ65" s="3"/>
+    </row>
+    <row r="66" spans="9:52" x14ac:dyDescent="0.2">
       <c r="I66" s="3"/>
       <c r="AG66" s="3"/>
-    </row>
-    <row r="67" spans="9:33" x14ac:dyDescent="0.2">
+      <c r="AZ66" s="3"/>
+    </row>
+    <row r="67" spans="9:52" x14ac:dyDescent="0.2">
       <c r="I67" s="3"/>
       <c r="AG67" s="3"/>
-    </row>
-    <row r="68" spans="9:33" x14ac:dyDescent="0.2">
+      <c r="AZ67" s="3"/>
+    </row>
+    <row r="68" spans="9:52" x14ac:dyDescent="0.2">
       <c r="I68" s="3"/>
       <c r="AG68" s="3"/>
-    </row>
-    <row r="69" spans="9:33" x14ac:dyDescent="0.2">
+      <c r="AZ68" s="3"/>
+    </row>
+    <row r="69" spans="9:52" x14ac:dyDescent="0.2">
       <c r="I69" s="3"/>
       <c r="AG69" s="3"/>
-    </row>
-    <row r="70" spans="9:33" x14ac:dyDescent="0.2">
+      <c r="AZ69" s="3"/>
+    </row>
+    <row r="70" spans="9:52" x14ac:dyDescent="0.2">
       <c r="I70" s="3"/>
       <c r="AG70" s="3"/>
-    </row>
-    <row r="71" spans="9:33" x14ac:dyDescent="0.2">
+      <c r="AZ70" s="3"/>
+    </row>
+    <row r="71" spans="9:52" x14ac:dyDescent="0.2">
       <c r="AG71" s="3"/>
-    </row>
-    <row r="72" spans="9:33" x14ac:dyDescent="0.2">
+      <c r="AZ71" s="3"/>
+    </row>
+    <row r="72" spans="9:52" x14ac:dyDescent="0.2">
       <c r="AG72" s="3"/>
-    </row>
-    <row r="73" spans="9:33" x14ac:dyDescent="0.2">
+      <c r="AZ72" s="3"/>
+    </row>
+    <row r="73" spans="9:52" x14ac:dyDescent="0.2">
       <c r="AG73" s="3"/>
-    </row>
-    <row r="74" spans="9:33" x14ac:dyDescent="0.2">
+      <c r="AZ73" s="3"/>
+    </row>
+    <row r="74" spans="9:52" x14ac:dyDescent="0.2">
       <c r="AG74" s="3"/>
-    </row>
-    <row r="75" spans="9:33" x14ac:dyDescent="0.2">
+      <c r="AZ74" s="3"/>
+    </row>
+    <row r="75" spans="9:52" x14ac:dyDescent="0.2">
       <c r="AG75" s="3"/>
-    </row>
-    <row r="76" spans="9:33" x14ac:dyDescent="0.2">
+      <c r="AZ75" s="3"/>
+    </row>
+    <row r="76" spans="9:52" x14ac:dyDescent="0.2">
       <c r="AG76" s="3"/>
-    </row>
-    <row r="77" spans="9:33" x14ac:dyDescent="0.2">
+      <c r="AZ76" s="3"/>
+    </row>
+    <row r="77" spans="9:52" x14ac:dyDescent="0.2">
       <c r="AG77" s="3"/>
-    </row>
-    <row r="78" spans="9:33" x14ac:dyDescent="0.2">
+      <c r="AZ77" s="3"/>
+    </row>
+    <row r="78" spans="9:52" x14ac:dyDescent="0.2">
       <c r="AG78" s="3"/>
-    </row>
-    <row r="79" spans="9:33" x14ac:dyDescent="0.2">
+      <c r="AZ78" s="3"/>
+    </row>
+    <row r="79" spans="9:52" x14ac:dyDescent="0.2">
       <c r="AG79" s="3"/>
-    </row>
-    <row r="80" spans="9:33" x14ac:dyDescent="0.2">
+      <c r="AZ79" s="3"/>
+    </row>
+    <row r="80" spans="9:52" x14ac:dyDescent="0.2">
       <c r="AG80" s="3"/>
-    </row>
-    <row r="81" spans="33:33" x14ac:dyDescent="0.2">
+      <c r="AZ80" s="3"/>
+    </row>
+    <row r="81" spans="33:52" x14ac:dyDescent="0.2">
       <c r="AG81" s="3"/>
-    </row>
-    <row r="82" spans="33:33" x14ac:dyDescent="0.2">
+      <c r="AZ81" s="3"/>
+    </row>
+    <row r="82" spans="33:52" x14ac:dyDescent="0.2">
       <c r="AG82" s="3"/>
     </row>
-    <row r="83" spans="33:33" x14ac:dyDescent="0.2">
+    <row r="83" spans="33:52" x14ac:dyDescent="0.2">
       <c r="AG83" s="3"/>
     </row>
-    <row r="84" spans="33:33" x14ac:dyDescent="0.2">
+    <row r="84" spans="33:52" x14ac:dyDescent="0.2">
       <c r="AG84" s="3"/>
     </row>
-    <row r="85" spans="33:33" x14ac:dyDescent="0.2">
+    <row r="85" spans="33:52" x14ac:dyDescent="0.2">
       <c r="AG85" s="3"/>
     </row>
-    <row r="86" spans="33:33" x14ac:dyDescent="0.2">
+    <row r="86" spans="33:52" x14ac:dyDescent="0.2">
       <c r="AG86" s="3"/>
     </row>
-    <row r="87" spans="33:33" x14ac:dyDescent="0.2">
+    <row r="87" spans="33:52" x14ac:dyDescent="0.2">
       <c r="AG87" s="3"/>
     </row>
-    <row r="88" spans="33:33" x14ac:dyDescent="0.2">
+    <row r="88" spans="33:52" x14ac:dyDescent="0.2">
       <c r="AG88" s="3"/>
     </row>
-    <row r="89" spans="33:33" x14ac:dyDescent="0.2">
+    <row r="89" spans="33:52" x14ac:dyDescent="0.2">
       <c r="AG89" s="3"/>
     </row>
-    <row r="90" spans="33:33" x14ac:dyDescent="0.2">
+    <row r="90" spans="33:52" x14ac:dyDescent="0.2">
       <c r="AG90" s="3"/>
     </row>
-    <row r="91" spans="33:33" x14ac:dyDescent="0.2">
+    <row r="91" spans="33:52" x14ac:dyDescent="0.2">
       <c r="AG91" s="3"/>
     </row>
-    <row r="92" spans="33:33" x14ac:dyDescent="0.2">
+    <row r="92" spans="33:52" x14ac:dyDescent="0.2">
       <c r="AG92" s="3"/>
     </row>
-    <row r="93" spans="33:33" x14ac:dyDescent="0.2">
+    <row r="93" spans="33:52" x14ac:dyDescent="0.2">
       <c r="AG93" s="3"/>
     </row>
-    <row r="94" spans="33:33" x14ac:dyDescent="0.2">
+    <row r="94" spans="33:52" x14ac:dyDescent="0.2">
       <c r="AG94" s="3"/>
     </row>
-    <row r="95" spans="33:33" x14ac:dyDescent="0.2">
+    <row r="95" spans="33:52" x14ac:dyDescent="0.2">
       <c r="AG95" s="3"/>
     </row>
-    <row r="96" spans="33:33" x14ac:dyDescent="0.2">
+    <row r="96" spans="33:52" x14ac:dyDescent="0.2">
       <c r="AG96" s="3"/>
     </row>
     <row r="97" spans="33:33" x14ac:dyDescent="0.2">
@@ -6176,6 +6775,32 @@
       <c r="AG110" s="3"/>
     </row>
   </sheetData>
+  <autoFilter ref="A1:A110" xr:uid="{7F37C204-69FB-8946-B201-7E43976BBF53}">
+    <filterColumn colId="0">
+      <filters blank="1">
+        <filter val="Alabama"/>
+        <filter val="Arizona"/>
+        <filter val="Arkansas"/>
+        <filter val="California"/>
+        <filter val="Florida"/>
+        <filter val="Georgia"/>
+        <filter val="Iowa"/>
+        <filter val="Kansas"/>
+        <filter val="Kentucky"/>
+        <filter val="Louisiana"/>
+        <filter val="Mississippi"/>
+        <filter val="North Carolina"/>
+        <filter val="North Dakota"/>
+        <filter val="Oklahoma"/>
+        <filter val="Pennsylvania"/>
+        <filter val="South Dakota"/>
+        <filter val="Texas"/>
+        <filter val="Utah"/>
+        <filter val="Vermont"/>
+        <filter val="West Virginia"/>
+      </filters>
+    </filterColumn>
+  </autoFilter>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -6185,7 +6810,8 @@
   <dimension ref="A1:A51"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:A51"/>
+      <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" sqref="A1:A1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -6446,6 +7072,7 @@
       </c>
     </row>
   </sheetData>
+  <autoFilter ref="A1:A51" xr:uid="{48541A15-86EE-DC49-B72C-33AAB33B8C19}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Andrew | Re-downloaded WV-H-4787 because it was corrupted. Finished driver license analysis.
</commit_message>
<xml_diff>
--- a/compliance/State Compliance Analysis.xlsx
+++ b/compliance/State Compliance Analysis.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/andrewhetzler/Documents/Documents - Andrew’s Money Maker/School/DISSERTATION/GitHub/dissertation/compliance/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F1915C8D-00DA-4847-8D09-806972B0BA5D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B5B98A61-BDAA-5240-B411-37546AB5F25A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="40960" windowHeight="24400" activeTab="1" xr2:uid="{FEE3D6CA-2CD0-2B4F-9478-6397B247951E}"/>
   </bookViews>
@@ -43,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="865" uniqueCount="211">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1251" uniqueCount="254">
   <si>
     <t>STATE</t>
   </si>
@@ -1065,6 +1065,282 @@
   </si>
   <si>
     <t>Optional (39-06-14(6))</t>
+  </si>
+  <si>
+    <t>Required (47-6-111(A)(1))</t>
+  </si>
+  <si>
+    <t>COUNTY OF RESIDENCE</t>
+  </si>
+  <si>
+    <t>Required (47-6-111(A)(2))</t>
+  </si>
+  <si>
+    <t>Ooptional (47-6-111(A)(4))</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Ooptional (47-6-111(A)(4)) </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>NOTE:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> calls out height specifically</t>
+    </r>
+  </si>
+  <si>
+    <t>Optional--only required if sex offender  (47-6-111(E )(1))</t>
+  </si>
+  <si>
+    <t>Optional--only required if required to use an interlock  (47-6-111(G))</t>
+  </si>
+  <si>
+    <t>MODIFICATIONS</t>
+  </si>
+  <si>
+    <t>Optional--only required if licensee has modified driving privileges (47-6-111(H))</t>
+  </si>
+  <si>
+    <t>Required (75-15-1510(a))</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Required (75-15-1510(a)) </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>NOTE</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> or restrictions</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Required (75-15-1510(a)) </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>NOTE</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> doesn't give details</t>
+    </r>
+  </si>
+  <si>
+    <t>Optional  (75-15-1510(a))</t>
+  </si>
+  <si>
+    <t>Optional  (75-15-1510(a)(1))</t>
+  </si>
+  <si>
+    <t>Required (32-12-17.10)</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Required (32-12-17.10) </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>NOTE</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> may be more than 1</t>
+    </r>
+  </si>
+  <si>
+    <t>TEMPORARY U.S. STATUS</t>
+  </si>
+  <si>
+    <t>Required (521.121(a)(1))</t>
+  </si>
+  <si>
+    <t>Required (521.121(a)(2))</t>
+  </si>
+  <si>
+    <t>Required (521.121(a)(3))</t>
+  </si>
+  <si>
+    <t>Required (521.121(a)(4))</t>
+  </si>
+  <si>
+    <t>Required (521.121(a)(5))</t>
+  </si>
+  <si>
+    <t>Required (521.121(b))</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Required (521.122(a)) </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>NOTE</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> may be more than 1</t>
+    </r>
+  </si>
+  <si>
+    <t>Optional--only required if between 18 and 21 (521.123(a))</t>
+  </si>
+  <si>
+    <t>Optional (521.1235)</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Required (521.125(a)) </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>NOTE</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> see section for details</t>
+    </r>
+  </si>
+  <si>
+    <t>Optional (521.1251)</t>
+  </si>
+  <si>
+    <t>Required (53-3-207(3)(a)(i))</t>
+  </si>
+  <si>
+    <t>Required (53-3-207(3)(a)(ii))</t>
+  </si>
+  <si>
+    <t>Required (53-3-207(3)(a)(iii))</t>
+  </si>
+  <si>
+    <t>Optional--only required if licensee has restrictions (53-3-207(3)(a)(iv))</t>
+  </si>
+  <si>
+    <t>Required (53-3-207(3)(a)(v))</t>
+  </si>
+  <si>
+    <t>Required (53-3-207(3)(a)(vi))</t>
+  </si>
+  <si>
+    <t>Required (53-3-207(3)(a)(vii))</t>
+  </si>
+  <si>
+    <t>Optional (53-3-207(3)(a)(viii))</t>
+  </si>
+  <si>
+    <t>Optional (53-3-207(4)(a))</t>
+  </si>
+  <si>
+    <t>Optional--only required if under 21 (53-3-207(7)(b))</t>
+  </si>
+  <si>
+    <t>PERMIT DISTINCTION</t>
+  </si>
+  <si>
+    <t>Optional--only required if it is a permit (53-3-207(9)(b))</t>
+  </si>
+  <si>
+    <t>Required (17B-2-8(a))</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Required (17B-2-8(a)) </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>NOTE</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> may be more than 1</t>
+    </r>
+  </si>
+  <si>
+    <t>Optional (17B-2-8(b))</t>
   </si>
 </sst>
 </file>
@@ -1757,11 +2033,11 @@
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7F37C204-69FB-8946-B201-7E43976BBF53}">
   <sheetPr filterMode="1"/>
-  <dimension ref="A1:AZ110"/>
+  <dimension ref="A1:BD110"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="AM1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="AZ35" sqref="AZ2:AZ35"/>
+      <pane ySplit="1" topLeftCell="A17" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="BE49" sqref="BE49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1774,7 +2050,7 @@
     <col min="6" max="6" width="31.83203125" customWidth="1"/>
     <col min="7" max="8" width="40.1640625" customWidth="1"/>
     <col min="9" max="9" width="30.1640625" customWidth="1"/>
-    <col min="10" max="10" width="21.33203125" customWidth="1"/>
+    <col min="10" max="10" width="23.6640625" customWidth="1"/>
     <col min="11" max="11" width="20.83203125" customWidth="1"/>
     <col min="12" max="12" width="28.6640625" customWidth="1"/>
     <col min="13" max="13" width="27.1640625" customWidth="1"/>
@@ -1816,9 +2092,13 @@
     <col min="49" max="49" width="15.33203125" customWidth="1"/>
     <col min="50" max="51" width="24" customWidth="1"/>
     <col min="52" max="52" width="23.6640625" customWidth="1"/>
+    <col min="53" max="53" width="21" customWidth="1"/>
+    <col min="54" max="54" width="26.1640625" customWidth="1"/>
+    <col min="55" max="55" width="43" customWidth="1"/>
+    <col min="56" max="56" width="19.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:52" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:56" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1975,8 +2255,20 @@
       <c r="AZ1" s="1" t="s">
         <v>208</v>
       </c>
-    </row>
-    <row r="2" spans="1:52" ht="51" x14ac:dyDescent="0.2">
+      <c r="BA1" s="1" t="s">
+        <v>212</v>
+      </c>
+      <c r="BB1" s="1" t="s">
+        <v>218</v>
+      </c>
+      <c r="BC1" s="1" t="s">
+        <v>227</v>
+      </c>
+      <c r="BD1" s="1" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="2" spans="1:56" ht="51" x14ac:dyDescent="0.2">
       <c r="A2" s="3" t="s">
         <v>9</v>
       </c>
@@ -2133,8 +2425,20 @@
       <c r="AZ2" s="2" t="s">
         <v>80</v>
       </c>
-    </row>
-    <row r="3" spans="1:52" hidden="1" x14ac:dyDescent="0.2">
+      <c r="BA2" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="BB2" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="BC2" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="BD2" s="2" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="3" spans="1:56" hidden="1" x14ac:dyDescent="0.2">
       <c r="A3" s="3" t="s">
         <v>10</v>
       </c>
@@ -2189,7 +2493,7 @@
       <c r="AX3" s="2"/>
       <c r="AY3" s="2"/>
     </row>
-    <row r="4" spans="1:52" ht="51" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:56" ht="51" x14ac:dyDescent="0.2">
       <c r="A4" s="3" t="s">
         <v>11</v>
       </c>
@@ -2346,8 +2650,20 @@
       <c r="AZ4" s="2" t="s">
         <v>80</v>
       </c>
-    </row>
-    <row r="5" spans="1:52" ht="68" x14ac:dyDescent="0.2">
+      <c r="BA4" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="BB4" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="BC4" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="BD4" s="2" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="5" spans="1:56" ht="68" x14ac:dyDescent="0.2">
       <c r="A5" s="3" t="s">
         <v>12</v>
       </c>
@@ -2500,8 +2816,20 @@
       <c r="AZ5" s="2" t="s">
         <v>80</v>
       </c>
-    </row>
-    <row r="6" spans="1:52" ht="68" x14ac:dyDescent="0.2">
+      <c r="BA5" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="BB5" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="BC5" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="BD5" s="2" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="6" spans="1:56" ht="68" x14ac:dyDescent="0.2">
       <c r="A6" s="3" t="s">
         <v>13</v>
       </c>
@@ -2658,8 +2986,20 @@
       <c r="AZ6" s="2" t="s">
         <v>80</v>
       </c>
-    </row>
-    <row r="7" spans="1:52" hidden="1" x14ac:dyDescent="0.2">
+      <c r="BA6" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="BB6" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="BC6" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="BD6" s="2" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="7" spans="1:56" hidden="1" x14ac:dyDescent="0.2">
       <c r="A7" s="3" t="s">
         <v>14</v>
       </c>
@@ -2714,7 +3054,7 @@
       <c r="AX7" s="2"/>
       <c r="AY7" s="2"/>
     </row>
-    <row r="8" spans="1:52" hidden="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:56" hidden="1" x14ac:dyDescent="0.2">
       <c r="A8" s="3" t="s">
         <v>58</v>
       </c>
@@ -2769,7 +3109,7 @@
       <c r="AX8" s="2"/>
       <c r="AY8" s="2"/>
     </row>
-    <row r="9" spans="1:52" hidden="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:56" hidden="1" x14ac:dyDescent="0.2">
       <c r="A9" s="3" t="s">
         <v>15</v>
       </c>
@@ -2824,7 +3164,7 @@
       <c r="AX9" s="2"/>
       <c r="AY9" s="2"/>
     </row>
-    <row r="10" spans="1:52" ht="85" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:56" ht="85" x14ac:dyDescent="0.2">
       <c r="A10" s="3" t="s">
         <v>16</v>
       </c>
@@ -2981,8 +3321,20 @@
       <c r="AZ10" s="2" t="s">
         <v>80</v>
       </c>
-    </row>
-    <row r="11" spans="1:52" ht="68" x14ac:dyDescent="0.2">
+      <c r="BA10" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="BB10" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="BC10" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="BD10" s="2" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="11" spans="1:56" ht="68" x14ac:dyDescent="0.2">
       <c r="A11" s="3" t="s">
         <v>17</v>
       </c>
@@ -3139,8 +3491,20 @@
       <c r="AZ11" s="2" t="s">
         <v>80</v>
       </c>
-    </row>
-    <row r="12" spans="1:52" hidden="1" x14ac:dyDescent="0.2">
+      <c r="BA11" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="BB11" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="BC11" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="BD11" s="2" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="12" spans="1:56" hidden="1" x14ac:dyDescent="0.2">
       <c r="A12" s="3" t="s">
         <v>18</v>
       </c>
@@ -3195,7 +3559,7 @@
       <c r="AX12" s="2"/>
       <c r="AY12" s="2"/>
     </row>
-    <row r="13" spans="1:52" hidden="1" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:56" hidden="1" x14ac:dyDescent="0.2">
       <c r="A13" s="3" t="s">
         <v>21</v>
       </c>
@@ -3250,7 +3614,7 @@
       <c r="AX13" s="2"/>
       <c r="AY13" s="2"/>
     </row>
-    <row r="14" spans="1:52" hidden="1" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:56" hidden="1" x14ac:dyDescent="0.2">
       <c r="A14" s="3" t="s">
         <v>19</v>
       </c>
@@ -3305,7 +3669,7 @@
       <c r="AX14" s="2"/>
       <c r="AY14" s="2"/>
     </row>
-    <row r="15" spans="1:52" hidden="1" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:56" hidden="1" x14ac:dyDescent="0.2">
       <c r="A15" s="3" t="s">
         <v>20</v>
       </c>
@@ -3360,7 +3724,7 @@
       <c r="AX15" s="2"/>
       <c r="AY15" s="2"/>
     </row>
-    <row r="16" spans="1:52" ht="68" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:56" ht="68" x14ac:dyDescent="0.2">
       <c r="A16" s="3" t="s">
         <v>22</v>
       </c>
@@ -3517,8 +3881,20 @@
       <c r="AZ16" s="2" t="s">
         <v>80</v>
       </c>
-    </row>
-    <row r="17" spans="1:52" ht="68" x14ac:dyDescent="0.2">
+      <c r="BA16" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="BB16" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="BC16" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="BD16" s="2" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="17" spans="1:56" ht="68" x14ac:dyDescent="0.2">
       <c r="A17" s="3" t="s">
         <v>23</v>
       </c>
@@ -3675,8 +4051,20 @@
       <c r="AZ17" s="2" t="s">
         <v>80</v>
       </c>
-    </row>
-    <row r="18" spans="1:52" ht="119" x14ac:dyDescent="0.2">
+      <c r="BA17" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="BB17" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="BC17" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="BD17" s="2" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="18" spans="1:56" ht="119" x14ac:dyDescent="0.2">
       <c r="A18" s="3" t="s">
         <v>24</v>
       </c>
@@ -3833,8 +4221,20 @@
       <c r="AZ18" s="2" t="s">
         <v>80</v>
       </c>
-    </row>
-    <row r="19" spans="1:52" ht="51" x14ac:dyDescent="0.2">
+      <c r="BA18" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="BB18" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="BC18" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="BD18" s="2" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="19" spans="1:56" ht="51" x14ac:dyDescent="0.2">
       <c r="A19" s="3" t="s">
         <v>25</v>
       </c>
@@ -3991,8 +4391,20 @@
       <c r="AZ19" s="2" t="s">
         <v>80</v>
       </c>
-    </row>
-    <row r="20" spans="1:52" hidden="1" x14ac:dyDescent="0.2">
+      <c r="BA19" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="BB19" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="BC19" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="BD19" s="2" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="20" spans="1:56" hidden="1" x14ac:dyDescent="0.2">
       <c r="A20" s="3" t="s">
         <v>26</v>
       </c>
@@ -4047,7 +4459,7 @@
       <c r="AX20" s="2"/>
       <c r="AY20" s="2"/>
     </row>
-    <row r="21" spans="1:52" hidden="1" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:56" hidden="1" x14ac:dyDescent="0.2">
       <c r="A21" s="3" t="s">
         <v>27</v>
       </c>
@@ -4102,7 +4514,7 @@
       <c r="AX21" s="2"/>
       <c r="AY21" s="2"/>
     </row>
-    <row r="22" spans="1:52" hidden="1" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:56" hidden="1" x14ac:dyDescent="0.2">
       <c r="A22" s="3" t="s">
         <v>28</v>
       </c>
@@ -4157,7 +4569,7 @@
       <c r="AX22" s="2"/>
       <c r="AY22" s="2"/>
     </row>
-    <row r="23" spans="1:52" hidden="1" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:56" hidden="1" x14ac:dyDescent="0.2">
       <c r="A23" s="3" t="s">
         <v>29</v>
       </c>
@@ -4212,7 +4624,7 @@
       <c r="AX23" s="2"/>
       <c r="AY23" s="2"/>
     </row>
-    <row r="24" spans="1:52" hidden="1" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:56" hidden="1" x14ac:dyDescent="0.2">
       <c r="A24" s="3" t="s">
         <v>30</v>
       </c>
@@ -4267,7 +4679,7 @@
       <c r="AX24" s="2"/>
       <c r="AY24" s="2"/>
     </row>
-    <row r="25" spans="1:52" ht="34" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:56" ht="34" x14ac:dyDescent="0.2">
       <c r="A25" s="3" t="s">
         <v>31</v>
       </c>
@@ -4424,8 +4836,20 @@
       <c r="AZ25" s="2" t="s">
         <v>80</v>
       </c>
-    </row>
-    <row r="26" spans="1:52" hidden="1" x14ac:dyDescent="0.2">
+      <c r="BA25" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="BB25" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="BC25" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="BD25" s="2" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="26" spans="1:56" hidden="1" x14ac:dyDescent="0.2">
       <c r="A26" s="3" t="s">
         <v>32</v>
       </c>
@@ -4480,7 +4904,7 @@
       <c r="AX26" s="2"/>
       <c r="AY26" s="2"/>
     </row>
-    <row r="27" spans="1:52" hidden="1" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:56" hidden="1" x14ac:dyDescent="0.2">
       <c r="A27" s="3" t="s">
         <v>33</v>
       </c>
@@ -4535,7 +4959,7 @@
       <c r="AX27" s="2"/>
       <c r="AY27" s="2"/>
     </row>
-    <row r="28" spans="1:52" hidden="1" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:56" hidden="1" x14ac:dyDescent="0.2">
       <c r="A28" s="3" t="s">
         <v>34</v>
       </c>
@@ -4590,7 +5014,7 @@
       <c r="AX28" s="2"/>
       <c r="AY28" s="2"/>
     </row>
-    <row r="29" spans="1:52" hidden="1" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:56" hidden="1" x14ac:dyDescent="0.2">
       <c r="A29" s="3" t="s">
         <v>35</v>
       </c>
@@ -4645,7 +5069,7 @@
       <c r="AX29" s="2"/>
       <c r="AY29" s="2"/>
     </row>
-    <row r="30" spans="1:52" hidden="1" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:56" hidden="1" x14ac:dyDescent="0.2">
       <c r="A30" s="3" t="s">
         <v>36</v>
       </c>
@@ -4700,7 +5124,7 @@
       <c r="AX30" s="2"/>
       <c r="AY30" s="2"/>
     </row>
-    <row r="31" spans="1:52" hidden="1" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:56" hidden="1" x14ac:dyDescent="0.2">
       <c r="A31" s="3" t="s">
         <v>37</v>
       </c>
@@ -4755,7 +5179,7 @@
       <c r="AX31" s="2"/>
       <c r="AY31" s="2"/>
     </row>
-    <row r="32" spans="1:52" hidden="1" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:56" hidden="1" x14ac:dyDescent="0.2">
       <c r="A32" s="3" t="s">
         <v>38</v>
       </c>
@@ -4810,7 +5234,7 @@
       <c r="AX32" s="2"/>
       <c r="AY32" s="2"/>
     </row>
-    <row r="33" spans="1:52" hidden="1" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:56" hidden="1" x14ac:dyDescent="0.2">
       <c r="A33" s="3" t="s">
         <v>39</v>
       </c>
@@ -4865,7 +5289,7 @@
       <c r="AX33" s="2"/>
       <c r="AY33" s="2"/>
     </row>
-    <row r="34" spans="1:52" ht="51" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:56" ht="51" x14ac:dyDescent="0.2">
       <c r="A34" s="3" t="s">
         <v>40</v>
       </c>
@@ -5022,8 +5446,20 @@
       <c r="AZ34" s="2" t="s">
         <v>80</v>
       </c>
-    </row>
-    <row r="35" spans="1:52" ht="34" x14ac:dyDescent="0.2">
+      <c r="BA34" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="BB34" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="BC34" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="BD34" s="2" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="35" spans="1:56" ht="34" x14ac:dyDescent="0.2">
       <c r="A35" s="3" t="s">
         <v>41</v>
       </c>
@@ -5180,8 +5616,20 @@
       <c r="AZ35" s="3" t="s">
         <v>209</v>
       </c>
-    </row>
-    <row r="36" spans="1:52" hidden="1" x14ac:dyDescent="0.2">
+      <c r="BA35" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="BB35" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="BC35" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="BD35" s="2" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="36" spans="1:56" hidden="1" x14ac:dyDescent="0.2">
       <c r="A36" s="3" t="s">
         <v>42</v>
       </c>
@@ -5236,63 +5684,177 @@
       <c r="AX36" s="2"/>
       <c r="AY36" s="2"/>
     </row>
-    <row r="37" spans="1:52" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:56" ht="51" x14ac:dyDescent="0.2">
       <c r="A37" s="3" t="s">
         <v>43</v>
       </c>
-      <c r="B37" s="2"/>
-      <c r="C37" s="2"/>
-      <c r="D37" s="2"/>
-      <c r="E37" s="2"/>
-      <c r="F37" s="2"/>
-      <c r="G37" s="2"/>
-      <c r="H37" s="2"/>
-      <c r="I37" s="2"/>
-      <c r="J37" s="2"/>
-      <c r="K37" s="2"/>
-      <c r="L37" s="2"/>
-      <c r="M37" s="2"/>
-      <c r="N37" s="2"/>
-      <c r="O37" s="2"/>
-      <c r="P37" s="2"/>
-      <c r="Q37" s="2"/>
-      <c r="R37" s="2"/>
-      <c r="S37" s="2"/>
-      <c r="T37" s="2"/>
-      <c r="U37" s="2"/>
-      <c r="V37" s="2"/>
-      <c r="W37" s="2"/>
-      <c r="X37" s="2"/>
-      <c r="Y37" s="2"/>
-      <c r="Z37" s="2"/>
-      <c r="AA37" s="2"/>
-      <c r="AB37" s="2"/>
-      <c r="AC37" s="2"/>
-      <c r="AD37" s="2"/>
-      <c r="AE37" s="2"/>
-      <c r="AF37" s="2"/>
-      <c r="AG37" s="2"/>
-      <c r="AH37" s="2"/>
-      <c r="AI37" s="2"/>
-      <c r="AJ37" s="2"/>
-      <c r="AK37" s="2"/>
-      <c r="AL37" s="2"/>
-      <c r="AM37" s="2"/>
-      <c r="AN37" s="2"/>
-      <c r="AO37" s="2"/>
-      <c r="AP37" s="2"/>
-      <c r="AQ37" s="2"/>
-      <c r="AR37" s="2"/>
-      <c r="AS37" s="2"/>
-      <c r="AT37" s="2"/>
-      <c r="AU37" s="2"/>
-      <c r="AV37" s="2"/>
-      <c r="AW37" s="2"/>
-      <c r="AX37" s="2"/>
-      <c r="AY37" s="2"/>
-      <c r="AZ37" s="3"/>
-    </row>
-    <row r="38" spans="1:52" hidden="1" x14ac:dyDescent="0.2">
+      <c r="B37" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="C37" s="2" t="s">
+        <v>211</v>
+      </c>
+      <c r="D37" s="2" t="s">
+        <v>211</v>
+      </c>
+      <c r="E37" s="2" t="s">
+        <v>211</v>
+      </c>
+      <c r="F37" s="2" t="s">
+        <v>211</v>
+      </c>
+      <c r="G37" s="2" t="s">
+        <v>211</v>
+      </c>
+      <c r="H37" s="2" t="s">
+        <v>215</v>
+      </c>
+      <c r="I37" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="J37" s="2" t="s">
+        <v>211</v>
+      </c>
+      <c r="K37" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="L37" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="M37" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="N37" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="O37" s="2" t="s">
+        <v>217</v>
+      </c>
+      <c r="P37" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="Q37" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="R37" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="S37" s="2" t="s">
+        <v>211</v>
+      </c>
+      <c r="T37" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="U37" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="V37" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="W37" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="X37" s="2" t="s">
+        <v>211</v>
+      </c>
+      <c r="Y37" s="2" t="s">
+        <v>214</v>
+      </c>
+      <c r="Z37" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="AA37" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="AB37" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="AC37" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="AD37" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="AE37" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="AF37" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="AG37" s="4" t="s">
+        <v>211</v>
+      </c>
+      <c r="AH37" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="AI37" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="AJ37" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="AK37" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="AL37" s="2" t="s">
+        <v>216</v>
+      </c>
+      <c r="AM37" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="AN37" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="AO37" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="AP37" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="AQ37" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="AR37" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="AS37" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="AT37" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="AU37" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="AV37" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="AW37" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="AX37" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="AY37" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="AZ37" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="BA37" s="4" t="s">
+        <v>213</v>
+      </c>
+      <c r="BB37" s="2" t="s">
+        <v>219</v>
+      </c>
+      <c r="BC37" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="BD37" s="2" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="38" spans="1:56" hidden="1" x14ac:dyDescent="0.2">
       <c r="A38" s="3" t="s">
         <v>44</v>
       </c>
@@ -5347,63 +5909,177 @@
       <c r="AX38" s="2"/>
       <c r="AY38" s="2"/>
     </row>
-    <row r="39" spans="1:52" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:56" ht="51" x14ac:dyDescent="0.2">
       <c r="A39" s="3" t="s">
         <v>45</v>
       </c>
-      <c r="B39" s="2"/>
-      <c r="C39" s="2"/>
-      <c r="D39" s="2"/>
-      <c r="E39" s="2"/>
-      <c r="F39" s="2"/>
-      <c r="G39" s="2"/>
-      <c r="H39" s="2"/>
-      <c r="I39" s="2"/>
-      <c r="J39" s="2"/>
-      <c r="K39" s="2"/>
-      <c r="L39" s="2"/>
-      <c r="M39" s="2"/>
-      <c r="N39" s="2"/>
-      <c r="O39" s="2"/>
-      <c r="P39" s="2"/>
-      <c r="Q39" s="2"/>
-      <c r="R39" s="2"/>
-      <c r="S39" s="2"/>
-      <c r="T39" s="2"/>
-      <c r="U39" s="2"/>
-      <c r="V39" s="2"/>
-      <c r="W39" s="2"/>
-      <c r="X39" s="2"/>
-      <c r="Y39" s="2"/>
-      <c r="Z39" s="2"/>
-      <c r="AA39" s="2"/>
-      <c r="AB39" s="2"/>
-      <c r="AC39" s="2"/>
-      <c r="AD39" s="2"/>
-      <c r="AE39" s="2"/>
-      <c r="AF39" s="2"/>
-      <c r="AG39" s="2"/>
-      <c r="AH39" s="2"/>
-      <c r="AI39" s="2"/>
-      <c r="AJ39" s="2"/>
-      <c r="AK39" s="2"/>
-      <c r="AL39" s="2"/>
-      <c r="AM39" s="2"/>
-      <c r="AN39" s="2"/>
-      <c r="AO39" s="2"/>
-      <c r="AP39" s="2"/>
-      <c r="AQ39" s="2"/>
-      <c r="AR39" s="2"/>
-      <c r="AS39" s="2"/>
-      <c r="AT39" s="2"/>
-      <c r="AU39" s="2"/>
-      <c r="AV39" s="2"/>
-      <c r="AW39" s="2"/>
-      <c r="AX39" s="2"/>
-      <c r="AY39" s="2"/>
-      <c r="AZ39" s="3"/>
-    </row>
-    <row r="40" spans="1:52" hidden="1" x14ac:dyDescent="0.2">
+      <c r="B39" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="C39" s="2" t="s">
+        <v>220</v>
+      </c>
+      <c r="D39" s="2" t="s">
+        <v>220</v>
+      </c>
+      <c r="E39" s="2" t="s">
+        <v>220</v>
+      </c>
+      <c r="F39" s="2" t="s">
+        <v>220</v>
+      </c>
+      <c r="G39" s="2" t="s">
+        <v>220</v>
+      </c>
+      <c r="H39" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="I39" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="J39" s="2" t="s">
+        <v>220</v>
+      </c>
+      <c r="K39" s="2" t="s">
+        <v>220</v>
+      </c>
+      <c r="L39" s="2" t="s">
+        <v>221</v>
+      </c>
+      <c r="M39" s="2" t="s">
+        <v>224</v>
+      </c>
+      <c r="N39" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="O39" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="P39" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="Q39" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="R39" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="S39" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="T39" s="2" t="s">
+        <v>223</v>
+      </c>
+      <c r="U39" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="V39" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="W39" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="X39" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="Y39" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="Z39" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="AA39" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="AB39" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="AC39" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="AD39" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="AE39" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="AF39" s="2" t="s">
+        <v>222</v>
+      </c>
+      <c r="AG39" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="AH39" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="AI39" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="AJ39" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="AK39" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="AL39" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="AM39" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="AN39" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="AO39" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="AP39" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="AQ39" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="AR39" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="AS39" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="AT39" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="AU39" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="AV39" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="AW39" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="AX39" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="AY39" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="AZ39" s="3" t="s">
+        <v>80</v>
+      </c>
+      <c r="BA39" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="BB39" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="BC39" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="BD39" s="2" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="40" spans="1:56" hidden="1" x14ac:dyDescent="0.2">
       <c r="A40" s="3" t="s">
         <v>46</v>
       </c>
@@ -5458,7 +6134,7 @@
       <c r="AX40" s="2"/>
       <c r="AY40" s="2"/>
     </row>
-    <row r="41" spans="1:52" hidden="1" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:56" hidden="1" x14ac:dyDescent="0.2">
       <c r="A41" s="3" t="s">
         <v>47</v>
       </c>
@@ -5513,63 +6189,177 @@
       <c r="AX41" s="2"/>
       <c r="AY41" s="2"/>
     </row>
-    <row r="42" spans="1:52" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:56" ht="51" x14ac:dyDescent="0.2">
       <c r="A42" s="3" t="s">
         <v>48</v>
       </c>
-      <c r="B42" s="2"/>
-      <c r="C42" s="2"/>
-      <c r="D42" s="2"/>
-      <c r="E42" s="2"/>
-      <c r="F42" s="2"/>
-      <c r="G42" s="2"/>
-      <c r="H42" s="2"/>
-      <c r="I42" s="2"/>
-      <c r="J42" s="2"/>
-      <c r="K42" s="2"/>
-      <c r="L42" s="2"/>
-      <c r="M42" s="2"/>
-      <c r="N42" s="2"/>
-      <c r="O42" s="2"/>
-      <c r="P42" s="2"/>
-      <c r="Q42" s="2"/>
-      <c r="R42" s="2"/>
-      <c r="S42" s="2"/>
-      <c r="T42" s="2"/>
-      <c r="U42" s="2"/>
-      <c r="V42" s="2"/>
-      <c r="W42" s="2"/>
-      <c r="X42" s="2"/>
-      <c r="Y42" s="2"/>
-      <c r="Z42" s="2"/>
-      <c r="AA42" s="2"/>
-      <c r="AB42" s="2"/>
-      <c r="AC42" s="2"/>
-      <c r="AD42" s="2"/>
-      <c r="AE42" s="2"/>
-      <c r="AF42" s="2"/>
-      <c r="AG42" s="2"/>
-      <c r="AH42" s="2"/>
-      <c r="AI42" s="2"/>
-      <c r="AJ42" s="2"/>
-      <c r="AK42" s="2"/>
-      <c r="AL42" s="2"/>
-      <c r="AM42" s="2"/>
-      <c r="AN42" s="2"/>
-      <c r="AO42" s="2"/>
-      <c r="AP42" s="2"/>
-      <c r="AQ42" s="2"/>
-      <c r="AR42" s="2"/>
-      <c r="AS42" s="2"/>
-      <c r="AT42" s="2"/>
-      <c r="AU42" s="2"/>
-      <c r="AV42" s="2"/>
-      <c r="AW42" s="2"/>
-      <c r="AX42" s="2"/>
-      <c r="AY42" s="2"/>
-      <c r="AZ42" s="3"/>
-    </row>
-    <row r="43" spans="1:52" hidden="1" x14ac:dyDescent="0.2">
+      <c r="B42" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="C42" s="2" t="s">
+        <v>225</v>
+      </c>
+      <c r="D42" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="E42" s="2" t="s">
+        <v>225</v>
+      </c>
+      <c r="F42" s="2" t="s">
+        <v>225</v>
+      </c>
+      <c r="G42" s="2" t="s">
+        <v>225</v>
+      </c>
+      <c r="H42" s="2" t="s">
+        <v>225</v>
+      </c>
+      <c r="I42" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="J42" s="2" t="s">
+        <v>225</v>
+      </c>
+      <c r="K42" s="2" t="s">
+        <v>226</v>
+      </c>
+      <c r="L42" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="M42" s="2" t="s">
+        <v>225</v>
+      </c>
+      <c r="N42" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="O42" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="P42" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="Q42" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="R42" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="S42" s="2" t="s">
+        <v>225</v>
+      </c>
+      <c r="T42" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="U42" s="2" t="s">
+        <v>225</v>
+      </c>
+      <c r="V42" s="2" t="s">
+        <v>225</v>
+      </c>
+      <c r="W42" s="2" t="s">
+        <v>225</v>
+      </c>
+      <c r="X42" s="2" t="s">
+        <v>225</v>
+      </c>
+      <c r="Y42" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="Z42" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="AA42" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="AB42" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="AC42" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="AD42" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="AE42" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="AF42" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="AG42" s="2" t="s">
+        <v>225</v>
+      </c>
+      <c r="AH42" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="AI42" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="AJ42" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="AK42" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="AL42" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="AM42" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="AN42" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="AO42" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="AP42" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="AQ42" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="AR42" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="AS42" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="AT42" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="AU42" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="AV42" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="AW42" s="2" t="s">
+        <v>225</v>
+      </c>
+      <c r="AX42" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="AY42" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="AZ42" s="3" t="s">
+        <v>80</v>
+      </c>
+      <c r="BA42" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="BB42" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="BC42" s="3" t="s">
+        <v>225</v>
+      </c>
+      <c r="BD42" s="2" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="43" spans="1:56" hidden="1" x14ac:dyDescent="0.2">
       <c r="A43" s="3" t="s">
         <v>49</v>
       </c>
@@ -5624,119 +6414,347 @@
       <c r="AX43" s="2"/>
       <c r="AY43" s="2"/>
     </row>
-    <row r="44" spans="1:52" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:56" ht="51" x14ac:dyDescent="0.2">
       <c r="A44" s="3" t="s">
         <v>50</v>
       </c>
-      <c r="B44" s="2"/>
-      <c r="C44" s="2"/>
-      <c r="D44" s="2"/>
-      <c r="E44" s="2"/>
-      <c r="F44" s="2"/>
-      <c r="G44" s="2"/>
-      <c r="H44" s="2"/>
-      <c r="I44" s="2"/>
-      <c r="J44" s="2"/>
-      <c r="K44" s="2"/>
-      <c r="L44" s="2"/>
-      <c r="M44" s="2"/>
-      <c r="N44" s="2"/>
-      <c r="O44" s="2"/>
-      <c r="P44" s="2"/>
-      <c r="Q44" s="2"/>
-      <c r="R44" s="2"/>
-      <c r="S44" s="2"/>
-      <c r="T44" s="2"/>
-      <c r="U44" s="2"/>
-      <c r="V44" s="2"/>
-      <c r="W44" s="2"/>
-      <c r="X44" s="2"/>
-      <c r="Y44" s="2"/>
-      <c r="Z44" s="2"/>
-      <c r="AA44" s="2"/>
-      <c r="AB44" s="2"/>
-      <c r="AC44" s="2"/>
-      <c r="AD44" s="2"/>
-      <c r="AE44" s="2"/>
-      <c r="AF44" s="2"/>
-      <c r="AG44" s="2"/>
-      <c r="AH44" s="2"/>
-      <c r="AI44" s="2"/>
-      <c r="AJ44" s="2"/>
-      <c r="AK44" s="2"/>
-      <c r="AL44" s="2"/>
-      <c r="AM44" s="2"/>
-      <c r="AN44" s="2"/>
-      <c r="AO44" s="2"/>
-      <c r="AP44" s="2"/>
-      <c r="AQ44" s="2"/>
-      <c r="AR44" s="2"/>
-      <c r="AS44" s="2"/>
-      <c r="AT44" s="2"/>
-      <c r="AU44" s="2"/>
-      <c r="AV44" s="2"/>
-      <c r="AW44" s="2"/>
-      <c r="AX44" s="2"/>
-      <c r="AY44" s="2"/>
-      <c r="AZ44" s="3"/>
-    </row>
-    <row r="45" spans="1:52" x14ac:dyDescent="0.2">
+      <c r="B44" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="C44" s="2" t="s">
+        <v>228</v>
+      </c>
+      <c r="D44" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="E44" s="2" t="s">
+        <v>230</v>
+      </c>
+      <c r="F44" s="2" t="s">
+        <v>230</v>
+      </c>
+      <c r="G44" s="2" t="s">
+        <v>232</v>
+      </c>
+      <c r="H44" s="2" t="s">
+        <v>231</v>
+      </c>
+      <c r="I44" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="J44" s="2" t="s">
+        <v>233</v>
+      </c>
+      <c r="K44" s="2" t="s">
+        <v>234</v>
+      </c>
+      <c r="L44" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="M44" s="2" t="s">
+        <v>236</v>
+      </c>
+      <c r="N44" s="2" t="s">
+        <v>235</v>
+      </c>
+      <c r="O44" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="P44" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="Q44" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="R44" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="S44" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="T44" s="2" t="s">
+        <v>237</v>
+      </c>
+      <c r="U44" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="V44" s="2" t="s">
+        <v>229</v>
+      </c>
+      <c r="W44" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="X44" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="Y44" s="2" t="s">
+        <v>238</v>
+      </c>
+      <c r="Z44" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="AA44" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="AB44" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="AC44" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="AD44" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="AE44" s="2" t="s">
+        <v>238</v>
+      </c>
+      <c r="AF44" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="AG44" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="AH44" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="AI44" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="AJ44" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="AK44" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="AL44" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="AM44" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="AN44" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="AO44" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="AP44" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="AQ44" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="AR44" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="AS44" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="AT44" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="AU44" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="AV44" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="AW44" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="AX44" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="AY44" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="AZ44" s="3" t="s">
+        <v>80</v>
+      </c>
+      <c r="BA44" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="BB44" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="BC44" s="3" t="s">
+        <v>80</v>
+      </c>
+      <c r="BD44" s="2" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="45" spans="1:56" ht="51" x14ac:dyDescent="0.2">
       <c r="A45" s="3" t="s">
         <v>51</v>
       </c>
-      <c r="B45" s="2"/>
-      <c r="C45" s="2"/>
-      <c r="D45" s="2"/>
-      <c r="E45" s="2"/>
-      <c r="F45" s="2"/>
-      <c r="G45" s="2"/>
-      <c r="H45" s="2"/>
-      <c r="I45" s="2"/>
-      <c r="J45" s="2"/>
-      <c r="K45" s="2"/>
-      <c r="L45" s="2"/>
-      <c r="M45" s="2"/>
-      <c r="N45" s="2"/>
-      <c r="O45" s="2"/>
-      <c r="P45" s="2"/>
-      <c r="Q45" s="2"/>
-      <c r="R45" s="2"/>
-      <c r="S45" s="2"/>
-      <c r="T45" s="2"/>
-      <c r="U45" s="2"/>
-      <c r="V45" s="2"/>
-      <c r="W45" s="2"/>
-      <c r="X45" s="2"/>
-      <c r="Y45" s="2"/>
-      <c r="Z45" s="2"/>
-      <c r="AA45" s="2"/>
-      <c r="AB45" s="2"/>
-      <c r="AC45" s="2"/>
-      <c r="AD45" s="2"/>
-      <c r="AE45" s="2"/>
-      <c r="AF45" s="2"/>
-      <c r="AG45" s="2"/>
-      <c r="AH45" s="2"/>
-      <c r="AI45" s="2"/>
-      <c r="AJ45" s="2"/>
-      <c r="AK45" s="2"/>
-      <c r="AL45" s="2"/>
-      <c r="AM45" s="2"/>
-      <c r="AN45" s="2"/>
-      <c r="AO45" s="2"/>
-      <c r="AP45" s="2"/>
-      <c r="AQ45" s="2"/>
-      <c r="AR45" s="2"/>
-      <c r="AS45" s="2"/>
-      <c r="AT45" s="2"/>
-      <c r="AU45" s="2"/>
-      <c r="AV45" s="2"/>
-      <c r="AW45" s="2"/>
-      <c r="AX45" s="2"/>
-      <c r="AY45" s="2"/>
-      <c r="AZ45" s="3"/>
-    </row>
-    <row r="46" spans="1:52" x14ac:dyDescent="0.2">
+      <c r="B45" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="C45" s="2" t="s">
+        <v>239</v>
+      </c>
+      <c r="D45" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="E45" s="2" t="s">
+        <v>240</v>
+      </c>
+      <c r="F45" s="2" t="s">
+        <v>240</v>
+      </c>
+      <c r="G45" s="2" t="s">
+        <v>240</v>
+      </c>
+      <c r="H45" s="2" t="s">
+        <v>241</v>
+      </c>
+      <c r="I45" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="J45" s="2" t="s">
+        <v>244</v>
+      </c>
+      <c r="K45" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="L45" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="M45" s="2" t="s">
+        <v>246</v>
+      </c>
+      <c r="N45" s="2" t="s">
+        <v>248</v>
+      </c>
+      <c r="O45" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="P45" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="Q45" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="R45" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="S45" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="T45" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="U45" s="2" t="s">
+        <v>245</v>
+      </c>
+      <c r="V45" s="2" t="s">
+        <v>243</v>
+      </c>
+      <c r="W45" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="X45" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="Y45" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="Z45" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="AA45" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="AB45" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="AC45" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="AD45" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="AE45" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="AF45" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="AG45" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="AH45" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="AI45" s="2" t="s">
+        <v>247</v>
+      </c>
+      <c r="AJ45" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="AK45" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="AL45" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="AM45" s="2" t="s">
+        <v>242</v>
+      </c>
+      <c r="AN45" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="AO45" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="AP45" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="AQ45" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="AR45" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="AS45" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="AT45" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="AU45" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="AV45" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="AW45" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="AX45" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="AY45" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="AZ45" s="3" t="s">
+        <v>80</v>
+      </c>
+      <c r="BA45" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="BB45" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="BC45" s="3" t="s">
+        <v>80</v>
+      </c>
+      <c r="BD45" s="3" t="s">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="46" spans="1:56" hidden="1" x14ac:dyDescent="0.2">
       <c r="A46" s="3" t="s">
         <v>52</v>
       </c>
@@ -5791,8 +6809,10 @@
       <c r="AX46" s="2"/>
       <c r="AY46" s="2"/>
       <c r="AZ46" s="3"/>
-    </row>
-    <row r="47" spans="1:52" hidden="1" x14ac:dyDescent="0.2">
+      <c r="BC46" s="3"/>
+      <c r="BD46" s="3"/>
+    </row>
+    <row r="47" spans="1:56" hidden="1" x14ac:dyDescent="0.2">
       <c r="A47" s="3" t="s">
         <v>53</v>
       </c>
@@ -5847,7 +6867,7 @@
       <c r="AX47" s="2"/>
       <c r="AY47" s="2"/>
     </row>
-    <row r="48" spans="1:52" hidden="1" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:56" hidden="1" x14ac:dyDescent="0.2">
       <c r="A48" s="3" t="s">
         <v>54</v>
       </c>
@@ -5902,63 +6922,177 @@
       <c r="AX48" s="2"/>
       <c r="AY48" s="2"/>
     </row>
-    <row r="49" spans="1:52" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:56" ht="51" x14ac:dyDescent="0.2">
       <c r="A49" s="3" t="s">
         <v>55</v>
       </c>
-      <c r="B49" s="2"/>
-      <c r="C49" s="2"/>
-      <c r="D49" s="2"/>
-      <c r="E49" s="2"/>
-      <c r="F49" s="2"/>
-      <c r="G49" s="2"/>
-      <c r="H49" s="2"/>
-      <c r="I49" s="2"/>
-      <c r="J49" s="2"/>
-      <c r="K49" s="2"/>
-      <c r="L49" s="2"/>
-      <c r="M49" s="2"/>
-      <c r="N49" s="2"/>
-      <c r="O49" s="2"/>
-      <c r="P49" s="2"/>
-      <c r="Q49" s="2"/>
-      <c r="R49" s="2"/>
-      <c r="S49" s="2"/>
-      <c r="T49" s="2"/>
-      <c r="U49" s="2"/>
-      <c r="V49" s="2"/>
-      <c r="W49" s="2"/>
-      <c r="X49" s="2"/>
-      <c r="Y49" s="2"/>
-      <c r="Z49" s="2"/>
-      <c r="AA49" s="2"/>
-      <c r="AB49" s="2"/>
-      <c r="AC49" s="2"/>
-      <c r="AD49" s="2"/>
-      <c r="AE49" s="2"/>
-      <c r="AF49" s="2"/>
-      <c r="AG49" s="2"/>
-      <c r="AH49" s="2"/>
-      <c r="AI49" s="2"/>
-      <c r="AJ49" s="2"/>
-      <c r="AK49" s="2"/>
-      <c r="AL49" s="2"/>
-      <c r="AM49" s="2"/>
-      <c r="AN49" s="2"/>
-      <c r="AO49" s="2"/>
-      <c r="AP49" s="2"/>
-      <c r="AQ49" s="2"/>
-      <c r="AR49" s="2"/>
-      <c r="AS49" s="2"/>
-      <c r="AT49" s="2"/>
-      <c r="AU49" s="2"/>
-      <c r="AV49" s="2"/>
-      <c r="AW49" s="2"/>
-      <c r="AX49" s="2"/>
-      <c r="AY49" s="2"/>
-      <c r="AZ49" s="3"/>
-    </row>
-    <row r="50" spans="1:52" hidden="1" x14ac:dyDescent="0.2">
+      <c r="B49" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="C49" s="2" t="s">
+        <v>251</v>
+      </c>
+      <c r="D49" s="2" t="s">
+        <v>251</v>
+      </c>
+      <c r="E49" s="2" t="s">
+        <v>251</v>
+      </c>
+      <c r="F49" s="2" t="s">
+        <v>251</v>
+      </c>
+      <c r="G49" s="2" t="s">
+        <v>251</v>
+      </c>
+      <c r="H49" s="2" t="s">
+        <v>251</v>
+      </c>
+      <c r="I49" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="J49" s="2" t="s">
+        <v>251</v>
+      </c>
+      <c r="K49" s="2" t="s">
+        <v>252</v>
+      </c>
+      <c r="L49" s="2" t="s">
+        <v>253</v>
+      </c>
+      <c r="M49" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="N49" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="O49" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="P49" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="Q49" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="R49" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="S49" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="T49" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="U49" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="V49" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="W49" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="X49" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="Y49" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="Z49" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="AA49" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="AB49" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="AC49" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="AD49" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="AE49" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="AF49" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="AG49" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="AH49" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="AI49" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="AJ49" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="AK49" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="AL49" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="AM49" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="AN49" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="AO49" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="AP49" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="AQ49" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="AR49" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="AS49" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="AT49" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="AU49" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="AV49" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="AW49" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="AX49" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="AY49" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="AZ49" s="3" t="s">
+        <v>80</v>
+      </c>
+      <c r="BA49" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="BB49" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="BC49" s="3" t="s">
+        <v>80</v>
+      </c>
+      <c r="BD49" s="3" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="50" spans="1:56" hidden="1" x14ac:dyDescent="0.2">
       <c r="A50" s="3" t="s">
         <v>57</v>
       </c>
@@ -6013,7 +7147,7 @@
       <c r="AX50" s="2"/>
       <c r="AY50" s="2"/>
     </row>
-    <row r="51" spans="1:52" hidden="1" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:56" hidden="1" x14ac:dyDescent="0.2">
       <c r="A51" s="3" t="s">
         <v>56</v>
       </c>
@@ -6068,7 +7202,7 @@
       <c r="AX51" s="2"/>
       <c r="AY51" s="2"/>
     </row>
-    <row r="52" spans="1:52" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:56" x14ac:dyDescent="0.2">
       <c r="B52" s="2"/>
       <c r="C52" s="2"/>
       <c r="D52" s="2"/>
@@ -6120,8 +7254,10 @@
       <c r="AX52" s="2"/>
       <c r="AY52" s="2"/>
       <c r="AZ52" s="3"/>
-    </row>
-    <row r="53" spans="1:52" x14ac:dyDescent="0.2">
+      <c r="BC52" s="3"/>
+      <c r="BD52" s="3"/>
+    </row>
+    <row r="53" spans="1:56" x14ac:dyDescent="0.2">
       <c r="B53" s="2"/>
       <c r="C53" s="2"/>
       <c r="D53" s="2"/>
@@ -6173,8 +7309,10 @@
       <c r="AX53" s="2"/>
       <c r="AY53" s="2"/>
       <c r="AZ53" s="3"/>
-    </row>
-    <row r="54" spans="1:52" x14ac:dyDescent="0.2">
+      <c r="BC53" s="3"/>
+      <c r="BD53" s="3"/>
+    </row>
+    <row r="54" spans="1:56" x14ac:dyDescent="0.2">
       <c r="B54" s="2"/>
       <c r="C54" s="2"/>
       <c r="D54" s="2"/>
@@ -6226,8 +7364,10 @@
       <c r="AX54" s="2"/>
       <c r="AY54" s="2"/>
       <c r="AZ54" s="3"/>
-    </row>
-    <row r="55" spans="1:52" x14ac:dyDescent="0.2">
+      <c r="BC54" s="3"/>
+      <c r="BD54" s="3"/>
+    </row>
+    <row r="55" spans="1:56" x14ac:dyDescent="0.2">
       <c r="B55" s="2"/>
       <c r="C55" s="2"/>
       <c r="D55" s="2"/>
@@ -6279,8 +7419,10 @@
       <c r="AX55" s="2"/>
       <c r="AY55" s="2"/>
       <c r="AZ55" s="3"/>
-    </row>
-    <row r="56" spans="1:52" x14ac:dyDescent="0.2">
+      <c r="BC55" s="3"/>
+      <c r="BD55" s="3"/>
+    </row>
+    <row r="56" spans="1:56" x14ac:dyDescent="0.2">
       <c r="B56" s="2"/>
       <c r="C56" s="2"/>
       <c r="D56" s="2"/>
@@ -6332,8 +7474,10 @@
       <c r="AX56" s="2"/>
       <c r="AY56" s="2"/>
       <c r="AZ56" s="3"/>
-    </row>
-    <row r="57" spans="1:52" x14ac:dyDescent="0.2">
+      <c r="BC56" s="3"/>
+      <c r="BD56" s="3"/>
+    </row>
+    <row r="57" spans="1:56" x14ac:dyDescent="0.2">
       <c r="B57" s="2"/>
       <c r="C57" s="2"/>
       <c r="D57" s="2"/>
@@ -6385,8 +7529,10 @@
       <c r="AX57" s="2"/>
       <c r="AY57" s="2"/>
       <c r="AZ57" s="3"/>
-    </row>
-    <row r="58" spans="1:52" x14ac:dyDescent="0.2">
+      <c r="BC57" s="3"/>
+      <c r="BD57" s="3"/>
+    </row>
+    <row r="58" spans="1:56" x14ac:dyDescent="0.2">
       <c r="B58" s="2"/>
       <c r="C58" s="2"/>
       <c r="D58" s="2"/>
@@ -6438,8 +7584,10 @@
       <c r="AX58" s="2"/>
       <c r="AY58" s="2"/>
       <c r="AZ58" s="3"/>
-    </row>
-    <row r="59" spans="1:52" x14ac:dyDescent="0.2">
+      <c r="BC58" s="3"/>
+      <c r="BD58" s="3"/>
+    </row>
+    <row r="59" spans="1:56" x14ac:dyDescent="0.2">
       <c r="B59" s="2"/>
       <c r="C59" s="2"/>
       <c r="D59" s="2"/>
@@ -6491,8 +7639,10 @@
       <c r="AX59" s="2"/>
       <c r="AY59" s="2"/>
       <c r="AZ59" s="3"/>
-    </row>
-    <row r="60" spans="1:52" x14ac:dyDescent="0.2">
+      <c r="BC59" s="3"/>
+      <c r="BD59" s="3"/>
+    </row>
+    <row r="60" spans="1:56" x14ac:dyDescent="0.2">
       <c r="B60" s="2"/>
       <c r="C60" s="2"/>
       <c r="D60" s="2"/>
@@ -6544,8 +7694,9 @@
       <c r="AX60" s="2"/>
       <c r="AY60" s="2"/>
       <c r="AZ60" s="3"/>
-    </row>
-    <row r="61" spans="1:52" x14ac:dyDescent="0.2">
+      <c r="BD60" s="3"/>
+    </row>
+    <row r="61" spans="1:56" x14ac:dyDescent="0.2">
       <c r="B61" s="2"/>
       <c r="C61" s="2"/>
       <c r="D61" s="2"/>
@@ -6598,17 +7749,17 @@
       <c r="AY61" s="2"/>
       <c r="AZ61" s="3"/>
     </row>
-    <row r="62" spans="1:52" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:56" x14ac:dyDescent="0.2">
       <c r="I62" s="3"/>
       <c r="AG62" s="3"/>
       <c r="AZ62" s="3"/>
     </row>
-    <row r="63" spans="1:52" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:56" x14ac:dyDescent="0.2">
       <c r="I63" s="3"/>
       <c r="AG63" s="3"/>
       <c r="AZ63" s="3"/>
     </row>
-    <row r="64" spans="1:52" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:56" x14ac:dyDescent="0.2">
       <c r="I64" s="3"/>
       <c r="AG64" s="3"/>
       <c r="AZ64" s="3"/>
@@ -6796,7 +7947,6 @@
         <filter val="South Dakota"/>
         <filter val="Texas"/>
         <filter val="Utah"/>
-        <filter val="Vermont"/>
         <filter val="West Virginia"/>
       </filters>
     </filterColumn>

</xml_diff>

<commit_message>
Andrew | Analyzed about half of the registration.
</commit_message>
<xml_diff>
--- a/compliance/State Compliance Analysis.xlsx
+++ b/compliance/State Compliance Analysis.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/andrewhetzler/Documents/Documents - Andrew’s Money Maker/School/DISSERTATION/GitHub/dissertation/compliance/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B5B98A61-BDAA-5240-B411-37546AB5F25A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{56FC8693-E4A1-E644-B14D-CE0C23A153A3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="40960" windowHeight="24400" activeTab="1" xr2:uid="{FEE3D6CA-2CD0-2B4F-9478-6397B247951E}"/>
+    <workbookView xWindow="-20" yWindow="500" windowWidth="40960" windowHeight="24400" activeTab="2" xr2:uid="{FEE3D6CA-2CD0-2B4F-9478-6397B247951E}"/>
   </bookViews>
   <sheets>
     <sheet name="Insurance" sheetId="1" r:id="rId1"/>
@@ -43,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1251" uniqueCount="254">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1365" uniqueCount="283">
   <si>
     <t>STATE</t>
   </si>
@@ -1341,6 +1341,114 @@
   </si>
   <si>
     <t>Optional (17B-2-8(b))</t>
+  </si>
+  <si>
+    <t>ISSUE DATE</t>
+  </si>
+  <si>
+    <t>REGISTRATION #</t>
+  </si>
+  <si>
+    <t>ADDRESS</t>
+  </si>
+  <si>
+    <t>DESCRIPTION OF VEHICLE</t>
+  </si>
+  <si>
+    <t>SERIAL #</t>
+  </si>
+  <si>
+    <t>Not applicable</t>
+  </si>
+  <si>
+    <t>Required (28-2158(B)(1)</t>
+  </si>
+  <si>
+    <t>Required (28-2158(B)(2)</t>
+  </si>
+  <si>
+    <t>Required (28-2158(B)(3)</t>
+  </si>
+  <si>
+    <t>Required (28-2158(B)(4)</t>
+  </si>
+  <si>
+    <t>Required (28-2158(B)(5)</t>
+  </si>
+  <si>
+    <t>AMOUNT OF FEES PAID TO REGISTER</t>
+  </si>
+  <si>
+    <t>Required (27-14-714(a)(1))</t>
+  </si>
+  <si>
+    <t>Required (27-14-713(b)(1))</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Not mentioned </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">NOTE: </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>would fall under description of vehicle.</t>
+    </r>
+  </si>
+  <si>
+    <t>FULLY AUTONOMOUS VEHICLE DISTINCTION</t>
+  </si>
+  <si>
+    <t>Required (S-219((3); 40-8-11(a)(5))</t>
+  </si>
+  <si>
+    <t>Required (H-7(4))</t>
+  </si>
+  <si>
+    <t>Required (H-1003(9)(1))</t>
+  </si>
+  <si>
+    <t>Required (H-469(1)(20-401)(f)(5)</t>
+  </si>
+  <si>
+    <t>Required (S-1541(5))</t>
+  </si>
+  <si>
+    <t>Required (H-4787(17H-1-9)(2)(b))</t>
+  </si>
+  <si>
+    <t>Required (S-313(7)(a))</t>
+  </si>
+  <si>
+    <t>OTHER STATEMENT OF FACTS</t>
+  </si>
+  <si>
+    <t>Required (8-131(a))</t>
+  </si>
+  <si>
+    <t>Required (186.040(2)</t>
+  </si>
+  <si>
+    <t>Required (20-57(b))</t>
+  </si>
+  <si>
+    <t>MULTIPLE OWNER DISTINCTION</t>
+  </si>
+  <si>
+    <t>Optional--only required if 2+ owners (20-57(b))</t>
   </si>
 </sst>
 </file>
@@ -1409,7 +1517,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1425,6 +1533,9 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1760,14 +1871,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4E61F571-54A4-994C-A02B-889943573726}">
+  <sheetPr filterMode="1"/>
   <dimension ref="A1:A51"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" sqref="A1:A1048576"/>
+      <selection pane="topRight" activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="14.5" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
@@ -1779,7 +1894,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A3" s="3" t="s">
         <v>10</v>
       </c>
@@ -1799,17 +1914,17 @@
         <v>13</v>
       </c>
     </row>
-    <row r="7" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A7" s="3" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="8" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A8" s="3" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="9" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A9" s="3" t="s">
         <v>15</v>
       </c>
@@ -1824,22 +1939,22 @@
         <v>17</v>
       </c>
     </row>
-    <row r="12" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A12" s="3" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="13" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A13" s="3" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="14" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A14" s="3" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="15" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A15" s="3" t="s">
         <v>20</v>
       </c>
@@ -1864,27 +1979,27 @@
         <v>25</v>
       </c>
     </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A20" s="3" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A21" s="3" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A22" s="3" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A23" s="3" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="24" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A24" s="3" t="s">
         <v>30</v>
       </c>
@@ -1894,42 +2009,42 @@
         <v>31</v>
       </c>
     </row>
-    <row r="26" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A26" s="3" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="27" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A27" s="3" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="28" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A28" s="3" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="29" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A29" s="3" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="30" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A30" s="3" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="31" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A31" s="3" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="32" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A32" s="3" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="33" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A33" s="3" t="s">
         <v>39</v>
       </c>
@@ -1944,7 +2059,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="36" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A36" s="3" t="s">
         <v>42</v>
       </c>
@@ -1954,7 +2069,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="38" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A38" s="3" t="s">
         <v>44</v>
       </c>
@@ -1964,12 +2079,12 @@
         <v>45</v>
       </c>
     </row>
-    <row r="40" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A40" s="3" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="41" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A41" s="3" t="s">
         <v>47</v>
       </c>
@@ -1979,7 +2094,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="43" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A43" s="3" t="s">
         <v>49</v>
       </c>
@@ -1999,12 +2114,12 @@
         <v>52</v>
       </c>
     </row>
-    <row r="47" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A47" s="3" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="48" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A48" s="3" t="s">
         <v>54</v>
       </c>
@@ -2014,18 +2129,43 @@
         <v>55</v>
       </c>
     </row>
-    <row r="50" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A50" s="3" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="51" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A51" s="3" t="s">
         <v>56</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:A51" xr:uid="{4E61F571-54A4-994C-A02B-889943573726}"/>
+  <autoFilter ref="A1:A51" xr:uid="{4E61F571-54A4-994C-A02B-889943573726}">
+    <filterColumn colId="0">
+      <filters>
+        <filter val="Alabama"/>
+        <filter val="Arizona"/>
+        <filter val="Arkansas"/>
+        <filter val="California"/>
+        <filter val="Florida"/>
+        <filter val="Georgia"/>
+        <filter val="Iowa"/>
+        <filter val="Kansas"/>
+        <filter val="Kentucky"/>
+        <filter val="Louisiana"/>
+        <filter val="Mississippi"/>
+        <filter val="North Carolina"/>
+        <filter val="North Dakota"/>
+        <filter val="Oklahoma"/>
+        <filter val="Pennsylvania"/>
+        <filter val="South Dakota"/>
+        <filter val="Texas"/>
+        <filter val="Utah"/>
+        <filter val="Vermont"/>
+        <filter val="West Virginia"/>
+      </filters>
+    </filterColumn>
+  </autoFilter>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -2035,8 +2175,8 @@
   <sheetPr filterMode="1"/>
   <dimension ref="A1:BD110"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A17" activePane="bottomLeft" state="frozen"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="BE49" sqref="BE49"/>
     </sheetView>
   </sheetViews>
@@ -7957,272 +8097,859 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{48541A15-86EE-DC49-B72C-33AAB33B8C19}">
-  <dimension ref="A1:A51"/>
+  <sheetPr filterMode="1"/>
+  <dimension ref="A1:T54"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" sqref="A1:A1048576"/>
+      <selection pane="topRight" activeCell="K34" sqref="K34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="15" customWidth="1"/>
+    <col min="2" max="2" width="22.83203125" customWidth="1"/>
+    <col min="3" max="3" width="22" customWidth="1"/>
+    <col min="4" max="4" width="22.83203125" customWidth="1"/>
+    <col min="5" max="5" width="26.1640625" customWidth="1"/>
+    <col min="6" max="6" width="24.83203125" customWidth="1"/>
+    <col min="7" max="7" width="21.5" customWidth="1"/>
+    <col min="8" max="8" width="32.5" customWidth="1"/>
+    <col min="9" max="9" width="31.33203125" customWidth="1"/>
+    <col min="10" max="10" width="41.1640625" customWidth="1"/>
+    <col min="11" max="11" width="39" customWidth="1"/>
+    <col min="12" max="12" width="30.33203125" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B1" s="1" t="s">
+        <v>254</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>255</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>256</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>257</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>258</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>265</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>269</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>277</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>281</v>
+      </c>
+      <c r="M1" s="1"/>
+      <c r="N1" s="1"/>
+      <c r="O1" s="1"/>
+      <c r="P1" s="1"/>
+      <c r="Q1" s="1"/>
+      <c r="R1" s="1"/>
+      <c r="S1" s="1"/>
+      <c r="T1" s="6"/>
+    </row>
+    <row r="2" spans="1:20" ht="17" x14ac:dyDescent="0.2">
       <c r="A2" s="3" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B2" s="2" t="s">
+        <v>259</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>259</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>259</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>259</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>259</v>
+      </c>
+      <c r="G2" s="2" t="s">
+        <v>259</v>
+      </c>
+      <c r="H2" s="2" t="s">
+        <v>259</v>
+      </c>
+      <c r="I2" s="2" t="s">
+        <v>259</v>
+      </c>
+      <c r="J2" s="2" t="s">
+        <v>259</v>
+      </c>
+      <c r="K2" s="2" t="s">
+        <v>259</v>
+      </c>
+      <c r="L2" s="2"/>
+      <c r="M2" s="2"/>
+      <c r="N2" s="2"/>
+    </row>
+    <row r="3" spans="1:20" hidden="1" x14ac:dyDescent="0.2">
       <c r="A3" s="3" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:20" ht="17" x14ac:dyDescent="0.2">
       <c r="A4" s="3" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B4" s="2" t="s">
+        <v>260</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>261</v>
+      </c>
+      <c r="D4" s="4" t="s">
+        <v>262</v>
+      </c>
+      <c r="E4" s="4" t="s">
+        <v>262</v>
+      </c>
+      <c r="F4" s="4" t="s">
+        <v>263</v>
+      </c>
+      <c r="G4" s="4" t="s">
+        <v>263</v>
+      </c>
+      <c r="H4" s="4" t="s">
+        <v>264</v>
+      </c>
+      <c r="I4" s="4" t="s">
+        <v>80</v>
+      </c>
+      <c r="J4" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="K4" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="L4" s="2"/>
+      <c r="M4" s="2"/>
+      <c r="N4" s="2"/>
+    </row>
+    <row r="5" spans="1:20" ht="51" x14ac:dyDescent="0.2">
       <c r="A5" s="3" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B5" s="2" t="s">
+        <v>267</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>267</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>267</v>
+      </c>
+      <c r="E5" s="2" t="s">
+        <v>267</v>
+      </c>
+      <c r="F5" s="2" t="s">
+        <v>267</v>
+      </c>
+      <c r="G5" s="2" t="s">
+        <v>268</v>
+      </c>
+      <c r="H5" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="I5" s="2" t="s">
+        <v>266</v>
+      </c>
+      <c r="J5" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="K5" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="L5" s="2"/>
+      <c r="M5" s="2"/>
+      <c r="N5" s="2"/>
+    </row>
+    <row r="6" spans="1:20" hidden="1" x14ac:dyDescent="0.2">
       <c r="A6" s="3" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="7" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B6" s="2"/>
+      <c r="C6" s="2"/>
+      <c r="D6" s="2"/>
+      <c r="E6" s="2"/>
+      <c r="F6" s="2"/>
+      <c r="G6" s="2"/>
+      <c r="H6" s="2"/>
+      <c r="I6" s="2"/>
+      <c r="J6" s="2"/>
+      <c r="K6" s="2"/>
+      <c r="L6" s="2"/>
+      <c r="M6" s="2"/>
+      <c r="N6" s="2"/>
+    </row>
+    <row r="7" spans="1:20" hidden="1" x14ac:dyDescent="0.2">
       <c r="A7" s="3" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="8" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:20" hidden="1" x14ac:dyDescent="0.2">
       <c r="A8" s="3" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="9" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:20" hidden="1" x14ac:dyDescent="0.2">
       <c r="A9" s="3" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="10" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:20" ht="17" x14ac:dyDescent="0.2">
       <c r="A10" s="3" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="11" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B10" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="D10" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="E10" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="F10" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="G10" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="H10" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="I10" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="J10" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="K10" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="L10" s="2"/>
+      <c r="M10" s="2"/>
+      <c r="N10" s="2"/>
+    </row>
+    <row r="11" spans="1:20" ht="17" x14ac:dyDescent="0.2">
       <c r="A11" s="3" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="12" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B11" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="C11" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="D11" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="E11" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="F11" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="G11" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="H11" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="I11" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="J11" s="2" t="s">
+        <v>270</v>
+      </c>
+      <c r="K11" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="L11" s="2"/>
+      <c r="M11" s="2"/>
+      <c r="N11" s="2"/>
+    </row>
+    <row r="12" spans="1:20" hidden="1" x14ac:dyDescent="0.2">
       <c r="A12" s="3" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="13" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:20" hidden="1" x14ac:dyDescent="0.2">
       <c r="A13" s="3" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="14" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:20" hidden="1" x14ac:dyDescent="0.2">
       <c r="A14" s="3" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="15" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:20" hidden="1" x14ac:dyDescent="0.2">
       <c r="A15" s="3" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="16" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:20" hidden="1" x14ac:dyDescent="0.2">
       <c r="A16" s="3" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B16" s="2"/>
+      <c r="C16" s="2"/>
+      <c r="D16" s="2"/>
+      <c r="E16" s="2"/>
+      <c r="F16" s="2"/>
+      <c r="G16" s="2"/>
+      <c r="H16" s="2"/>
+      <c r="I16" s="2"/>
+      <c r="J16" s="2"/>
+      <c r="K16" s="2"/>
+      <c r="L16" s="2"/>
+      <c r="M16" s="2"/>
+      <c r="N16" s="2"/>
+    </row>
+    <row r="17" spans="1:14" ht="17" x14ac:dyDescent="0.2">
       <c r="A17" s="3" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B17" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="C17" s="2" t="s">
+        <v>278</v>
+      </c>
+      <c r="D17" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="E17" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="F17" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="G17" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="H17" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="I17" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="J17" s="2" t="s">
+        <v>276</v>
+      </c>
+      <c r="K17" s="2" t="s">
+        <v>278</v>
+      </c>
+      <c r="L17" s="2"/>
+      <c r="M17" s="2"/>
+      <c r="N17" s="2"/>
+    </row>
+    <row r="18" spans="1:14" ht="17" x14ac:dyDescent="0.2">
       <c r="A18" s="3" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B18" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="C18" s="2" t="s">
+        <v>279</v>
+      </c>
+      <c r="D18" s="2" t="s">
+        <v>279</v>
+      </c>
+      <c r="E18" s="2" t="s">
+        <v>279</v>
+      </c>
+      <c r="F18" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="G18" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="H18" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="I18" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="J18" s="2" t="s">
+        <v>271</v>
+      </c>
+      <c r="K18" s="2" t="s">
+        <v>279</v>
+      </c>
+      <c r="L18" s="2"/>
+      <c r="M18" s="2"/>
+      <c r="N18" s="2"/>
+    </row>
+    <row r="19" spans="1:14" ht="17" x14ac:dyDescent="0.2">
       <c r="A19" s="3" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B19" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="C19" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="D19" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="E19" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="F19" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="G19" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="H19" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="I19" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="J19" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="K19" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="L19" s="2"/>
+      <c r="M19" s="2"/>
+      <c r="N19" s="2"/>
+    </row>
+    <row r="20" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A20" s="3" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A21" s="3" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A22" s="3" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A23" s="3" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="24" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A24" s="3" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="25" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A25" s="3" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="26" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B25" t="s">
+        <v>80</v>
+      </c>
+      <c r="C25" t="s">
+        <v>80</v>
+      </c>
+      <c r="D25" t="s">
+        <v>80</v>
+      </c>
+      <c r="E25" t="s">
+        <v>80</v>
+      </c>
+      <c r="F25" t="s">
+        <v>80</v>
+      </c>
+      <c r="G25" t="s">
+        <v>80</v>
+      </c>
+      <c r="H25" t="s">
+        <v>80</v>
+      </c>
+      <c r="I25" t="s">
+        <v>80</v>
+      </c>
+      <c r="J25" t="s">
+        <v>272</v>
+      </c>
+      <c r="K25" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="26" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A26" s="3" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="27" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A27" s="3" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="28" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A28" s="3" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="29" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A29" s="3" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="30" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A30" s="3" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="31" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A31" s="3" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="32" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A32" s="3" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="33" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A33" s="3" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="34" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:14" ht="34" x14ac:dyDescent="0.2">
       <c r="A34" s="3" t="s">
         <v>40</v>
       </c>
-    </row>
-    <row r="35" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B34" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="C34" s="2" t="s">
+        <v>280</v>
+      </c>
+      <c r="D34" s="2" t="s">
+        <v>280</v>
+      </c>
+      <c r="E34" s="2" t="s">
+        <v>280</v>
+      </c>
+      <c r="F34" s="2" t="s">
+        <v>280</v>
+      </c>
+      <c r="G34" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="H34" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="I34" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="J34" s="2" t="s">
+        <v>273</v>
+      </c>
+      <c r="K34" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="L34" s="2" t="s">
+        <v>282</v>
+      </c>
+      <c r="M34" s="2"/>
+      <c r="N34" s="2"/>
+    </row>
+    <row r="35" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A35" s="3" t="s">
         <v>41</v>
       </c>
-    </row>
-    <row r="36" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B35" s="2"/>
+      <c r="C35" s="2"/>
+      <c r="D35" s="2"/>
+      <c r="E35" s="2"/>
+      <c r="F35" s="2"/>
+      <c r="G35" s="2"/>
+      <c r="H35" s="2"/>
+      <c r="I35" s="2"/>
+      <c r="J35" s="2"/>
+      <c r="K35" s="2"/>
+      <c r="L35" s="2"/>
+      <c r="M35" s="2"/>
+      <c r="N35" s="2"/>
+    </row>
+    <row r="36" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A36" s="3" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="37" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:14" ht="17" x14ac:dyDescent="0.2">
       <c r="A37" s="3" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="38" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B37" s="2"/>
+      <c r="C37" s="2"/>
+      <c r="D37" s="2"/>
+      <c r="E37" s="2"/>
+      <c r="F37" s="2"/>
+      <c r="G37" s="2"/>
+      <c r="H37" s="2"/>
+      <c r="I37" s="2"/>
+      <c r="J37" s="2" t="s">
+        <v>274</v>
+      </c>
+      <c r="K37" s="2"/>
+      <c r="L37" s="2"/>
+      <c r="M37" s="2"/>
+      <c r="N37" s="2"/>
+    </row>
+    <row r="38" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A38" s="3" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="39" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A39" s="3" t="s">
         <v>45</v>
       </c>
-    </row>
-    <row r="40" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B39" s="2"/>
+      <c r="C39" s="2"/>
+      <c r="D39" s="2"/>
+      <c r="E39" s="2"/>
+      <c r="F39" s="2"/>
+      <c r="G39" s="2"/>
+      <c r="H39" s="2"/>
+      <c r="I39" s="2"/>
+      <c r="J39" s="2"/>
+      <c r="K39" s="2"/>
+      <c r="L39" s="2"/>
+      <c r="M39" s="2"/>
+      <c r="N39" s="2"/>
+    </row>
+    <row r="40" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A40" s="3" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="41" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A41" s="3" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="42" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A42" s="3" t="s">
         <v>48</v>
       </c>
-    </row>
-    <row r="43" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B42" s="2"/>
+      <c r="C42" s="2"/>
+      <c r="D42" s="2"/>
+      <c r="E42" s="2"/>
+      <c r="F42" s="2"/>
+      <c r="G42" s="2"/>
+      <c r="H42" s="2"/>
+      <c r="I42" s="2"/>
+      <c r="J42" s="2"/>
+      <c r="K42" s="2"/>
+      <c r="L42" s="2"/>
+      <c r="M42" s="2"/>
+      <c r="N42" s="2"/>
+    </row>
+    <row r="43" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A43" s="3" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="44" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A44" s="3" t="s">
         <v>50</v>
       </c>
-    </row>
-    <row r="45" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B44" s="2"/>
+      <c r="C44" s="2"/>
+      <c r="D44" s="2"/>
+      <c r="E44" s="2"/>
+      <c r="F44" s="2"/>
+      <c r="G44" s="2"/>
+      <c r="H44" s="2"/>
+      <c r="I44" s="2"/>
+      <c r="J44" s="2"/>
+      <c r="K44" s="2"/>
+      <c r="L44" s="2"/>
+      <c r="M44" s="2"/>
+      <c r="N44" s="2"/>
+    </row>
+    <row r="45" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A45" s="3" t="s">
         <v>51</v>
       </c>
-    </row>
-    <row r="46" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B45" s="2"/>
+      <c r="C45" s="2"/>
+      <c r="D45" s="2"/>
+      <c r="E45" s="2"/>
+      <c r="F45" s="2"/>
+      <c r="G45" s="2"/>
+      <c r="H45" s="2"/>
+      <c r="I45" s="2"/>
+      <c r="J45" s="2"/>
+      <c r="K45" s="2"/>
+      <c r="L45" s="2"/>
+      <c r="M45" s="2"/>
+      <c r="N45" s="2"/>
+    </row>
+    <row r="46" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A46" s="3" t="s">
         <v>52</v>
       </c>
-    </row>
-    <row r="47" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B46" s="2"/>
+      <c r="C46" s="2"/>
+      <c r="D46" s="2"/>
+      <c r="E46" s="2"/>
+      <c r="F46" s="2"/>
+      <c r="G46" s="2"/>
+      <c r="H46" s="2"/>
+      <c r="I46" s="2"/>
+      <c r="J46" s="2"/>
+      <c r="K46" s="2"/>
+      <c r="L46" s="2"/>
+      <c r="M46" s="2"/>
+      <c r="N46" s="2"/>
+    </row>
+    <row r="47" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A47" s="3" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="48" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A48" s="3" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="49" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:14" ht="17" x14ac:dyDescent="0.2">
       <c r="A49" s="3" t="s">
         <v>55</v>
       </c>
-    </row>
-    <row r="50" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B49" s="2"/>
+      <c r="C49" s="2"/>
+      <c r="D49" s="2"/>
+      <c r="E49" s="2"/>
+      <c r="F49" s="2"/>
+      <c r="G49" s="2"/>
+      <c r="H49" s="2"/>
+      <c r="I49" s="2"/>
+      <c r="J49" s="2" t="s">
+        <v>275</v>
+      </c>
+      <c r="K49" s="2"/>
+      <c r="L49" s="2"/>
+      <c r="M49" s="2"/>
+      <c r="N49" s="2"/>
+    </row>
+    <row r="50" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A50" s="3" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="51" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A51" s="3" t="s">
         <v>56</v>
       </c>
     </row>
+    <row r="52" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="B52" s="2"/>
+      <c r="C52" s="2"/>
+      <c r="D52" s="2"/>
+      <c r="E52" s="2"/>
+      <c r="F52" s="2"/>
+      <c r="G52" s="2"/>
+      <c r="H52" s="2"/>
+      <c r="I52" s="2"/>
+      <c r="J52" s="2"/>
+      <c r="K52" s="2"/>
+      <c r="L52" s="2"/>
+      <c r="M52" s="2"/>
+      <c r="N52" s="2"/>
+    </row>
+    <row r="53" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="B53" s="2"/>
+      <c r="C53" s="2"/>
+      <c r="D53" s="2"/>
+      <c r="E53" s="2"/>
+      <c r="F53" s="2"/>
+      <c r="G53" s="2"/>
+      <c r="H53" s="2"/>
+      <c r="I53" s="2"/>
+      <c r="J53" s="2"/>
+      <c r="K53" s="2"/>
+      <c r="L53" s="2"/>
+      <c r="M53" s="2"/>
+      <c r="N53" s="2"/>
+    </row>
+    <row r="54" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="B54" s="2"/>
+      <c r="C54" s="2"/>
+      <c r="D54" s="2"/>
+      <c r="E54" s="2"/>
+      <c r="F54" s="2"/>
+      <c r="G54" s="2"/>
+      <c r="H54" s="2"/>
+      <c r="I54" s="2"/>
+      <c r="J54" s="2"/>
+      <c r="K54" s="2"/>
+      <c r="L54" s="2"/>
+      <c r="M54" s="2"/>
+      <c r="N54" s="2"/>
+    </row>
   </sheetData>
-  <autoFilter ref="A1:A51" xr:uid="{48541A15-86EE-DC49-B72C-33AAB33B8C19}"/>
+  <autoFilter ref="A1:A51" xr:uid="{48541A15-86EE-DC49-B72C-33AAB33B8C19}">
+    <filterColumn colId="0">
+      <filters>
+        <filter val="Alabama"/>
+        <filter val="Arizona"/>
+        <filter val="Arkansas"/>
+        <filter val="Florida"/>
+        <filter val="Georgia"/>
+        <filter val="Kansas"/>
+        <filter val="Kentucky"/>
+        <filter val="Louisiana"/>
+        <filter val="Mississippi"/>
+        <filter val="North Carolina"/>
+        <filter val="North Dakota"/>
+        <filter val="Oklahoma"/>
+        <filter val="Pennsylvania"/>
+        <filter val="South Dakota"/>
+        <filter val="Texas"/>
+        <filter val="Utah"/>
+        <filter val="Vermont"/>
+        <filter val="West Virginia"/>
+      </filters>
+    </filterColumn>
+  </autoFilter>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Andrew | Finished registration.
</commit_message>
<xml_diff>
--- a/compliance/State Compliance Analysis.xlsx
+++ b/compliance/State Compliance Analysis.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/andrewhetzler/Documents/Documents - Andrew’s Money Maker/School/DISSERTATION/GitHub/dissertation/compliance/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{56FC8693-E4A1-E644-B14D-CE0C23A153A3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C4C35EA4-7FA4-F145-9E2D-4DE6DF48EF34}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-20" yWindow="500" windowWidth="40960" windowHeight="24400" activeTab="2" xr2:uid="{FEE3D6CA-2CD0-2B4F-9478-6397B247951E}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="40960" windowHeight="24400" activeTab="2" xr2:uid="{FEE3D6CA-2CD0-2B4F-9478-6397B247951E}"/>
   </bookViews>
   <sheets>
     <sheet name="Insurance" sheetId="1" r:id="rId1"/>
@@ -43,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1365" uniqueCount="283">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1606" uniqueCount="312">
   <si>
     <t>STATE</t>
   </si>
@@ -1424,9 +1424,6 @@
     <t>Required (H-469(1)(20-401)(f)(5)</t>
   </si>
   <si>
-    <t>Required (S-1541(5))</t>
-  </si>
-  <si>
     <t>Required (H-4787(17H-1-9)(2)(b))</t>
   </si>
   <si>
@@ -1449,6 +1446,138 @@
   </si>
   <si>
     <t>Optional--only required if 2+ owners (20-57(b))</t>
+  </si>
+  <si>
+    <t>DIRECTOR SIGNATURE</t>
+  </si>
+  <si>
+    <t>B</t>
+  </si>
+  <si>
+    <t>TILE/LIEN STATEMENT</t>
+  </si>
+  <si>
+    <t>Repealed</t>
+  </si>
+  <si>
+    <t>Required (S-1541(5)(A))</t>
+  </si>
+  <si>
+    <t>Required (1308)(a)</t>
+  </si>
+  <si>
+    <t>NAME OF OWNER</t>
+  </si>
+  <si>
+    <t>Optional--only required if registrant name is different than owner (1308)(a)</t>
+  </si>
+  <si>
+    <t>GROSS WEIGHT</t>
+  </si>
+  <si>
+    <t>GROSS WEIGHT COMBINATION</t>
+  </si>
+  <si>
+    <t>PASSENGER SEAT CAPACITY</t>
+  </si>
+  <si>
+    <t>Optional--only required for specific types (1308)(b), (c), and (d)</t>
+  </si>
+  <si>
+    <t>Optional--only required for specific types (1308)(b) and ©</t>
+  </si>
+  <si>
+    <t>Optional--only required for buses (1308)(e)</t>
+  </si>
+  <si>
+    <t>Required (32-5-90)</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Required (32-5-90) </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>NOTE:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> specifically calls out: make, model year, and model</t>
+    </r>
+  </si>
+  <si>
+    <t>Required (41-1a-213)(2)(a)</t>
+  </si>
+  <si>
+    <t>Required (41-1a-213)(2)(b)</t>
+  </si>
+  <si>
+    <r>
+      <t>Required (41-1a-213)(2)(C )</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>NOTE:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> must include year, make, VIN, and license plate</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">Required (41-1a-213)(2)(c ) see description of vehicle </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Required (41-1a-213)(2)(d) </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Required (41-1a-213)(2)(e) </t>
+  </si>
+  <si>
+    <t>(Could be license plate mentioned in description of vehicle)</t>
+  </si>
+  <si>
+    <t>LESSEE NAME</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Optional--only required if leased more than 45 days ( (41-1a-213)(3)(b)) </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Optional--only required for specific types Required (41-1a-213)(4)) </t>
+  </si>
+  <si>
+    <t>Required ((23-304)(a))</t>
+  </si>
+  <si>
+    <t>Not mentioned NOTE: would fall under description of vehicle.</t>
+  </si>
+  <si>
+    <t>Required (17A-3-10)</t>
+  </si>
+  <si>
+    <t>Required (17A-3-11)</t>
   </si>
 </sst>
 </file>
@@ -1517,7 +1646,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1533,9 +1662,6 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -2176,7 +2302,7 @@
   <dimension ref="A1:BD110"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="1" topLeftCell="A17" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="BE49" sqref="BE49"/>
     </sheetView>
   </sheetViews>
@@ -8098,11 +8224,11 @@
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{48541A15-86EE-DC49-B72C-33AAB33B8C19}">
   <sheetPr filterMode="1"/>
-  <dimension ref="A1:T54"/>
+  <dimension ref="A1:U58"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="K34" sqref="K34"/>
+      <pane xSplit="1" topLeftCell="K1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="T49" sqref="T49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -8113,15 +8239,23 @@
     <col min="4" max="4" width="22.83203125" customWidth="1"/>
     <col min="5" max="5" width="26.1640625" customWidth="1"/>
     <col min="6" max="6" width="24.83203125" customWidth="1"/>
-    <col min="7" max="7" width="21.5" customWidth="1"/>
+    <col min="7" max="7" width="23.6640625" customWidth="1"/>
     <col min="8" max="8" width="32.5" customWidth="1"/>
     <col min="9" max="9" width="31.33203125" customWidth="1"/>
     <col min="10" max="10" width="41.1640625" customWidth="1"/>
     <col min="11" max="11" width="39" customWidth="1"/>
     <col min="12" max="12" width="30.33203125" customWidth="1"/>
+    <col min="13" max="13" width="37.83203125" customWidth="1"/>
+    <col min="14" max="14" width="32.6640625" customWidth="1"/>
+    <col min="15" max="15" width="30.83203125" customWidth="1"/>
+    <col min="16" max="16" width="33.1640625" customWidth="1"/>
+    <col min="17" max="17" width="21.1640625" customWidth="1"/>
+    <col min="18" max="18" width="25.1640625" customWidth="1"/>
+    <col min="19" max="19" width="25.83203125" customWidth="1"/>
+    <col min="20" max="20" width="28" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -8153,21 +8287,37 @@
         <v>269</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="L1" s="1" t="s">
-        <v>281</v>
-      </c>
-      <c r="M1" s="1"/>
-      <c r="N1" s="1"/>
-      <c r="O1" s="1"/>
-      <c r="P1" s="1"/>
-      <c r="Q1" s="1"/>
-      <c r="R1" s="1"/>
-      <c r="S1" s="1"/>
-      <c r="T1" s="6"/>
-    </row>
-    <row r="2" spans="1:20" ht="17" x14ac:dyDescent="0.2">
+        <v>280</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>282</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>284</v>
+      </c>
+      <c r="O1" s="1" t="s">
+        <v>288</v>
+      </c>
+      <c r="P1" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="Q1" s="1" t="s">
+        <v>290</v>
+      </c>
+      <c r="R1" s="1" t="s">
+        <v>291</v>
+      </c>
+      <c r="S1" s="1" t="s">
+        <v>292</v>
+      </c>
+      <c r="T1" s="1" t="s">
+        <v>305</v>
+      </c>
+    </row>
+    <row r="2" spans="1:21" ht="17" x14ac:dyDescent="0.2">
       <c r="A2" s="3" t="s">
         <v>9</v>
       </c>
@@ -8201,16 +8351,41 @@
       <c r="K2" s="2" t="s">
         <v>259</v>
       </c>
-      <c r="L2" s="2"/>
-      <c r="M2" s="2"/>
-      <c r="N2" s="2"/>
-    </row>
-    <row r="3" spans="1:20" hidden="1" x14ac:dyDescent="0.2">
+      <c r="L2" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="M2" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="N2" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="O2" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="P2" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="Q2" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="R2" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="S2" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="T2" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="U2" s="2"/>
+    </row>
+    <row r="3" spans="1:21" hidden="1" x14ac:dyDescent="0.2">
       <c r="A3" s="3" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="4" spans="1:20" ht="17" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:21" ht="17" x14ac:dyDescent="0.2">
       <c r="A4" s="3" t="s">
         <v>11</v>
       </c>
@@ -8244,11 +8419,36 @@
       <c r="K4" s="2" t="s">
         <v>80</v>
       </c>
-      <c r="L4" s="2"/>
-      <c r="M4" s="2"/>
-      <c r="N4" s="2"/>
-    </row>
-    <row r="5" spans="1:20" ht="51" x14ac:dyDescent="0.2">
+      <c r="L4" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="M4" s="2" t="s">
+        <v>283</v>
+      </c>
+      <c r="N4" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="O4" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="P4" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="Q4" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="R4" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="S4" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="T4" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="U4" s="2"/>
+    </row>
+    <row r="5" spans="1:21" ht="51" x14ac:dyDescent="0.2">
       <c r="A5" s="3" t="s">
         <v>12</v>
       </c>
@@ -8282,11 +8482,36 @@
       <c r="K5" s="2" t="s">
         <v>80</v>
       </c>
-      <c r="L5" s="2"/>
-      <c r="M5" s="2"/>
-      <c r="N5" s="2"/>
-    </row>
-    <row r="6" spans="1:20" hidden="1" x14ac:dyDescent="0.2">
+      <c r="L5" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="M5" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="N5" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="O5" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="P5" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="Q5" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="R5" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="S5" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="T5" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="U5" s="2"/>
+    </row>
+    <row r="6" spans="1:21" hidden="1" x14ac:dyDescent="0.2">
       <c r="A6" s="3" t="s">
         <v>13</v>
       </c>
@@ -8304,22 +8529,22 @@
       <c r="M6" s="2"/>
       <c r="N6" s="2"/>
     </row>
-    <row r="7" spans="1:20" hidden="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:21" hidden="1" x14ac:dyDescent="0.2">
       <c r="A7" s="3" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="8" spans="1:20" hidden="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:21" hidden="1" x14ac:dyDescent="0.2">
       <c r="A8" s="3" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="9" spans="1:20" hidden="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:21" hidden="1" x14ac:dyDescent="0.2">
       <c r="A9" s="3" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="10" spans="1:20" ht="17" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:21" ht="17" x14ac:dyDescent="0.2">
       <c r="A10" s="3" t="s">
         <v>16</v>
       </c>
@@ -8353,11 +8578,36 @@
       <c r="K10" s="2" t="s">
         <v>80</v>
       </c>
-      <c r="L10" s="2"/>
-      <c r="M10" s="2"/>
-      <c r="N10" s="2"/>
-    </row>
-    <row r="11" spans="1:20" ht="17" x14ac:dyDescent="0.2">
+      <c r="L10" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="M10" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="N10" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="O10" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="P10" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="Q10" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="R10" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="S10" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="T10" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="U10" s="2"/>
+    </row>
+    <row r="11" spans="1:21" ht="17" x14ac:dyDescent="0.2">
       <c r="A11" s="3" t="s">
         <v>17</v>
       </c>
@@ -8391,31 +8641,56 @@
       <c r="K11" s="2" t="s">
         <v>80</v>
       </c>
-      <c r="L11" s="2"/>
-      <c r="M11" s="2"/>
-      <c r="N11" s="2"/>
-    </row>
-    <row r="12" spans="1:20" hidden="1" x14ac:dyDescent="0.2">
+      <c r="L11" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="M11" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="N11" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="O11" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="P11" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="Q11" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="R11" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="S11" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="T11" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="U11" s="2"/>
+    </row>
+    <row r="12" spans="1:21" hidden="1" x14ac:dyDescent="0.2">
       <c r="A12" s="3" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="13" spans="1:20" hidden="1" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:21" hidden="1" x14ac:dyDescent="0.2">
       <c r="A13" s="3" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="14" spans="1:20" hidden="1" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:21" hidden="1" x14ac:dyDescent="0.2">
       <c r="A14" s="3" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="15" spans="1:20" hidden="1" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:21" hidden="1" x14ac:dyDescent="0.2">
       <c r="A15" s="3" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="16" spans="1:20" hidden="1" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:21" hidden="1" x14ac:dyDescent="0.2">
       <c r="A16" s="3" t="s">
         <v>22</v>
       </c>
@@ -8433,7 +8708,7 @@
       <c r="M16" s="2"/>
       <c r="N16" s="2"/>
     </row>
-    <row r="17" spans="1:14" ht="17" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:21" ht="17" x14ac:dyDescent="0.2">
       <c r="A17" s="3" t="s">
         <v>23</v>
       </c>
@@ -8441,7 +8716,7 @@
         <v>80</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="D17" s="2" t="s">
         <v>80</v>
@@ -8462,16 +8737,41 @@
         <v>80</v>
       </c>
       <c r="J17" s="2" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="K17" s="2" t="s">
-        <v>278</v>
-      </c>
-      <c r="L17" s="2"/>
-      <c r="M17" s="2"/>
-      <c r="N17" s="2"/>
-    </row>
-    <row r="18" spans="1:14" ht="17" x14ac:dyDescent="0.2">
+        <v>277</v>
+      </c>
+      <c r="L17" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="M17" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="N17" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="O17" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="P17" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="Q17" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="R17" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="S17" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="T17" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="U17" s="2"/>
+    </row>
+    <row r="18" spans="1:21" ht="17" x14ac:dyDescent="0.2">
       <c r="A18" s="3" t="s">
         <v>24</v>
       </c>
@@ -8479,13 +8779,13 @@
         <v>80</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="D18" s="2" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="E18" s="2" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="F18" s="2" t="s">
         <v>80</v>
@@ -8503,13 +8803,38 @@
         <v>271</v>
       </c>
       <c r="K18" s="2" t="s">
-        <v>279</v>
-      </c>
-      <c r="L18" s="2"/>
-      <c r="M18" s="2"/>
-      <c r="N18" s="2"/>
-    </row>
-    <row r="19" spans="1:14" ht="17" x14ac:dyDescent="0.2">
+        <v>278</v>
+      </c>
+      <c r="L18" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="M18" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="N18" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="O18" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="P18" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="Q18" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="R18" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="S18" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="T18" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="U18" s="2"/>
+    </row>
+    <row r="19" spans="1:21" ht="17" x14ac:dyDescent="0.2">
       <c r="A19" s="3" t="s">
         <v>25</v>
       </c>
@@ -8543,36 +8868,61 @@
       <c r="K19" s="2" t="s">
         <v>80</v>
       </c>
-      <c r="L19" s="2"/>
-      <c r="M19" s="2"/>
-      <c r="N19" s="2"/>
-    </row>
-    <row r="20" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
+      <c r="L19" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="M19" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="N19" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="O19" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="P19" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="Q19" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="R19" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="S19" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="T19" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="U19" s="2"/>
+    </row>
+    <row r="20" spans="1:21" hidden="1" x14ac:dyDescent="0.2">
       <c r="A20" s="3" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="21" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:21" hidden="1" x14ac:dyDescent="0.2">
       <c r="A21" s="3" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="22" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:21" hidden="1" x14ac:dyDescent="0.2">
       <c r="A22" s="3" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="23" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:21" hidden="1" x14ac:dyDescent="0.2">
       <c r="A23" s="3" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="24" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:21" hidden="1" x14ac:dyDescent="0.2">
       <c r="A24" s="3" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="25" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:21" ht="17" x14ac:dyDescent="0.2">
       <c r="A25" s="3" t="s">
         <v>31</v>
       </c>
@@ -8606,48 +8956,76 @@
       <c r="K25" t="s">
         <v>80</v>
       </c>
-    </row>
-    <row r="26" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
+      <c r="L25" t="s">
+        <v>80</v>
+      </c>
+      <c r="M25" t="s">
+        <v>80</v>
+      </c>
+      <c r="N25" t="s">
+        <v>80</v>
+      </c>
+      <c r="O25" s="3" t="s">
+        <v>80</v>
+      </c>
+      <c r="P25" s="3" t="s">
+        <v>80</v>
+      </c>
+      <c r="Q25" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="R25" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="S25" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="T25" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="U25" s="2"/>
+    </row>
+    <row r="26" spans="1:21" hidden="1" x14ac:dyDescent="0.2">
       <c r="A26" s="3" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="27" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:21" hidden="1" x14ac:dyDescent="0.2">
       <c r="A27" s="3" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="28" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:21" hidden="1" x14ac:dyDescent="0.2">
       <c r="A28" s="3" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="29" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:21" hidden="1" x14ac:dyDescent="0.2">
       <c r="A29" s="3" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="30" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:21" hidden="1" x14ac:dyDescent="0.2">
       <c r="A30" s="3" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="31" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:21" hidden="1" x14ac:dyDescent="0.2">
       <c r="A31" s="3" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="32" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:21" hidden="1" x14ac:dyDescent="0.2">
       <c r="A32" s="3" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="33" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:21" hidden="1" x14ac:dyDescent="0.2">
       <c r="A33" s="3" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="34" spans="1:14" ht="34" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:21" ht="34" x14ac:dyDescent="0.2">
       <c r="A34" s="3" t="s">
         <v>40</v>
       </c>
@@ -8655,16 +9033,16 @@
         <v>80</v>
       </c>
       <c r="C34" s="2" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="D34" s="2" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="E34" s="2" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="F34" s="2" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="G34" s="2" t="s">
         <v>80</v>
@@ -8682,205 +9060,565 @@
         <v>80</v>
       </c>
       <c r="L34" s="2" t="s">
-        <v>282</v>
-      </c>
-      <c r="M34" s="2"/>
-      <c r="N34" s="2"/>
-    </row>
-    <row r="35" spans="1:14" x14ac:dyDescent="0.2">
+        <v>281</v>
+      </c>
+      <c r="M34" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="N34" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="O34" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="P34" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="Q34" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="R34" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="S34" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="T34" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="U34" s="2"/>
+    </row>
+    <row r="35" spans="1:21" ht="17" hidden="1" x14ac:dyDescent="0.2">
       <c r="A35" s="3" t="s">
         <v>41</v>
       </c>
-      <c r="B35" s="2"/>
-      <c r="C35" s="2"/>
-      <c r="D35" s="2"/>
-      <c r="E35" s="2"/>
-      <c r="F35" s="2"/>
-      <c r="G35" s="2"/>
-      <c r="H35" s="2"/>
-      <c r="I35" s="2"/>
-      <c r="J35" s="2"/>
-      <c r="K35" s="2"/>
-      <c r="L35" s="2"/>
-      <c r="M35" s="2"/>
-      <c r="N35" s="2"/>
-    </row>
-    <row r="36" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
+      <c r="B35" s="2" t="s">
+        <v>285</v>
+      </c>
+      <c r="C35" s="2" t="s">
+        <v>285</v>
+      </c>
+      <c r="D35" s="2" t="s">
+        <v>285</v>
+      </c>
+      <c r="E35" s="2" t="s">
+        <v>285</v>
+      </c>
+      <c r="F35" s="2" t="s">
+        <v>285</v>
+      </c>
+      <c r="G35" s="2" t="s">
+        <v>285</v>
+      </c>
+      <c r="H35" s="2" t="s">
+        <v>285</v>
+      </c>
+      <c r="I35" s="2" t="s">
+        <v>285</v>
+      </c>
+      <c r="J35" s="2" t="s">
+        <v>285</v>
+      </c>
+      <c r="K35" s="2" t="s">
+        <v>285</v>
+      </c>
+      <c r="L35" s="2" t="s">
+        <v>285</v>
+      </c>
+      <c r="M35" s="2" t="s">
+        <v>285</v>
+      </c>
+      <c r="N35" s="2" t="s">
+        <v>285</v>
+      </c>
+    </row>
+    <row r="36" spans="1:21" hidden="1" x14ac:dyDescent="0.2">
       <c r="A36" s="3" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="37" spans="1:14" ht="17" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:21" ht="17" x14ac:dyDescent="0.2">
       <c r="A37" s="3" t="s">
         <v>43</v>
       </c>
-      <c r="B37" s="2"/>
-      <c r="C37" s="2"/>
-      <c r="D37" s="2"/>
-      <c r="E37" s="2"/>
-      <c r="F37" s="2"/>
-      <c r="G37" s="2"/>
-      <c r="H37" s="2"/>
-      <c r="I37" s="2"/>
+      <c r="B37" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="C37" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="D37" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="E37" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="F37" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="G37" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="H37" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="I37" s="2" t="s">
+        <v>80</v>
+      </c>
       <c r="J37" s="2" t="s">
-        <v>274</v>
-      </c>
-      <c r="K37" s="2"/>
-      <c r="L37" s="2"/>
-      <c r="M37" s="2"/>
-      <c r="N37" s="2"/>
-    </row>
-    <row r="38" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
+        <v>286</v>
+      </c>
+      <c r="K37" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="L37" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="M37" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="N37" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="O37" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="P37" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="Q37" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="R37" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="S37" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="T37" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="U37" s="2"/>
+    </row>
+    <row r="38" spans="1:21" hidden="1" x14ac:dyDescent="0.2">
       <c r="A38" s="3" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="39" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:21" ht="51" x14ac:dyDescent="0.2">
       <c r="A39" s="3" t="s">
         <v>45</v>
       </c>
-      <c r="B39" s="2"/>
-      <c r="C39" s="2"/>
-      <c r="D39" s="2"/>
-      <c r="E39" s="2"/>
-      <c r="F39" s="2"/>
-      <c r="G39" s="2"/>
-      <c r="H39" s="2"/>
-      <c r="I39" s="2"/>
-      <c r="J39" s="2"/>
-      <c r="K39" s="2"/>
-      <c r="L39" s="2"/>
-      <c r="M39" s="2"/>
-      <c r="N39" s="2"/>
-    </row>
-    <row r="40" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
+      <c r="B39" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="C39" s="2" t="s">
+        <v>287</v>
+      </c>
+      <c r="D39" s="2" t="s">
+        <v>287</v>
+      </c>
+      <c r="E39" s="2" t="s">
+        <v>287</v>
+      </c>
+      <c r="F39" s="2" t="s">
+        <v>287</v>
+      </c>
+      <c r="G39" s="2" t="s">
+        <v>287</v>
+      </c>
+      <c r="H39" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="I39" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="J39" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="K39" s="2" t="s">
+        <v>287</v>
+      </c>
+      <c r="L39" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="M39" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="N39" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="O39" s="3" t="s">
+        <v>289</v>
+      </c>
+      <c r="P39" s="3" t="s">
+        <v>287</v>
+      </c>
+      <c r="Q39" s="2" t="s">
+        <v>293</v>
+      </c>
+      <c r="R39" s="2" t="s">
+        <v>294</v>
+      </c>
+      <c r="S39" s="2" t="s">
+        <v>295</v>
+      </c>
+      <c r="T39" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="U39" s="2"/>
+    </row>
+    <row r="40" spans="1:21" hidden="1" x14ac:dyDescent="0.2">
       <c r="A40" s="3" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="41" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:21" hidden="1" x14ac:dyDescent="0.2">
       <c r="A41" s="3" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="42" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:21" ht="51" x14ac:dyDescent="0.2">
       <c r="A42" s="3" t="s">
         <v>48</v>
       </c>
-      <c r="B42" s="2"/>
-      <c r="C42" s="2"/>
-      <c r="D42" s="2"/>
-      <c r="E42" s="2"/>
-      <c r="F42" s="2"/>
-      <c r="G42" s="2"/>
-      <c r="H42" s="2"/>
-      <c r="I42" s="2"/>
-      <c r="J42" s="2"/>
-      <c r="K42" s="2"/>
-      <c r="L42" s="2"/>
-      <c r="M42" s="2"/>
-      <c r="N42" s="2"/>
-    </row>
-    <row r="43" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
+      <c r="B42" s="2" t="s">
+        <v>296</v>
+      </c>
+      <c r="C42" s="2" t="s">
+        <v>296</v>
+      </c>
+      <c r="D42" s="2" t="s">
+        <v>296</v>
+      </c>
+      <c r="E42" s="2" t="s">
+        <v>296</v>
+      </c>
+      <c r="F42" s="2" t="s">
+        <v>297</v>
+      </c>
+      <c r="G42" s="2" t="s">
+        <v>296</v>
+      </c>
+      <c r="H42" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="I42" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="J42" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="K42" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="L42" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="M42" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="N42" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="O42" s="3" t="s">
+        <v>80</v>
+      </c>
+      <c r="P42" s="3" t="s">
+        <v>80</v>
+      </c>
+      <c r="Q42" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="R42" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="S42" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="T42" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="U42" s="2"/>
+    </row>
+    <row r="43" spans="1:21" hidden="1" x14ac:dyDescent="0.2">
       <c r="A43" s="3" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="44" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:21" ht="17" x14ac:dyDescent="0.2">
       <c r="A44" s="3" t="s">
         <v>50</v>
       </c>
-      <c r="B44" s="2"/>
-      <c r="C44" s="2"/>
-      <c r="D44" s="2"/>
-      <c r="E44" s="2"/>
-      <c r="F44" s="2"/>
-      <c r="G44" s="2"/>
-      <c r="H44" s="2"/>
-      <c r="I44" s="2"/>
-      <c r="J44" s="2"/>
-      <c r="K44" s="2"/>
-      <c r="L44" s="2"/>
-      <c r="M44" s="2"/>
-      <c r="N44" s="2"/>
-    </row>
-    <row r="45" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="B44" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="C44" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="D44" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="E44" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="F44" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="G44" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="H44" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="I44" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="J44" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="K44" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="L44" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="M44" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="N44" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="O44" s="3" t="s">
+        <v>80</v>
+      </c>
+      <c r="P44" s="3" t="s">
+        <v>80</v>
+      </c>
+      <c r="Q44" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="R44" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="S44" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="T44" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="U44" s="2"/>
+    </row>
+    <row r="45" spans="1:21" ht="68" x14ac:dyDescent="0.2">
       <c r="A45" s="3" t="s">
         <v>51</v>
       </c>
-      <c r="B45" s="2"/>
-      <c r="C45" s="2"/>
-      <c r="D45" s="2"/>
-      <c r="E45" s="2"/>
-      <c r="F45" s="2"/>
-      <c r="G45" s="2"/>
-      <c r="H45" s="2"/>
-      <c r="I45" s="2"/>
-      <c r="J45" s="2"/>
-      <c r="K45" s="2"/>
-      <c r="L45" s="2"/>
-      <c r="M45" s="2"/>
-      <c r="N45" s="2"/>
-    </row>
-    <row r="46" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="B45" s="2" t="s">
+        <v>298</v>
+      </c>
+      <c r="C45" s="2" t="s">
+        <v>304</v>
+      </c>
+      <c r="D45" s="2" t="s">
+        <v>299</v>
+      </c>
+      <c r="E45" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="F45" s="2" t="s">
+        <v>300</v>
+      </c>
+      <c r="G45" s="2" t="s">
+        <v>301</v>
+      </c>
+      <c r="H45" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="I45" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="J45" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="K45" s="2" t="s">
+        <v>303</v>
+      </c>
+      <c r="L45" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="M45" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="N45" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="O45" s="3" t="s">
+        <v>80</v>
+      </c>
+      <c r="P45" s="3" t="s">
+        <v>302</v>
+      </c>
+      <c r="Q45" s="2" t="s">
+        <v>307</v>
+      </c>
+      <c r="R45" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="S45" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="T45" s="2" t="s">
+        <v>306</v>
+      </c>
+      <c r="U45" s="2"/>
+    </row>
+    <row r="46" spans="1:21" ht="51" x14ac:dyDescent="0.2">
       <c r="A46" s="3" t="s">
         <v>52</v>
       </c>
-      <c r="B46" s="2"/>
-      <c r="C46" s="2"/>
-      <c r="D46" s="2"/>
-      <c r="E46" s="2"/>
-      <c r="F46" s="2"/>
-      <c r="G46" s="2"/>
-      <c r="H46" s="2"/>
-      <c r="I46" s="2"/>
-      <c r="J46" s="2"/>
-      <c r="K46" s="2"/>
-      <c r="L46" s="2"/>
-      <c r="M46" s="2"/>
-      <c r="N46" s="2"/>
-    </row>
-    <row r="47" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
+      <c r="B46" s="2" t="s">
+        <v>308</v>
+      </c>
+      <c r="C46" s="2" t="s">
+        <v>308</v>
+      </c>
+      <c r="D46" s="2" t="s">
+        <v>308</v>
+      </c>
+      <c r="E46" s="2" t="s">
+        <v>308</v>
+      </c>
+      <c r="F46" s="2" t="s">
+        <v>308</v>
+      </c>
+      <c r="G46" s="2" t="s">
+        <v>309</v>
+      </c>
+      <c r="H46" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="I46" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="J46" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="K46" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="L46" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="M46" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="N46" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="O46" s="3" t="s">
+        <v>80</v>
+      </c>
+      <c r="P46" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="Q46" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="R46" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="S46" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="T46" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="U46" s="2"/>
+    </row>
+    <row r="47" spans="1:21" hidden="1" x14ac:dyDescent="0.2">
       <c r="A47" s="3" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="48" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:21" hidden="1" x14ac:dyDescent="0.2">
       <c r="A48" s="3" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="49" spans="1:14" ht="17" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:21" ht="51" x14ac:dyDescent="0.2">
       <c r="A49" s="3" t="s">
         <v>55</v>
       </c>
-      <c r="B49" s="2"/>
-      <c r="C49" s="2"/>
-      <c r="D49" s="2"/>
-      <c r="E49" s="2"/>
-      <c r="F49" s="2"/>
-      <c r="G49" s="2"/>
-      <c r="H49" s="2"/>
-      <c r="I49" s="2"/>
+      <c r="B49" s="2" t="s">
+        <v>310</v>
+      </c>
+      <c r="C49" s="2" t="s">
+        <v>310</v>
+      </c>
+      <c r="D49" s="2" t="s">
+        <v>310</v>
+      </c>
+      <c r="E49" s="2" t="s">
+        <v>310</v>
+      </c>
+      <c r="F49" s="2" t="s">
+        <v>310</v>
+      </c>
+      <c r="G49" s="2" t="s">
+        <v>309</v>
+      </c>
+      <c r="H49" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="I49" s="2" t="s">
+        <v>80</v>
+      </c>
       <c r="J49" s="2" t="s">
-        <v>275</v>
-      </c>
-      <c r="K49" s="2"/>
-      <c r="L49" s="2"/>
-      <c r="M49" s="2"/>
-      <c r="N49" s="2"/>
-    </row>
-    <row r="50" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
+        <v>274</v>
+      </c>
+      <c r="K49" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="L49" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="M49" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="N49" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="O49" s="3" t="s">
+        <v>80</v>
+      </c>
+      <c r="P49" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="Q49" s="2" t="s">
+        <v>311</v>
+      </c>
+      <c r="R49" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="S49" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="T49" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="U49" s="2"/>
+    </row>
+    <row r="50" spans="1:21" hidden="1" x14ac:dyDescent="0.2">
       <c r="A50" s="3" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="51" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:21" hidden="1" x14ac:dyDescent="0.2">
       <c r="A51" s="3" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="52" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:21" x14ac:dyDescent="0.2">
       <c r="B52" s="2"/>
       <c r="C52" s="2"/>
       <c r="D52" s="2"/>
@@ -8894,8 +9632,14 @@
       <c r="L52" s="2"/>
       <c r="M52" s="2"/>
       <c r="N52" s="2"/>
-    </row>
-    <row r="53" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O52" s="3"/>
+      <c r="Q52" s="2"/>
+      <c r="R52" s="2"/>
+      <c r="S52" s="2"/>
+      <c r="T52" s="2"/>
+      <c r="U52" s="2"/>
+    </row>
+    <row r="53" spans="1:21" x14ac:dyDescent="0.2">
       <c r="B53" s="2"/>
       <c r="C53" s="2"/>
       <c r="D53" s="2"/>
@@ -8909,8 +9653,14 @@
       <c r="L53" s="2"/>
       <c r="M53" s="2"/>
       <c r="N53" s="2"/>
-    </row>
-    <row r="54" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O53" s="3"/>
+      <c r="Q53" s="2"/>
+      <c r="R53" s="2"/>
+      <c r="S53" s="2"/>
+      <c r="T53" s="2"/>
+      <c r="U53" s="2"/>
+    </row>
+    <row r="54" spans="1:21" x14ac:dyDescent="0.2">
       <c r="B54" s="2"/>
       <c r="C54" s="2"/>
       <c r="D54" s="2"/>
@@ -8924,6 +9674,39 @@
       <c r="L54" s="2"/>
       <c r="M54" s="2"/>
       <c r="N54" s="2"/>
+      <c r="Q54" s="2"/>
+      <c r="R54" s="2"/>
+      <c r="S54" s="2"/>
+      <c r="T54" s="2"/>
+      <c r="U54" s="2"/>
+    </row>
+    <row r="55" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="Q55" s="2"/>
+      <c r="R55" s="2"/>
+      <c r="S55" s="2"/>
+      <c r="T55" s="2"/>
+      <c r="U55" s="2"/>
+    </row>
+    <row r="56" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="Q56" s="2"/>
+      <c r="R56" s="2"/>
+      <c r="S56" s="2"/>
+      <c r="T56" s="2"/>
+      <c r="U56" s="2"/>
+    </row>
+    <row r="57" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="Q57" s="2"/>
+      <c r="R57" s="2"/>
+      <c r="S57" s="2"/>
+      <c r="T57" s="2"/>
+      <c r="U57" s="2"/>
+    </row>
+    <row r="58" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="Q58" s="2"/>
+      <c r="R58" s="2"/>
+      <c r="S58" s="2"/>
+      <c r="T58" s="2"/>
+      <c r="U58" s="2"/>
     </row>
   </sheetData>
   <autoFilter ref="A1:A51" xr:uid="{48541A15-86EE-DC49-B72C-33AAB33B8C19}">
@@ -8939,7 +9722,6 @@
         <filter val="Louisiana"/>
         <filter val="Mississippi"/>
         <filter val="North Carolina"/>
-        <filter val="North Dakota"/>
         <filter val="Oklahoma"/>
         <filter val="Pennsylvania"/>
         <filter val="South Dakota"/>

</xml_diff>

<commit_message>
Andrew | Added more proof of financial responsibility analysis.
</commit_message>
<xml_diff>
--- a/compliance/State Compliance Analysis.xlsx
+++ b/compliance/State Compliance Analysis.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/andrewhetzler/Documents/Documents - Andrew’s Money Maker/School/DISSERTATION/GitHub/dissertation/compliance/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DE55FF1A-96E6-564E-8B7F-A86E22A61D8A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5282DD08-44F2-E84E-BC20-F1D2A5F37F11}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="40960" windowHeight="24400" activeTab="1" xr2:uid="{FEE3D6CA-2CD0-2B4F-9478-6397B247951E}"/>
   </bookViews>
@@ -49,7 +49,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1896" uniqueCount="374">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2103" uniqueCount="395">
   <si>
     <t>STATE</t>
   </si>
@@ -1732,9 +1732,6 @@
     <t>Required (28-4011(A))</t>
   </si>
   <si>
-    <t>Required (28-4007(A))</t>
-  </si>
-  <si>
     <t>NOTE</t>
   </si>
   <si>
@@ -1916,6 +1913,102 @@
   </si>
   <si>
     <t>PENALTY STATEMENT</t>
+  </si>
+  <si>
+    <t>Required (33-34-5.1)(a))</t>
+  </si>
+  <si>
+    <t>REQUIRES DEPOSIT</t>
+  </si>
+  <si>
+    <t>Optional--required only for taxicabs (33-34-5.1)(a)(3)(C))</t>
+  </si>
+  <si>
+    <t>Required (321.20B(2)(a))</t>
+  </si>
+  <si>
+    <t>Required (321A.34(1)(a))</t>
+  </si>
+  <si>
+    <t>Required (40-3104(e))</t>
+  </si>
+  <si>
+    <t>Required (40-3104(f))</t>
+  </si>
+  <si>
+    <t>Required (304-39-117(2)(c))</t>
+  </si>
+  <si>
+    <t>Law requires either insurance or self-insurance, but gives no details</t>
+  </si>
+  <si>
+    <t>Required (32-898(A))</t>
+  </si>
+  <si>
+    <t>DESCRIPTION OR REFERNCE OF VEHICLE</t>
+  </si>
+  <si>
+    <t>Required unless person is not owner of vehicle(32-898(A))</t>
+  </si>
+  <si>
+    <t>No details on what is issued for a bond (32-903)</t>
+  </si>
+  <si>
+    <t>Required (32-1042(A))</t>
+  </si>
+  <si>
+    <t>Required (63-15-39)</t>
+  </si>
+  <si>
+    <t>Required  unless person is not owner of vehicle(63-15-39)</t>
+  </si>
+  <si>
+    <t>See description</t>
+  </si>
+  <si>
+    <r>
+      <t>NOTE</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> also support deposit (63-15-51(1))</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">- </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>no details on deposit certificate</t>
+    </r>
+  </si>
+  <si>
+    <t>Required (63-15-51(2)</t>
+  </si>
+  <si>
+    <t>Required (20-279.19)</t>
+  </si>
+  <si>
+    <t>Required (20-279.33(b))</t>
+  </si>
+  <si>
+    <t>Required (28-4007(B))</t>
   </si>
 </sst>
 </file>
@@ -1991,7 +2084,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -2006,6 +2099,9 @@
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -2347,7 +2443,7 @@
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="D10" sqref="D10"/>
+      <selection pane="topRight" activeCell="B49" sqref="B49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2372,7 +2468,7 @@
       </c>
       <c r="C1" s="1"/>
       <c r="D1" s="1" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="E1" s="1"/>
       <c r="F1" s="1"/>
@@ -2397,16 +2493,16 @@
       <c r="Y1" s="1"/>
       <c r="Z1" s="1"/>
     </row>
-    <row r="2" spans="1:26" ht="17" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:26" ht="17" hidden="1" x14ac:dyDescent="0.2">
       <c r="A2" s="3" t="s">
         <v>9</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
       <c r="C2" s="2"/>
       <c r="D2" s="2" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
       <c r="E2" s="2"/>
       <c r="F2" s="2"/>
@@ -2436,11 +2532,11 @@
         <v>11</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>368</v>
+        <v>367</v>
       </c>
       <c r="C4" s="2"/>
       <c r="D4" s="2" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
       <c r="E4" s="2"/>
       <c r="F4" s="2"/>
@@ -2460,7 +2556,7 @@
       <c r="T4" s="2"/>
       <c r="U4" s="2"/>
     </row>
-    <row r="5" spans="1:26" ht="17" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:26" ht="17" hidden="1" x14ac:dyDescent="0.2">
       <c r="A5" s="3" t="s">
         <v>12</v>
       </c>
@@ -2469,7 +2565,7 @@
       </c>
       <c r="C5" s="2"/>
       <c r="D5" s="2" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
       <c r="E5" s="2"/>
       <c r="F5" s="2"/>
@@ -2529,16 +2625,16 @@
         <v>15</v>
       </c>
     </row>
-    <row r="10" spans="1:26" ht="34" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:26" ht="34" hidden="1" x14ac:dyDescent="0.2">
       <c r="A10" s="3" t="s">
         <v>16</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
       <c r="C10" s="2"/>
       <c r="D10" s="2" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
       <c r="E10" s="2"/>
       <c r="F10" s="2"/>
@@ -2558,7 +2654,7 @@
       <c r="T10" s="2"/>
       <c r="U10" s="2"/>
     </row>
-    <row r="11" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:26" hidden="1" x14ac:dyDescent="0.2">
       <c r="A11" s="3" t="s">
         <v>17</v>
       </c>
@@ -2603,7 +2699,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="16" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:26" hidden="1" x14ac:dyDescent="0.2">
       <c r="A16" s="3" t="s">
         <v>22</v>
       </c>
@@ -2628,7 +2724,7 @@
       <c r="T16" s="2"/>
       <c r="U16" s="2"/>
     </row>
-    <row r="17" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:21" hidden="1" x14ac:dyDescent="0.2">
       <c r="A17" s="3" t="s">
         <v>23</v>
       </c>
@@ -2653,7 +2749,7 @@
       <c r="T17" s="2"/>
       <c r="U17" s="2"/>
     </row>
-    <row r="18" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:21" hidden="1" x14ac:dyDescent="0.2">
       <c r="A18" s="3" t="s">
         <v>24</v>
       </c>
@@ -2678,13 +2774,17 @@
       <c r="T18" s="2"/>
       <c r="U18" s="2"/>
     </row>
-    <row r="19" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:21" ht="34" hidden="1" x14ac:dyDescent="0.2">
       <c r="A19" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="B19" s="2"/>
+      <c r="B19" s="2" t="s">
+        <v>80</v>
+      </c>
       <c r="C19" s="2"/>
-      <c r="D19" s="2"/>
+      <c r="D19" s="2" t="s">
+        <v>385</v>
+      </c>
       <c r="E19" s="2"/>
       <c r="F19" s="2"/>
       <c r="G19" s="2"/>
@@ -2728,13 +2828,17 @@
         <v>30</v>
       </c>
     </row>
-    <row r="25" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:21" ht="34" x14ac:dyDescent="0.2">
       <c r="A25" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="B25" s="2"/>
+      <c r="B25" s="2" t="s">
+        <v>80</v>
+      </c>
       <c r="C25" s="2"/>
-      <c r="D25" s="2"/>
+      <c r="D25" s="6" t="s">
+        <v>390</v>
+      </c>
       <c r="E25" s="2"/>
       <c r="F25" s="2"/>
       <c r="G25" s="2"/>
@@ -2793,7 +2897,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="34" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:21" hidden="1" x14ac:dyDescent="0.2">
       <c r="A34" s="3" t="s">
         <v>40</v>
       </c>
@@ -3375,17 +3479,8 @@
   <autoFilter ref="A1:A51" xr:uid="{4E61F571-54A4-994C-A02B-889943573726}">
     <filterColumn colId="0">
       <filters>
-        <filter val="Alabama"/>
         <filter val="Arizona"/>
-        <filter val="Arkansas"/>
-        <filter val="Florida"/>
-        <filter val="Georgia"/>
-        <filter val="Iowa"/>
-        <filter val="Kansas"/>
-        <filter val="Kentucky"/>
-        <filter val="Louisiana"/>
         <filter val="Mississippi"/>
-        <filter val="North Carolina"/>
         <filter val="North Dakota"/>
         <filter val="Oklahoma"/>
         <filter val="Pennsylvania"/>
@@ -3408,7 +3503,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="S10" sqref="S10"/>
+      <selection pane="topRight" activeCell="H19" sqref="H19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3431,6 +3526,8 @@
     <col min="16" max="16" width="23.33203125" customWidth="1"/>
     <col min="17" max="17" width="29.5" customWidth="1"/>
     <col min="18" max="18" width="41" customWidth="1"/>
+    <col min="19" max="19" width="25.6640625" customWidth="1"/>
+    <col min="20" max="20" width="34.5" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:27" x14ac:dyDescent="0.2">
@@ -3462,34 +3559,38 @@
         <v>85</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="L1" s="1" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="M1" s="1" t="s">
+        <v>351</v>
+      </c>
+      <c r="N1" s="1" t="s">
         <v>352</v>
       </c>
-      <c r="N1" s="1" t="s">
+      <c r="O1" s="1" t="s">
         <v>353</v>
       </c>
-      <c r="O1" s="1" t="s">
-        <v>354</v>
-      </c>
       <c r="P1" s="1" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
       <c r="Q1" s="1" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
       <c r="R1" s="1" t="s">
-        <v>373</v>
-      </c>
-      <c r="S1" s="1"/>
-      <c r="T1" s="1"/>
+        <v>372</v>
+      </c>
+      <c r="S1" s="1" t="s">
+        <v>255</v>
+      </c>
+      <c r="T1" s="1" t="s">
+        <v>383</v>
+      </c>
       <c r="U1" s="1"/>
       <c r="V1" s="1"/>
       <c r="W1" s="1"/>
@@ -3533,7 +3634,7 @@
         <v>80</v>
       </c>
       <c r="L2" s="2" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
       <c r="M2" s="2" t="s">
         <v>80</v>
@@ -3553,8 +3654,12 @@
       <c r="R2" s="2" t="s">
         <v>80</v>
       </c>
-      <c r="S2" s="2"/>
-      <c r="T2" s="2"/>
+      <c r="S2" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="T2" s="2" t="s">
+        <v>80</v>
+      </c>
       <c r="U2" s="2"/>
       <c r="V2" s="2"/>
     </row>
@@ -3574,28 +3679,28 @@
         <v>80</v>
       </c>
       <c r="D4" s="2" t="s">
+        <v>343</v>
+      </c>
+      <c r="E4" s="2" t="s">
         <v>344</v>
       </c>
-      <c r="E4" s="2" t="s">
+      <c r="F4" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="G4" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="H4" s="2" t="s">
         <v>345</v>
       </c>
-      <c r="F4" s="2" t="s">
-        <v>80</v>
-      </c>
-      <c r="G4" s="2" t="s">
-        <v>80</v>
-      </c>
-      <c r="H4" s="2" t="s">
-        <v>346</v>
-      </c>
       <c r="I4" s="2" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="J4" s="2" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="K4" s="2" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="L4" s="2" t="s">
         <v>80</v>
@@ -3618,8 +3723,12 @@
       <c r="R4" s="2" t="s">
         <v>80</v>
       </c>
-      <c r="S4" s="2"/>
-      <c r="T4" s="2"/>
+      <c r="S4" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="T4" s="2" t="s">
+        <v>80</v>
+      </c>
       <c r="U4" s="2"/>
       <c r="V4" s="2"/>
     </row>
@@ -3628,58 +3737,62 @@
         <v>12</v>
       </c>
       <c r="B5" s="2" t="s">
+        <v>359</v>
+      </c>
+      <c r="C5" s="2" t="s">
         <v>360</v>
       </c>
-      <c r="C5" s="2" t="s">
+      <c r="D5" s="2" t="s">
+        <v>358</v>
+      </c>
+      <c r="E5" s="2" t="s">
         <v>361</v>
       </c>
-      <c r="D5" s="2" t="s">
-        <v>359</v>
-      </c>
-      <c r="E5" s="2" t="s">
-        <v>362</v>
-      </c>
       <c r="F5" s="2" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="G5" s="2" t="s">
+        <v>356</v>
+      </c>
+      <c r="H5" s="2" t="s">
         <v>357</v>
       </c>
-      <c r="H5" s="2" t="s">
-        <v>358</v>
-      </c>
       <c r="I5" s="2" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="J5" s="2" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
       <c r="K5" s="2" t="s">
         <v>80</v>
       </c>
       <c r="L5" s="2" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="M5" s="2" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="N5" s="2" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="O5" s="2" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="P5" s="2" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="Q5" s="2" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
       <c r="R5" s="2" t="s">
         <v>80</v>
       </c>
-      <c r="S5" s="2"/>
-      <c r="T5" s="2"/>
+      <c r="S5" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="T5" s="2" t="s">
+        <v>80</v>
+      </c>
       <c r="U5" s="2"/>
       <c r="V5" s="2"/>
     </row>
@@ -3729,22 +3842,22 @@
         <v>16</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
       <c r="E10" s="2" t="s">
         <v>80</v>
       </c>
       <c r="F10" s="2" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
       <c r="G10" s="2" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
       <c r="H10" s="2" t="s">
         <v>80</v>
@@ -3779,34 +3892,76 @@
       <c r="R10" s="2" t="s">
         <v>80</v>
       </c>
-      <c r="S10" s="2"/>
-      <c r="T10" s="2"/>
+      <c r="S10" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="T10" s="2" t="s">
+        <v>80</v>
+      </c>
       <c r="U10" s="2"/>
       <c r="V10" s="2"/>
     </row>
-    <row r="11" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:27" ht="17" x14ac:dyDescent="0.2">
       <c r="A11" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="B11" s="2"/>
-      <c r="C11" s="2"/>
-      <c r="D11" s="2"/>
-      <c r="E11" s="2"/>
-      <c r="F11" s="2"/>
-      <c r="G11" s="2"/>
-      <c r="H11" s="2"/>
-      <c r="I11" s="2"/>
-      <c r="J11" s="2"/>
-      <c r="K11" s="2"/>
-      <c r="L11" s="2"/>
-      <c r="M11" s="2"/>
-      <c r="N11" s="2"/>
-      <c r="O11" s="2"/>
-      <c r="P11" s="2"/>
-      <c r="Q11" s="2"/>
-      <c r="R11" s="2"/>
-      <c r="S11" s="2"/>
-      <c r="T11" s="2"/>
+      <c r="B11" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="C11" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="D11" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="E11" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="F11" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="G11" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="H11" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="I11" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="J11" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="K11" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="L11" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="M11" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="N11" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="O11" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="P11" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="Q11" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="R11" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="S11" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="T11" s="2" t="s">
+        <v>80</v>
+      </c>
       <c r="U11" s="2"/>
       <c r="V11" s="2"/>
     </row>
@@ -3830,107 +3985,259 @@
         <v>20</v>
       </c>
     </row>
-    <row r="16" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:27" ht="17" x14ac:dyDescent="0.2">
       <c r="A16" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="B16" s="2"/>
-      <c r="C16" s="2"/>
-      <c r="D16" s="2"/>
-      <c r="E16" s="2"/>
-      <c r="F16" s="2"/>
-      <c r="G16" s="2"/>
-      <c r="H16" s="2"/>
-      <c r="I16" s="2"/>
-      <c r="J16" s="2"/>
-      <c r="K16" s="2"/>
-      <c r="L16" s="2"/>
-      <c r="M16" s="2"/>
-      <c r="N16" s="2"/>
-      <c r="O16" s="2"/>
-      <c r="P16" s="2"/>
-      <c r="Q16" s="2"/>
-      <c r="R16" s="2"/>
-      <c r="S16" s="2"/>
-      <c r="T16" s="2"/>
+      <c r="B16" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="C16" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="D16" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="E16" s="2" t="s">
+        <v>376</v>
+      </c>
+      <c r="F16" s="2" t="s">
+        <v>376</v>
+      </c>
+      <c r="G16" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="H16" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="I16" s="2" t="s">
+        <v>376</v>
+      </c>
+      <c r="J16" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="K16" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="L16" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="M16" s="2" t="s">
+        <v>376</v>
+      </c>
+      <c r="N16" s="2" t="s">
+        <v>376</v>
+      </c>
+      <c r="O16" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="P16" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="Q16" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="R16" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="S16" s="2" t="s">
+        <v>376</v>
+      </c>
+      <c r="T16" s="2" t="s">
+        <v>80</v>
+      </c>
       <c r="U16" s="2"/>
       <c r="V16" s="2"/>
     </row>
-    <row r="17" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:22" ht="17" x14ac:dyDescent="0.2">
       <c r="A17" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="B17" s="2"/>
-      <c r="C17" s="2"/>
-      <c r="D17" s="2"/>
-      <c r="E17" s="2"/>
-      <c r="F17" s="2"/>
-      <c r="G17" s="2"/>
-      <c r="H17" s="2"/>
-      <c r="I17" s="2"/>
-      <c r="J17" s="2"/>
-      <c r="K17" s="2"/>
-      <c r="L17" s="2"/>
-      <c r="M17" s="2"/>
-      <c r="N17" s="2"/>
-      <c r="O17" s="2"/>
-      <c r="P17" s="2"/>
-      <c r="Q17" s="2"/>
-      <c r="R17" s="2"/>
-      <c r="S17" s="2"/>
-      <c r="T17" s="2"/>
+      <c r="B17" s="2" t="s">
+        <v>378</v>
+      </c>
+      <c r="C17" s="2" t="s">
+        <v>378</v>
+      </c>
+      <c r="D17" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="E17" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="F17" s="2" t="s">
+        <v>378</v>
+      </c>
+      <c r="G17" s="2" t="s">
+        <v>378</v>
+      </c>
+      <c r="H17" s="2" t="s">
+        <v>378</v>
+      </c>
+      <c r="I17" s="2" t="s">
+        <v>378</v>
+      </c>
+      <c r="J17" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="K17" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="L17" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="M17" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="N17" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="O17" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="P17" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="Q17" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="R17" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="S17" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="T17" s="2" t="s">
+        <v>80</v>
+      </c>
       <c r="U17" s="2"/>
       <c r="V17" s="2"/>
     </row>
-    <row r="18" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:22" ht="17" x14ac:dyDescent="0.2">
       <c r="A18" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="B18" s="2"/>
-      <c r="C18" s="2"/>
-      <c r="D18" s="2"/>
-      <c r="E18" s="2"/>
-      <c r="F18" s="2"/>
-      <c r="G18" s="2"/>
-      <c r="H18" s="2"/>
-      <c r="I18" s="2"/>
-      <c r="J18" s="2"/>
-      <c r="K18" s="2"/>
-      <c r="L18" s="2"/>
-      <c r="M18" s="2"/>
-      <c r="N18" s="2"/>
-      <c r="O18" s="2"/>
-      <c r="P18" s="2"/>
-      <c r="Q18" s="2"/>
-      <c r="R18" s="2"/>
-      <c r="S18" s="2"/>
-      <c r="T18" s="2"/>
+      <c r="B18" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="C18" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="D18" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="E18" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="F18" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="G18" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="H18" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="I18" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="J18" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="K18" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="L18" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="M18" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="N18" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="O18" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="P18" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="Q18" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="R18" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="S18" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="T18" s="2" t="s">
+        <v>80</v>
+      </c>
       <c r="U18" s="2"/>
       <c r="V18" s="2"/>
     </row>
-    <row r="19" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:22" ht="34" x14ac:dyDescent="0.2">
       <c r="A19" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="B19" s="2"/>
-      <c r="C19" s="2"/>
-      <c r="D19" s="2"/>
-      <c r="E19" s="2"/>
-      <c r="F19" s="2"/>
-      <c r="G19" s="2"/>
-      <c r="H19" s="2"/>
-      <c r="I19" s="2"/>
-      <c r="J19" s="2"/>
-      <c r="K19" s="2"/>
-      <c r="L19" s="2"/>
-      <c r="M19" s="2"/>
-      <c r="N19" s="2"/>
-      <c r="O19" s="2"/>
-      <c r="P19" s="2"/>
-      <c r="Q19" s="2"/>
-      <c r="R19" s="2"/>
-      <c r="S19" s="2"/>
-      <c r="T19" s="2"/>
+      <c r="B19" s="2" t="s">
+        <v>389</v>
+      </c>
+      <c r="C19" s="2" t="s">
+        <v>389</v>
+      </c>
+      <c r="D19" s="2" t="s">
+        <v>389</v>
+      </c>
+      <c r="E19" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="F19" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="G19" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="H19" s="2" t="s">
+        <v>382</v>
+      </c>
+      <c r="I19" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="J19" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="K19" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="L19" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="M19" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="N19" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="O19" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="P19" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="Q19" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="R19" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="S19" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="T19" s="2" t="s">
+        <v>384</v>
+      </c>
       <c r="U19" s="2"/>
       <c r="V19" s="2"/>
     </row>
@@ -3959,29 +4266,67 @@
         <v>30</v>
       </c>
     </row>
-    <row r="25" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:22" ht="34" x14ac:dyDescent="0.2">
       <c r="A25" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="B25" s="2"/>
-      <c r="C25" s="2"/>
-      <c r="D25" s="2"/>
-      <c r="E25" s="2"/>
-      <c r="F25" s="2"/>
-      <c r="G25" s="2"/>
-      <c r="H25" s="2"/>
-      <c r="I25" s="2"/>
-      <c r="J25" s="2"/>
-      <c r="K25" s="2"/>
-      <c r="L25" s="2"/>
-      <c r="M25" s="2"/>
-      <c r="N25" s="2"/>
-      <c r="O25" s="2"/>
-      <c r="P25" s="2"/>
-      <c r="Q25" s="2"/>
-      <c r="R25" s="2"/>
-      <c r="S25" s="2"/>
-      <c r="T25" s="2"/>
+      <c r="B25" s="2" t="s">
+        <v>389</v>
+      </c>
+      <c r="C25" s="2" t="s">
+        <v>389</v>
+      </c>
+      <c r="D25" s="2" t="s">
+        <v>389</v>
+      </c>
+      <c r="E25" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="F25" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="G25" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="H25" s="2" t="s">
+        <v>387</v>
+      </c>
+      <c r="I25" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="J25" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="K25" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="L25" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="M25" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="N25" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="O25" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="P25" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="Q25" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="R25" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="S25" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="T25" s="2" t="s">
+        <v>388</v>
+      </c>
       <c r="U25" s="2"/>
       <c r="V25" s="2"/>
     </row>
@@ -4025,29 +4370,67 @@
         <v>39</v>
       </c>
     </row>
-    <row r="34" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:22" ht="17" x14ac:dyDescent="0.2">
       <c r="A34" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="B34" s="2"/>
-      <c r="C34" s="2"/>
-      <c r="D34" s="2"/>
-      <c r="E34" s="2"/>
-      <c r="F34" s="2"/>
-      <c r="G34" s="2"/>
-      <c r="H34" s="2"/>
-      <c r="I34" s="2"/>
-      <c r="J34" s="2"/>
-      <c r="K34" s="2"/>
-      <c r="L34" s="2"/>
-      <c r="M34" s="2"/>
-      <c r="N34" s="2"/>
-      <c r="O34" s="2"/>
-      <c r="P34" s="2"/>
-      <c r="Q34" s="2"/>
-      <c r="R34" s="2"/>
-      <c r="S34" s="2"/>
-      <c r="T34" s="2"/>
+      <c r="B34" s="2" t="s">
+        <v>389</v>
+      </c>
+      <c r="C34" s="2" t="s">
+        <v>389</v>
+      </c>
+      <c r="D34" s="2" t="s">
+        <v>389</v>
+      </c>
+      <c r="E34" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="F34" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="G34" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="H34" s="2" t="s">
+        <v>392</v>
+      </c>
+      <c r="I34" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="J34" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="K34" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="L34" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="M34" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="N34" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="O34" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="P34" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="Q34" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="R34" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="S34" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="T34" s="2" t="s">
+        <v>392</v>
+      </c>
       <c r="U34" s="2"/>
       <c r="V34" s="2"/>
     </row>
@@ -4662,8 +5045,8 @@
   <dimension ref="A1:Z65"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="E5" sqref="E5"/>
+      <pane xSplit="1" topLeftCell="D1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="I18" sqref="I18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -4782,31 +5165,31 @@
         <v>11</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="F4" s="2" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="G4" s="2" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="H4" s="2" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="I4" s="2" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="J4" s="2" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="K4" s="2"/>
       <c r="L4" s="2"/>
@@ -4820,19 +5203,37 @@
       <c r="T4" s="2"/>
       <c r="U4" s="2"/>
     </row>
-    <row r="5" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:26" ht="17" hidden="1" x14ac:dyDescent="0.2">
       <c r="A5" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="B5" s="2"/>
-      <c r="C5" s="2"/>
-      <c r="D5" s="2"/>
-      <c r="E5" s="2"/>
-      <c r="F5" s="2"/>
-      <c r="G5" s="2"/>
-      <c r="H5" s="2"/>
-      <c r="I5" s="2"/>
-      <c r="J5" s="2"/>
+      <c r="B5" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="E5" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="F5" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="G5" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="H5" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="I5" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="J5" s="2" t="s">
+        <v>80</v>
+      </c>
       <c r="K5" s="2"/>
       <c r="L5" s="2"/>
       <c r="M5" s="2"/>
@@ -4885,19 +5286,37 @@
         <v>15</v>
       </c>
     </row>
-    <row r="10" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:26" ht="17" hidden="1" x14ac:dyDescent="0.2">
       <c r="A10" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="B10" s="2"/>
-      <c r="C10" s="2"/>
-      <c r="D10" s="2"/>
-      <c r="E10" s="2"/>
-      <c r="F10" s="2"/>
-      <c r="G10" s="2"/>
-      <c r="H10" s="2"/>
-      <c r="I10" s="2"/>
-      <c r="J10" s="2"/>
+      <c r="B10" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="D10" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="E10" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="F10" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="G10" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="H10" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="I10" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="J10" s="2" t="s">
+        <v>80</v>
+      </c>
       <c r="K10" s="2"/>
       <c r="L10" s="2"/>
       <c r="M10" s="2"/>
@@ -4910,19 +5329,37 @@
       <c r="T10" s="2"/>
       <c r="U10" s="2"/>
     </row>
-    <row r="11" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:26" ht="17" hidden="1" x14ac:dyDescent="0.2">
       <c r="A11" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="B11" s="2"/>
-      <c r="C11" s="2"/>
-      <c r="D11" s="2"/>
-      <c r="E11" s="2"/>
-      <c r="F11" s="2"/>
-      <c r="G11" s="2"/>
-      <c r="H11" s="2"/>
-      <c r="I11" s="2"/>
-      <c r="J11" s="2"/>
+      <c r="B11" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="C11" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="D11" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="E11" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="F11" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="G11" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="H11" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="I11" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="J11" s="2" t="s">
+        <v>80</v>
+      </c>
       <c r="K11" s="2"/>
       <c r="L11" s="2"/>
       <c r="M11" s="2"/>
@@ -4955,7 +5392,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="16" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:26" hidden="1" x14ac:dyDescent="0.2">
       <c r="A16" s="3" t="s">
         <v>22</v>
       </c>
@@ -4980,7 +5417,7 @@
       <c r="T16" s="2"/>
       <c r="U16" s="2"/>
     </row>
-    <row r="17" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:21" hidden="1" x14ac:dyDescent="0.2">
       <c r="A17" s="3" t="s">
         <v>23</v>
       </c>
@@ -5005,7 +5442,7 @@
       <c r="T17" s="2"/>
       <c r="U17" s="2"/>
     </row>
-    <row r="18" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:21" ht="17" x14ac:dyDescent="0.2">
       <c r="A18" s="3" t="s">
         <v>24</v>
       </c>
@@ -5016,7 +5453,9 @@
       <c r="F18" s="2"/>
       <c r="G18" s="2"/>
       <c r="H18" s="2"/>
-      <c r="I18" s="2"/>
+      <c r="I18" s="2" t="s">
+        <v>380</v>
+      </c>
       <c r="J18" s="2"/>
       <c r="K18" s="2"/>
       <c r="L18" s="2"/>
@@ -5030,7 +5469,7 @@
       <c r="T18" s="2"/>
       <c r="U18" s="2"/>
     </row>
-    <row r="19" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:21" hidden="1" x14ac:dyDescent="0.2">
       <c r="A19" s="3" t="s">
         <v>25</v>
       </c>
@@ -5080,7 +5519,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="25" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:21" hidden="1" x14ac:dyDescent="0.2">
       <c r="A25" s="3" t="s">
         <v>31</v>
       </c>
@@ -5145,7 +5584,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="34" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:21" hidden="1" x14ac:dyDescent="0.2">
       <c r="A34" s="3" t="s">
         <v>40</v>
       </c>
@@ -5728,15 +6167,7 @@
     <filterColumn colId="0">
       <filters>
         <filter val="Alabama"/>
-        <filter val="Arkansas"/>
-        <filter val="Florida"/>
-        <filter val="Georgia"/>
-        <filter val="Iowa"/>
-        <filter val="Kansas"/>
         <filter val="Kentucky"/>
-        <filter val="Louisiana"/>
-        <filter val="Mississippi"/>
-        <filter val="North Carolina"/>
         <filter val="North Dakota"/>
         <filter val="Oklahoma"/>
         <filter val="Pennsylvania"/>
@@ -5755,11 +6186,11 @@
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0D0B7835-E2B6-374A-9F51-E6E6BCA6388F}">
   <sheetPr filterMode="1"/>
-  <dimension ref="A1:AA65"/>
+  <dimension ref="A1:AB65"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="B10" sqref="B10"/>
+      <selection pane="topRight" activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -5767,16 +6198,16 @@
     <col min="1" max="1" width="14.5" customWidth="1"/>
     <col min="2" max="2" width="26.5" customWidth="1"/>
     <col min="3" max="3" width="21" customWidth="1"/>
-    <col min="4" max="4" width="21.83203125" customWidth="1"/>
-    <col min="5" max="5" width="37.5" customWidth="1"/>
-    <col min="6" max="6" width="21.83203125" customWidth="1"/>
-    <col min="7" max="7" width="21" customWidth="1"/>
-    <col min="8" max="8" width="21.1640625" customWidth="1"/>
-    <col min="9" max="9" width="24.6640625" customWidth="1"/>
-    <col min="10" max="10" width="33.1640625" customWidth="1"/>
+    <col min="4" max="5" width="21.83203125" customWidth="1"/>
+    <col min="6" max="6" width="37.5" customWidth="1"/>
+    <col min="7" max="7" width="21.83203125" customWidth="1"/>
+    <col min="8" max="8" width="21" customWidth="1"/>
+    <col min="9" max="9" width="21.1640625" customWidth="1"/>
+    <col min="10" max="10" width="24.6640625" customWidth="1"/>
+    <col min="11" max="11" width="33.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -5786,11 +6217,13 @@
       <c r="C1" s="1" t="s">
         <v>338</v>
       </c>
-      <c r="D1" s="1"/>
-      <c r="E1" s="1" t="s">
-        <v>341</v>
-      </c>
-      <c r="F1" s="1"/>
+      <c r="D1" s="1" t="s">
+        <v>374</v>
+      </c>
+      <c r="E1" s="1"/>
+      <c r="F1" s="1" t="s">
+        <v>340</v>
+      </c>
       <c r="G1" s="1"/>
       <c r="H1" s="1"/>
       <c r="I1" s="1"/>
@@ -5812,22 +6245,25 @@
       <c r="Y1" s="1"/>
       <c r="Z1" s="1"/>
       <c r="AA1" s="1"/>
-    </row>
-    <row r="2" spans="1:27" ht="17" x14ac:dyDescent="0.2">
+      <c r="AB1" s="1"/>
+    </row>
+    <row r="2" spans="1:28" ht="17" hidden="1" x14ac:dyDescent="0.2">
       <c r="A2" s="3" t="s">
         <v>9</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
       <c r="C2" s="2" t="s">
         <v>80</v>
       </c>
-      <c r="D2" s="2"/>
-      <c r="E2" s="2" t="s">
-        <v>342</v>
-      </c>
-      <c r="F2" s="2"/>
+      <c r="D2" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="E2" s="2"/>
+      <c r="F2" s="2" t="s">
+        <v>341</v>
+      </c>
       <c r="G2" s="2"/>
       <c r="H2" s="2"/>
       <c r="I2" s="2"/>
@@ -5844,27 +6280,30 @@
       <c r="T2" s="2"/>
       <c r="U2" s="2"/>
       <c r="V2" s="2"/>
-    </row>
-    <row r="3" spans="1:27" hidden="1" x14ac:dyDescent="0.2">
+      <c r="W2" s="2"/>
+    </row>
+    <row r="3" spans="1:28" hidden="1" x14ac:dyDescent="0.2">
       <c r="A3" s="3" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="4" spans="1:27" ht="17" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:28" ht="17" x14ac:dyDescent="0.2">
       <c r="A4" s="3" t="s">
         <v>11</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>340</v>
+        <v>394</v>
       </c>
       <c r="C4" s="2" t="s">
         <v>339</v>
       </c>
-      <c r="D4" s="2"/>
-      <c r="E4" s="2" t="s">
-        <v>342</v>
-      </c>
-      <c r="F4" s="2"/>
+      <c r="D4" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="E4" s="2"/>
+      <c r="F4" s="2" t="s">
+        <v>341</v>
+      </c>
       <c r="G4" s="2"/>
       <c r="H4" s="2"/>
       <c r="I4" s="2"/>
@@ -5881,22 +6320,25 @@
       <c r="T4" s="2"/>
       <c r="U4" s="2"/>
       <c r="V4" s="2"/>
-    </row>
-    <row r="5" spans="1:27" ht="17" x14ac:dyDescent="0.2">
+      <c r="W4" s="2"/>
+    </row>
+    <row r="5" spans="1:28" ht="17" hidden="1" x14ac:dyDescent="0.2">
       <c r="A5" s="3" t="s">
         <v>12</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
       <c r="C5" s="2" t="s">
         <v>80</v>
       </c>
-      <c r="D5" s="2"/>
-      <c r="E5" s="2" t="s">
-        <v>342</v>
-      </c>
-      <c r="F5" s="2"/>
+      <c r="D5" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="E5" s="2"/>
+      <c r="F5" s="2" t="s">
+        <v>341</v>
+      </c>
       <c r="G5" s="2"/>
       <c r="H5" s="2"/>
       <c r="I5" s="2"/>
@@ -5913,8 +6355,9 @@
       <c r="T5" s="2"/>
       <c r="U5" s="2"/>
       <c r="V5" s="2"/>
-    </row>
-    <row r="6" spans="1:27" hidden="1" x14ac:dyDescent="0.2">
+      <c r="W5" s="2"/>
+    </row>
+    <row r="6" spans="1:28" hidden="1" x14ac:dyDescent="0.2">
       <c r="A6" s="3" t="s">
         <v>13</v>
       </c>
@@ -5939,37 +6382,40 @@
       <c r="T6" s="2"/>
       <c r="U6" s="2"/>
       <c r="V6" s="2"/>
-    </row>
-    <row r="7" spans="1:27" hidden="1" x14ac:dyDescent="0.2">
+      <c r="W6" s="2"/>
+    </row>
+    <row r="7" spans="1:28" hidden="1" x14ac:dyDescent="0.2">
       <c r="A7" s="3" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="8" spans="1:27" hidden="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:28" hidden="1" x14ac:dyDescent="0.2">
       <c r="A8" s="3" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="9" spans="1:27" hidden="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:28" hidden="1" x14ac:dyDescent="0.2">
       <c r="A9" s="3" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="10" spans="1:27" ht="17" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:28" ht="17" hidden="1" x14ac:dyDescent="0.2">
       <c r="A10" s="3" t="s">
         <v>16</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
       <c r="C10" s="2" t="s">
         <v>80</v>
       </c>
-      <c r="D10" s="2"/>
-      <c r="E10" s="2" t="s">
-        <v>342</v>
-      </c>
-      <c r="F10" s="2"/>
+      <c r="D10" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="E10" s="2"/>
+      <c r="F10" s="2" t="s">
+        <v>341</v>
+      </c>
       <c r="G10" s="2"/>
       <c r="H10" s="2"/>
       <c r="I10" s="2"/>
@@ -5986,16 +6432,23 @@
       <c r="T10" s="2"/>
       <c r="U10" s="2"/>
       <c r="V10" s="2"/>
-    </row>
-    <row r="11" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="W10" s="2"/>
+    </row>
+    <row r="11" spans="1:28" ht="51" x14ac:dyDescent="0.2">
       <c r="A11" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="B11" s="2"/>
+      <c r="B11" s="2" t="s">
+        <v>373</v>
+      </c>
       <c r="C11" s="2"/>
-      <c r="D11" s="2"/>
+      <c r="D11" s="2" t="s">
+        <v>375</v>
+      </c>
       <c r="E11" s="2"/>
-      <c r="F11" s="2"/>
+      <c r="F11" s="2" t="s">
+        <v>341</v>
+      </c>
       <c r="G11" s="2"/>
       <c r="H11" s="2"/>
       <c r="I11" s="2"/>
@@ -6012,36 +6465,45 @@
       <c r="T11" s="2"/>
       <c r="U11" s="2"/>
       <c r="V11" s="2"/>
-    </row>
-    <row r="12" spans="1:27" hidden="1" x14ac:dyDescent="0.2">
+      <c r="W11" s="2"/>
+    </row>
+    <row r="12" spans="1:28" hidden="1" x14ac:dyDescent="0.2">
       <c r="A12" s="3" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="13" spans="1:27" hidden="1" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:28" hidden="1" x14ac:dyDescent="0.2">
       <c r="A13" s="3" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="14" spans="1:27" hidden="1" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:28" hidden="1" x14ac:dyDescent="0.2">
       <c r="A14" s="3" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="15" spans="1:27" hidden="1" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:28" hidden="1" x14ac:dyDescent="0.2">
       <c r="A15" s="3" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="16" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:28" ht="17" x14ac:dyDescent="0.2">
       <c r="A16" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="B16" s="2"/>
-      <c r="C16" s="2"/>
-      <c r="D16" s="2"/>
+      <c r="B16" s="2" t="s">
+        <v>377</v>
+      </c>
+      <c r="C16" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="D16" s="2" t="s">
+        <v>80</v>
+      </c>
       <c r="E16" s="2"/>
-      <c r="F16" s="2"/>
+      <c r="F16" s="2" t="s">
+        <v>341</v>
+      </c>
       <c r="G16" s="2"/>
       <c r="H16" s="2"/>
       <c r="I16" s="2"/>
@@ -6058,16 +6520,25 @@
       <c r="T16" s="2"/>
       <c r="U16" s="2"/>
       <c r="V16" s="2"/>
-    </row>
-    <row r="17" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="W16" s="2"/>
+    </row>
+    <row r="17" spans="1:23" ht="17" x14ac:dyDescent="0.2">
       <c r="A17" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="B17" s="2"/>
-      <c r="C17" s="2"/>
-      <c r="D17" s="2"/>
+      <c r="B17" s="2" t="s">
+        <v>379</v>
+      </c>
+      <c r="C17" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="D17" s="2" t="s">
+        <v>80</v>
+      </c>
       <c r="E17" s="2"/>
-      <c r="F17" s="2"/>
+      <c r="F17" s="2" t="s">
+        <v>341</v>
+      </c>
       <c r="G17" s="2"/>
       <c r="H17" s="2"/>
       <c r="I17" s="2"/>
@@ -6084,16 +6555,25 @@
       <c r="T17" s="2"/>
       <c r="U17" s="2"/>
       <c r="V17" s="2"/>
-    </row>
-    <row r="18" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="W17" s="2"/>
+    </row>
+    <row r="18" spans="1:23" ht="34" x14ac:dyDescent="0.2">
       <c r="A18" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="B18" s="2"/>
-      <c r="C18" s="2"/>
-      <c r="D18" s="2"/>
+      <c r="B18" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="C18" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="D18" s="2" t="s">
+        <v>80</v>
+      </c>
       <c r="E18" s="2"/>
-      <c r="F18" s="2"/>
+      <c r="F18" s="2" t="s">
+        <v>381</v>
+      </c>
       <c r="G18" s="2"/>
       <c r="H18" s="2"/>
       <c r="I18" s="2"/>
@@ -6110,16 +6590,25 @@
       <c r="T18" s="2"/>
       <c r="U18" s="2"/>
       <c r="V18" s="2"/>
-    </row>
-    <row r="19" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="W18" s="2"/>
+    </row>
+    <row r="19" spans="1:23" ht="17" hidden="1" x14ac:dyDescent="0.2">
       <c r="A19" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="B19" s="2"/>
-      <c r="C19" s="2"/>
-      <c r="D19" s="2"/>
+      <c r="B19" s="2" t="s">
+        <v>386</v>
+      </c>
+      <c r="C19" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="D19" s="2" t="s">
+        <v>80</v>
+      </c>
       <c r="E19" s="2"/>
-      <c r="F19" s="2"/>
+      <c r="F19" s="2" t="s">
+        <v>341</v>
+      </c>
       <c r="G19" s="2"/>
       <c r="H19" s="2"/>
       <c r="I19" s="2"/>
@@ -6136,41 +6625,50 @@
       <c r="T19" s="2"/>
       <c r="U19" s="2"/>
       <c r="V19" s="2"/>
-    </row>
-    <row r="20" spans="1:22" hidden="1" x14ac:dyDescent="0.2">
+      <c r="W19" s="2"/>
+    </row>
+    <row r="20" spans="1:23" hidden="1" x14ac:dyDescent="0.2">
       <c r="A20" s="3" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="21" spans="1:22" hidden="1" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:23" hidden="1" x14ac:dyDescent="0.2">
       <c r="A21" s="3" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="22" spans="1:22" hidden="1" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:23" hidden="1" x14ac:dyDescent="0.2">
       <c r="A22" s="3" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="23" spans="1:22" hidden="1" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:23" hidden="1" x14ac:dyDescent="0.2">
       <c r="A23" s="3" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="24" spans="1:22" hidden="1" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:23" hidden="1" x14ac:dyDescent="0.2">
       <c r="A24" s="3" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="25" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:23" ht="17" x14ac:dyDescent="0.2">
       <c r="A25" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="B25" s="2"/>
-      <c r="C25" s="2"/>
-      <c r="D25" s="2"/>
+      <c r="B25" s="2" t="s">
+        <v>391</v>
+      </c>
+      <c r="C25" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="D25" s="2" t="s">
+        <v>80</v>
+      </c>
       <c r="E25" s="2"/>
-      <c r="F25" s="2"/>
+      <c r="F25" s="2" t="s">
+        <v>341</v>
+      </c>
       <c r="G25" s="2"/>
       <c r="H25" s="2"/>
       <c r="I25" s="2"/>
@@ -6187,56 +6685,65 @@
       <c r="T25" s="2"/>
       <c r="U25" s="2"/>
       <c r="V25" s="2"/>
-    </row>
-    <row r="26" spans="1:22" hidden="1" x14ac:dyDescent="0.2">
+      <c r="W25" s="2"/>
+    </row>
+    <row r="26" spans="1:23" hidden="1" x14ac:dyDescent="0.2">
       <c r="A26" s="3" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="27" spans="1:22" hidden="1" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:23" hidden="1" x14ac:dyDescent="0.2">
       <c r="A27" s="3" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="28" spans="1:22" hidden="1" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:23" hidden="1" x14ac:dyDescent="0.2">
       <c r="A28" s="3" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="29" spans="1:22" hidden="1" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:23" hidden="1" x14ac:dyDescent="0.2">
       <c r="A29" s="3" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="30" spans="1:22" hidden="1" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:23" hidden="1" x14ac:dyDescent="0.2">
       <c r="A30" s="3" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="31" spans="1:22" hidden="1" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:23" hidden="1" x14ac:dyDescent="0.2">
       <c r="A31" s="3" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="32" spans="1:22" hidden="1" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:23" hidden="1" x14ac:dyDescent="0.2">
       <c r="A32" s="3" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="33" spans="1:22" hidden="1" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:23" hidden="1" x14ac:dyDescent="0.2">
       <c r="A33" s="3" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="34" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:23" ht="17" hidden="1" x14ac:dyDescent="0.2">
       <c r="A34" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="B34" s="2"/>
-      <c r="C34" s="2"/>
-      <c r="D34" s="2"/>
+      <c r="B34" s="2" t="s">
+        <v>393</v>
+      </c>
+      <c r="C34" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="D34" s="2" t="s">
+        <v>80</v>
+      </c>
       <c r="E34" s="2"/>
-      <c r="F34" s="2"/>
+      <c r="F34" s="2" t="s">
+        <v>341</v>
+      </c>
       <c r="G34" s="2"/>
       <c r="H34" s="2"/>
       <c r="I34" s="2"/>
@@ -6253,8 +6760,9 @@
       <c r="T34" s="2"/>
       <c r="U34" s="2"/>
       <c r="V34" s="2"/>
-    </row>
-    <row r="35" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="W34" s="2"/>
+    </row>
+    <row r="35" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A35" s="3" t="s">
         <v>41</v>
       </c>
@@ -6279,13 +6787,14 @@
       <c r="T35" s="2"/>
       <c r="U35" s="2"/>
       <c r="V35" s="2"/>
-    </row>
-    <row r="36" spans="1:22" hidden="1" x14ac:dyDescent="0.2">
+      <c r="W35" s="2"/>
+    </row>
+    <row r="36" spans="1:23" hidden="1" x14ac:dyDescent="0.2">
       <c r="A36" s="3" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="37" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A37" s="3" t="s">
         <v>43</v>
       </c>
@@ -6310,13 +6819,14 @@
       <c r="T37" s="2"/>
       <c r="U37" s="2"/>
       <c r="V37" s="2"/>
-    </row>
-    <row r="38" spans="1:22" hidden="1" x14ac:dyDescent="0.2">
+      <c r="W37" s="2"/>
+    </row>
+    <row r="38" spans="1:23" hidden="1" x14ac:dyDescent="0.2">
       <c r="A38" s="3" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="39" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A39" s="3" t="s">
         <v>45</v>
       </c>
@@ -6341,18 +6851,19 @@
       <c r="T39" s="2"/>
       <c r="U39" s="2"/>
       <c r="V39" s="2"/>
-    </row>
-    <row r="40" spans="1:22" hidden="1" x14ac:dyDescent="0.2">
+      <c r="W39" s="2"/>
+    </row>
+    <row r="40" spans="1:23" hidden="1" x14ac:dyDescent="0.2">
       <c r="A40" s="3" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="41" spans="1:22" hidden="1" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:23" hidden="1" x14ac:dyDescent="0.2">
       <c r="A41" s="3" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="42" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A42" s="3" t="s">
         <v>48</v>
       </c>
@@ -6377,13 +6888,14 @@
       <c r="T42" s="2"/>
       <c r="U42" s="2"/>
       <c r="V42" s="2"/>
-    </row>
-    <row r="43" spans="1:22" hidden="1" x14ac:dyDescent="0.2">
+      <c r="W42" s="2"/>
+    </row>
+    <row r="43" spans="1:23" hidden="1" x14ac:dyDescent="0.2">
       <c r="A43" s="3" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="44" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A44" s="3" t="s">
         <v>50</v>
       </c>
@@ -6408,8 +6920,9 @@
       <c r="T44" s="2"/>
       <c r="U44" s="2"/>
       <c r="V44" s="2"/>
-    </row>
-    <row r="45" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="W44" s="2"/>
+    </row>
+    <row r="45" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A45" s="3" t="s">
         <v>51</v>
       </c>
@@ -6434,8 +6947,9 @@
       <c r="T45" s="2"/>
       <c r="U45" s="2"/>
       <c r="V45" s="2"/>
-    </row>
-    <row r="46" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="W45" s="2"/>
+    </row>
+    <row r="46" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A46" s="3" t="s">
         <v>52</v>
       </c>
@@ -6460,18 +6974,19 @@
       <c r="T46" s="2"/>
       <c r="U46" s="2"/>
       <c r="V46" s="2"/>
-    </row>
-    <row r="47" spans="1:22" hidden="1" x14ac:dyDescent="0.2">
+      <c r="W46" s="2"/>
+    </row>
+    <row r="47" spans="1:23" hidden="1" x14ac:dyDescent="0.2">
       <c r="A47" s="3" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="48" spans="1:22" hidden="1" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:23" hidden="1" x14ac:dyDescent="0.2">
       <c r="A48" s="3" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="49" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A49" s="3" t="s">
         <v>55</v>
       </c>
@@ -6496,18 +7011,19 @@
       <c r="T49" s="2"/>
       <c r="U49" s="2"/>
       <c r="V49" s="2"/>
-    </row>
-    <row r="50" spans="1:22" hidden="1" x14ac:dyDescent="0.2">
+      <c r="W49" s="2"/>
+    </row>
+    <row r="50" spans="1:23" hidden="1" x14ac:dyDescent="0.2">
       <c r="A50" s="3" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="51" spans="1:22" hidden="1" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:23" hidden="1" x14ac:dyDescent="0.2">
       <c r="A51" s="3" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="52" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:23" x14ac:dyDescent="0.2">
       <c r="B52" s="2"/>
       <c r="C52" s="2"/>
       <c r="D52" s="2"/>
@@ -6529,8 +7045,9 @@
       <c r="T52" s="2"/>
       <c r="U52" s="2"/>
       <c r="V52" s="2"/>
-    </row>
-    <row r="53" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="W52" s="2"/>
+    </row>
+    <row r="53" spans="1:23" x14ac:dyDescent="0.2">
       <c r="B53" s="2"/>
       <c r="C53" s="2"/>
       <c r="D53" s="2"/>
@@ -6552,8 +7069,9 @@
       <c r="T53" s="2"/>
       <c r="U53" s="2"/>
       <c r="V53" s="2"/>
-    </row>
-    <row r="54" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="W53" s="2"/>
+    </row>
+    <row r="54" spans="1:23" x14ac:dyDescent="0.2">
       <c r="B54" s="2"/>
       <c r="C54" s="2"/>
       <c r="D54" s="2"/>
@@ -6575,8 +7093,9 @@
       <c r="T54" s="2"/>
       <c r="U54" s="2"/>
       <c r="V54" s="2"/>
-    </row>
-    <row r="55" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="W54" s="2"/>
+    </row>
+    <row r="55" spans="1:23" x14ac:dyDescent="0.2">
       <c r="B55" s="2"/>
       <c r="C55" s="2"/>
       <c r="D55" s="2"/>
@@ -6598,8 +7117,9 @@
       <c r="T55" s="2"/>
       <c r="U55" s="2"/>
       <c r="V55" s="2"/>
-    </row>
-    <row r="56" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="W55" s="2"/>
+    </row>
+    <row r="56" spans="1:23" x14ac:dyDescent="0.2">
       <c r="B56" s="2"/>
       <c r="C56" s="2"/>
       <c r="D56" s="2"/>
@@ -6621,8 +7141,9 @@
       <c r="T56" s="2"/>
       <c r="U56" s="2"/>
       <c r="V56" s="2"/>
-    </row>
-    <row r="57" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="W56" s="2"/>
+    </row>
+    <row r="57" spans="1:23" x14ac:dyDescent="0.2">
       <c r="B57" s="2"/>
       <c r="C57" s="2"/>
       <c r="D57" s="2"/>
@@ -6644,8 +7165,9 @@
       <c r="T57" s="2"/>
       <c r="U57" s="2"/>
       <c r="V57" s="2"/>
-    </row>
-    <row r="58" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="W57" s="2"/>
+    </row>
+    <row r="58" spans="1:23" x14ac:dyDescent="0.2">
       <c r="B58" s="2"/>
       <c r="C58" s="2"/>
       <c r="D58" s="2"/>
@@ -6667,8 +7189,9 @@
       <c r="T58" s="2"/>
       <c r="U58" s="2"/>
       <c r="V58" s="2"/>
-    </row>
-    <row r="59" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="W58" s="2"/>
+    </row>
+    <row r="59" spans="1:23" x14ac:dyDescent="0.2">
       <c r="B59" s="2"/>
       <c r="C59" s="2"/>
       <c r="D59" s="2"/>
@@ -6690,8 +7213,9 @@
       <c r="T59" s="2"/>
       <c r="U59" s="2"/>
       <c r="V59" s="2"/>
-    </row>
-    <row r="60" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="W59" s="2"/>
+    </row>
+    <row r="60" spans="1:23" x14ac:dyDescent="0.2">
       <c r="B60" s="2"/>
       <c r="C60" s="2"/>
       <c r="D60" s="2"/>
@@ -6713,8 +7237,9 @@
       <c r="T60" s="2"/>
       <c r="U60" s="2"/>
       <c r="V60" s="2"/>
-    </row>
-    <row r="61" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="W60" s="2"/>
+    </row>
+    <row r="61" spans="1:23" x14ac:dyDescent="0.2">
       <c r="B61" s="2"/>
       <c r="C61" s="2"/>
       <c r="D61" s="2"/>
@@ -6736,8 +7261,9 @@
       <c r="T61" s="2"/>
       <c r="U61" s="2"/>
       <c r="V61" s="2"/>
-    </row>
-    <row r="62" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="W61" s="2"/>
+    </row>
+    <row r="62" spans="1:23" x14ac:dyDescent="0.2">
       <c r="B62" s="2"/>
       <c r="C62" s="2"/>
       <c r="D62" s="2"/>
@@ -6759,8 +7285,9 @@
       <c r="T62" s="2"/>
       <c r="U62" s="2"/>
       <c r="V62" s="2"/>
-    </row>
-    <row r="63" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="W62" s="2"/>
+    </row>
+    <row r="63" spans="1:23" x14ac:dyDescent="0.2">
       <c r="B63" s="2"/>
       <c r="C63" s="2"/>
       <c r="D63" s="2"/>
@@ -6782,8 +7309,9 @@
       <c r="T63" s="2"/>
       <c r="U63" s="2"/>
       <c r="V63" s="2"/>
-    </row>
-    <row r="64" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="W63" s="2"/>
+    </row>
+    <row r="64" spans="1:23" x14ac:dyDescent="0.2">
       <c r="B64" s="2"/>
       <c r="C64" s="2"/>
       <c r="D64" s="2"/>
@@ -6805,8 +7333,9 @@
       <c r="T64" s="2"/>
       <c r="U64" s="2"/>
       <c r="V64" s="2"/>
-    </row>
-    <row r="65" spans="2:22" x14ac:dyDescent="0.2">
+      <c r="W64" s="2"/>
+    </row>
+    <row r="65" spans="2:23" x14ac:dyDescent="0.2">
       <c r="B65" s="2"/>
       <c r="C65" s="2"/>
       <c r="D65" s="2"/>
@@ -6828,22 +7357,18 @@
       <c r="T65" s="2"/>
       <c r="U65" s="2"/>
       <c r="V65" s="2"/>
+      <c r="W65" s="2"/>
     </row>
   </sheetData>
   <autoFilter ref="A1:A51" xr:uid="{4E61F571-54A4-994C-A02B-889943573726}">
     <filterColumn colId="0">
       <filters>
-        <filter val="Alabama"/>
         <filter val="Arizona"/>
-        <filter val="Arkansas"/>
-        <filter val="Florida"/>
         <filter val="Georgia"/>
         <filter val="Iowa"/>
         <filter val="Kansas"/>
         <filter val="Kentucky"/>
-        <filter val="Louisiana"/>
         <filter val="Mississippi"/>
-        <filter val="North Carolina"/>
         <filter val="North Dakota"/>
         <filter val="Oklahoma"/>
         <filter val="Pennsylvania"/>

</xml_diff>

<commit_message>
Andrew | Finished proof of financial responsibility analysis.
</commit_message>
<xml_diff>
--- a/compliance/State Compliance Analysis.xlsx
+++ b/compliance/State Compliance Analysis.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/andrewhetzler/Documents/Documents - Andrew’s Money Maker/School/DISSERTATION/GitHub/dissertation/compliance/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5282DD08-44F2-E84E-BC20-F1D2A5F37F11}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9A8423E4-3D35-2D46-B787-C66640C79940}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="40960" windowHeight="24400" activeTab="1" xr2:uid="{FEE3D6CA-2CD0-2B4F-9478-6397B247951E}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="40960" windowHeight="24400" activeTab="3" xr2:uid="{FEE3D6CA-2CD0-2B4F-9478-6397B247951E}"/>
   </bookViews>
   <sheets>
     <sheet name="PoFR - Bond" sheetId="6" r:id="rId1"/>
@@ -49,7 +49,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2103" uniqueCount="395">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2457" uniqueCount="446">
   <si>
     <t>STATE</t>
   </si>
@@ -2009,6 +2009,350 @@
   </si>
   <si>
     <t>Required (28-4007(B))</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">NOTE </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>alos supports deposit (39-16.1-15(1))</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>which also issues a certificate. No details on the  deposit cert</t>
+    </r>
+  </si>
+  <si>
+    <t>Required (39-16.1-09(1))</t>
+  </si>
+  <si>
+    <t>Optional--only required if driver is not insured for all vehicles on policy (39-16.1-09(2))</t>
+  </si>
+  <si>
+    <t>Required (47-7-601.1(A)(1)(a)</t>
+  </si>
+  <si>
+    <t>Optional--only required if insurance is not carrier  (47-7-601.1(A)(1)(b))</t>
+  </si>
+  <si>
+    <t>ADDRESS OF LOCAL AGENT</t>
+  </si>
+  <si>
+    <t>Required (47-7-601.1(A)(1)(c ))</t>
+  </si>
+  <si>
+    <t>Explicitly excluded</t>
+  </si>
+  <si>
+    <t>STATEMENT OF COMPLIANCE</t>
+  </si>
+  <si>
+    <t>Required (47-7-601.1(A)(1)(d))</t>
+  </si>
+  <si>
+    <t>Required (47-7-601.1(A)(1)(e ))</t>
+  </si>
+  <si>
+    <t>MODEL</t>
+  </si>
+  <si>
+    <t>Required (47-7-601.1(A)(1)(f))</t>
+  </si>
+  <si>
+    <t>Required (47-7-601.1(A)(1)(g))</t>
+  </si>
+  <si>
+    <t>Optional (47-7-601.1(A)(2))</t>
+  </si>
+  <si>
+    <t>Optional--only required if fleet distinction missing (47-7-601.1(A)(2))</t>
+  </si>
+  <si>
+    <t>(47-7-601.1(A)(2))</t>
+  </si>
+  <si>
+    <t>WARNING TO CARRY PROOF</t>
+  </si>
+  <si>
+    <t>Required (47-7-601.1(A)(1)(h))</t>
+  </si>
+  <si>
+    <t>EXAMINE POLICY EXCLUSIONS STATEMENT</t>
+  </si>
+  <si>
+    <t>Required (47-7-601.1(A)(1)(i))</t>
+  </si>
+  <si>
+    <t>Required (47-7-503)(a)</t>
+  </si>
+  <si>
+    <t>Optional--just one of several ways to pay (75-17-1787(a))</t>
+  </si>
+  <si>
+    <t>No details on how to prove self-insurance.</t>
+  </si>
+  <si>
+    <t>Required (75-17-1782(d))</t>
+  </si>
+  <si>
+    <t>INFORMATION NEEDED BY INSURANCE DEPT</t>
+  </si>
+  <si>
+    <t>Required (32-35-90)</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>NOTE</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> also supports deposits</t>
+    </r>
+  </si>
+  <si>
+    <t>Required (32-35-65)</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Required (32-35-65) </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>NOTE</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> unless driver is not owner</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>. Must be for all vehicles</t>
+    </r>
+  </si>
+  <si>
+    <t>Required (601.081(b)(1))</t>
+  </si>
+  <si>
+    <t>Required (601.081(b)(2))</t>
+  </si>
+  <si>
+    <t>Required (601.081(b)(3))</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Required (601.081(b)(4)) </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>NOTE</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> may be multiple</t>
+    </r>
+  </si>
+  <si>
+    <t>LIMITS OR STATEMENT OF COVERAGE</t>
+  </si>
+  <si>
+    <t>Required (601.081(b)(5))</t>
+  </si>
+  <si>
+    <t>Required (601.081(b)(6)) NOTE may be multiple</t>
+  </si>
+  <si>
+    <t>Required (601.124(a))</t>
+  </si>
+  <si>
+    <t>May not (41-12a-303.2(2)(c ))</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>NOTE</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> also supports treasurer certification (41-12a-406. No details on bond or treasurer certificate</t>
+    </r>
+  </si>
+  <si>
+    <t>Required (41-12a-407)</t>
+  </si>
+  <si>
+    <t>Required (41-12a-402)</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve"> Required (41-12a-402) </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>NOTE</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> may be multiple</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>. Also unless issuee is not owner of vehicle</t>
+    </r>
+  </si>
+  <si>
+    <t>No details</t>
+  </si>
+  <si>
+    <t>Required (23-801(c ))</t>
+  </si>
+  <si>
+    <t>Required (23-804(a))</t>
+  </si>
+  <si>
+    <t>Required (17D-2A-4(a))</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Required (17D-2A-4(a)) </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">NOTE </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>may be multiple. Also unless issuee is not owner of vehicle</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Required (17D-2A-4(a)) </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>NOTE</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> must list owner name if different from insured</t>
+    </r>
+  </si>
+  <si>
+    <t>LIABILITY COVERAGE STATEMENT</t>
+  </si>
+  <si>
+    <t>Required (17D-6-2(b))</t>
   </si>
 </sst>
 </file>
@@ -2443,7 +2787,7 @@
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="B49" sqref="B49"/>
+      <selection pane="topRight" activeCell="B46" sqref="B46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2922,13 +3266,17 @@
       <c r="T34" s="2"/>
       <c r="U34" s="2"/>
     </row>
-    <row r="35" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:21" ht="51" x14ac:dyDescent="0.2">
       <c r="A35" s="3" t="s">
         <v>41</v>
       </c>
-      <c r="B35" s="2"/>
+      <c r="B35" s="2" t="s">
+        <v>80</v>
+      </c>
       <c r="C35" s="2"/>
-      <c r="D35" s="2"/>
+      <c r="D35" s="6" t="s">
+        <v>395</v>
+      </c>
       <c r="E35" s="2"/>
       <c r="F35" s="2"/>
       <c r="G35" s="2"/>
@@ -2952,7 +3300,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="37" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:21" hidden="1" x14ac:dyDescent="0.2">
       <c r="A37" s="3" t="s">
         <v>43</v>
       </c>
@@ -2982,7 +3330,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="39" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:21" hidden="1" x14ac:dyDescent="0.2">
       <c r="A39" s="3" t="s">
         <v>45</v>
       </c>
@@ -3017,13 +3365,17 @@
         <v>47</v>
       </c>
     </row>
-    <row r="42" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:21" ht="17" x14ac:dyDescent="0.2">
       <c r="A42" s="3" t="s">
         <v>48</v>
       </c>
-      <c r="B42" s="2"/>
+      <c r="B42" s="2" t="s">
+        <v>80</v>
+      </c>
       <c r="C42" s="2"/>
-      <c r="D42" s="2"/>
+      <c r="D42" s="5" t="s">
+        <v>422</v>
+      </c>
       <c r="E42" s="2"/>
       <c r="F42" s="2"/>
       <c r="G42" s="2"/>
@@ -3047,7 +3399,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="44" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:21" hidden="1" x14ac:dyDescent="0.2">
       <c r="A44" s="3" t="s">
         <v>50</v>
       </c>
@@ -3072,13 +3424,17 @@
       <c r="T44" s="2"/>
       <c r="U44" s="2"/>
     </row>
-    <row r="45" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:21" ht="51" x14ac:dyDescent="0.2">
       <c r="A45" s="3" t="s">
         <v>51</v>
       </c>
-      <c r="B45" s="2"/>
+      <c r="B45" s="2" t="s">
+        <v>80</v>
+      </c>
       <c r="C45" s="2"/>
-      <c r="D45" s="2"/>
+      <c r="D45" s="5" t="s">
+        <v>434</v>
+      </c>
       <c r="E45" s="2"/>
       <c r="F45" s="2"/>
       <c r="G45" s="2"/>
@@ -3097,13 +3453,17 @@
       <c r="T45" s="2"/>
       <c r="U45" s="2"/>
     </row>
-    <row r="46" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:21" ht="17" x14ac:dyDescent="0.2">
       <c r="A46" s="3" t="s">
         <v>52</v>
       </c>
-      <c r="B46" s="2"/>
+      <c r="B46" s="2" t="s">
+        <v>80</v>
+      </c>
       <c r="C46" s="2"/>
-      <c r="D46" s="2"/>
+      <c r="D46" s="2" t="s">
+        <v>438</v>
+      </c>
       <c r="E46" s="2"/>
       <c r="F46" s="2"/>
       <c r="G46" s="2"/>
@@ -3132,7 +3492,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="49" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:21" hidden="1" x14ac:dyDescent="0.2">
       <c r="A49" s="3" t="s">
         <v>55</v>
       </c>
@@ -3482,13 +3842,9 @@
         <filter val="Arizona"/>
         <filter val="Mississippi"/>
         <filter val="North Dakota"/>
-        <filter val="Oklahoma"/>
-        <filter val="Pennsylvania"/>
         <filter val="South Dakota"/>
-        <filter val="Texas"/>
         <filter val="Utah"/>
         <filter val="Vermont"/>
-        <filter val="West Virginia"/>
       </filters>
     </filterColumn>
   </autoFilter>
@@ -3499,11 +3855,11 @@
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4E61F571-54A4-994C-A02B-889943573726}">
   <sheetPr filterMode="1"/>
-  <dimension ref="A1:AA65"/>
+  <dimension ref="A1:AB65"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="H19" sqref="H19"/>
+    <sheetView workbookViewId="0">
+      <pane xSplit="1" topLeftCell="U1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="AB49" sqref="AB49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3528,9 +3884,17 @@
     <col min="18" max="18" width="41" customWidth="1"/>
     <col min="19" max="19" width="25.6640625" customWidth="1"/>
     <col min="20" max="20" width="34.5" customWidth="1"/>
+    <col min="21" max="21" width="35.1640625" customWidth="1"/>
+    <col min="22" max="22" width="33.6640625" customWidth="1"/>
+    <col min="23" max="23" width="25.5" customWidth="1"/>
+    <col min="24" max="24" width="40.5" customWidth="1"/>
+    <col min="25" max="25" width="36.5" customWidth="1"/>
+    <col min="26" max="26" width="50.1640625" customWidth="1"/>
+    <col min="27" max="27" width="31.5" customWidth="1"/>
+    <col min="28" max="28" width="41.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -3591,15 +3955,32 @@
       <c r="T1" s="1" t="s">
         <v>383</v>
       </c>
-      <c r="U1" s="1"/>
-      <c r="V1" s="1"/>
-      <c r="W1" s="1"/>
-      <c r="X1" s="1"/>
-      <c r="Y1" s="1"/>
-      <c r="Z1" s="1"/>
-      <c r="AA1" s="1"/>
-    </row>
-    <row r="2" spans="1:27" ht="34" x14ac:dyDescent="0.2">
+      <c r="U1" s="1" t="s">
+        <v>400</v>
+      </c>
+      <c r="V1" s="1" t="s">
+        <v>403</v>
+      </c>
+      <c r="W1" s="1" t="s">
+        <v>406</v>
+      </c>
+      <c r="X1" s="1" t="s">
+        <v>412</v>
+      </c>
+      <c r="Y1" s="1" t="s">
+        <v>414</v>
+      </c>
+      <c r="Z1" s="1" t="s">
+        <v>420</v>
+      </c>
+      <c r="AA1" s="1" t="s">
+        <v>429</v>
+      </c>
+      <c r="AB1" s="1" t="s">
+        <v>444</v>
+      </c>
+    </row>
+    <row r="2" spans="1:28" ht="34" x14ac:dyDescent="0.2">
       <c r="A2" s="3" t="s">
         <v>9</v>
       </c>
@@ -3660,15 +4041,37 @@
       <c r="T2" s="2" t="s">
         <v>80</v>
       </c>
-      <c r="U2" s="2"/>
-      <c r="V2" s="2"/>
-    </row>
-    <row r="3" spans="1:27" hidden="1" x14ac:dyDescent="0.2">
+      <c r="U2" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="V2" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="W2" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="X2" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="Y2" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="Z2" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="AA2" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="AB2" s="2" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="3" spans="1:28" hidden="1" x14ac:dyDescent="0.2">
       <c r="A3" s="3" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="4" spans="1:27" ht="51" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:28" ht="51" x14ac:dyDescent="0.2">
       <c r="A4" s="3" t="s">
         <v>11</v>
       </c>
@@ -3729,10 +4132,32 @@
       <c r="T4" s="2" t="s">
         <v>80</v>
       </c>
-      <c r="U4" s="2"/>
-      <c r="V4" s="2"/>
-    </row>
-    <row r="5" spans="1:27" ht="68" x14ac:dyDescent="0.2">
+      <c r="U4" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="V4" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="W4" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="X4" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="Y4" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="Z4" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="AA4" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="AB4" s="2" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="5" spans="1:28" ht="68" x14ac:dyDescent="0.2">
       <c r="A5" s="3" t="s">
         <v>12</v>
       </c>
@@ -3793,10 +4218,32 @@
       <c r="T5" s="2" t="s">
         <v>80</v>
       </c>
-      <c r="U5" s="2"/>
-      <c r="V5" s="2"/>
-    </row>
-    <row r="6" spans="1:27" hidden="1" x14ac:dyDescent="0.2">
+      <c r="U5" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="V5" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="W5" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="X5" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="Y5" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="Z5" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="AA5" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="AB5" s="2" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="6" spans="1:28" hidden="1" x14ac:dyDescent="0.2">
       <c r="A6" s="3" t="s">
         <v>13</v>
       </c>
@@ -3822,22 +4269,22 @@
       <c r="U6" s="2"/>
       <c r="V6" s="2"/>
     </row>
-    <row r="7" spans="1:27" hidden="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:28" hidden="1" x14ac:dyDescent="0.2">
       <c r="A7" s="3" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="8" spans="1:27" hidden="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:28" hidden="1" x14ac:dyDescent="0.2">
       <c r="A8" s="3" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="9" spans="1:27" hidden="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:28" hidden="1" x14ac:dyDescent="0.2">
       <c r="A9" s="3" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="10" spans="1:27" ht="17" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:28" ht="17" x14ac:dyDescent="0.2">
       <c r="A10" s="3" t="s">
         <v>16</v>
       </c>
@@ -3898,10 +4345,32 @@
       <c r="T10" s="2" t="s">
         <v>80</v>
       </c>
-      <c r="U10" s="2"/>
-      <c r="V10" s="2"/>
-    </row>
-    <row r="11" spans="1:27" ht="17" x14ac:dyDescent="0.2">
+      <c r="U10" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="V10" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="W10" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="X10" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="Y10" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="Z10" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="AA10" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="AB10" s="2" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="11" spans="1:28" ht="17" x14ac:dyDescent="0.2">
       <c r="A11" s="3" t="s">
         <v>17</v>
       </c>
@@ -3962,30 +4431,52 @@
       <c r="T11" s="2" t="s">
         <v>80</v>
       </c>
-      <c r="U11" s="2"/>
-      <c r="V11" s="2"/>
-    </row>
-    <row r="12" spans="1:27" hidden="1" x14ac:dyDescent="0.2">
+      <c r="U11" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="V11" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="W11" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="X11" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="Y11" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="Z11" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="AA11" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="AB11" s="2" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="12" spans="1:28" hidden="1" x14ac:dyDescent="0.2">
       <c r="A12" s="3" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="13" spans="1:27" hidden="1" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:28" hidden="1" x14ac:dyDescent="0.2">
       <c r="A13" s="3" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="14" spans="1:27" hidden="1" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:28" hidden="1" x14ac:dyDescent="0.2">
       <c r="A14" s="3" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="15" spans="1:27" hidden="1" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:28" hidden="1" x14ac:dyDescent="0.2">
       <c r="A15" s="3" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="16" spans="1:27" ht="17" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:28" ht="17" x14ac:dyDescent="0.2">
       <c r="A16" s="3" t="s">
         <v>22</v>
       </c>
@@ -4046,10 +4537,32 @@
       <c r="T16" s="2" t="s">
         <v>80</v>
       </c>
-      <c r="U16" s="2"/>
-      <c r="V16" s="2"/>
-    </row>
-    <row r="17" spans="1:22" ht="17" x14ac:dyDescent="0.2">
+      <c r="U16" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="V16" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="W16" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="X16" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="Y16" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="Z16" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="AA16" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="AB16" s="2" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="17" spans="1:28" ht="17" x14ac:dyDescent="0.2">
       <c r="A17" s="3" t="s">
         <v>23</v>
       </c>
@@ -4110,10 +4623,32 @@
       <c r="T17" s="2" t="s">
         <v>80</v>
       </c>
-      <c r="U17" s="2"/>
-      <c r="V17" s="2"/>
-    </row>
-    <row r="18" spans="1:22" ht="17" x14ac:dyDescent="0.2">
+      <c r="U17" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="V17" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="W17" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="X17" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="Y17" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="Z17" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="AA17" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="AB17" s="2" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="18" spans="1:28" ht="17" x14ac:dyDescent="0.2">
       <c r="A18" s="3" t="s">
         <v>24</v>
       </c>
@@ -4174,10 +4709,32 @@
       <c r="T18" s="2" t="s">
         <v>80</v>
       </c>
-      <c r="U18" s="2"/>
-      <c r="V18" s="2"/>
-    </row>
-    <row r="19" spans="1:22" ht="34" x14ac:dyDescent="0.2">
+      <c r="U18" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="V18" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="W18" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="X18" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="Y18" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="Z18" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="AA18" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="AB18" s="2" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="19" spans="1:28" ht="34" x14ac:dyDescent="0.2">
       <c r="A19" s="3" t="s">
         <v>25</v>
       </c>
@@ -4238,35 +4795,57 @@
       <c r="T19" s="2" t="s">
         <v>384</v>
       </c>
-      <c r="U19" s="2"/>
-      <c r="V19" s="2"/>
-    </row>
-    <row r="20" spans="1:22" hidden="1" x14ac:dyDescent="0.2">
+      <c r="U19" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="V19" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="W19" s="2" t="s">
+        <v>389</v>
+      </c>
+      <c r="X19" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="Y19" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="Z19" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="AA19" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="AB19" s="2" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="20" spans="1:28" hidden="1" x14ac:dyDescent="0.2">
       <c r="A20" s="3" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="21" spans="1:22" hidden="1" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:28" hidden="1" x14ac:dyDescent="0.2">
       <c r="A21" s="3" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="22" spans="1:22" hidden="1" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:28" hidden="1" x14ac:dyDescent="0.2">
       <c r="A22" s="3" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="23" spans="1:22" hidden="1" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:28" hidden="1" x14ac:dyDescent="0.2">
       <c r="A23" s="3" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="24" spans="1:22" hidden="1" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:28" hidden="1" x14ac:dyDescent="0.2">
       <c r="A24" s="3" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="25" spans="1:22" ht="34" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:28" ht="34" x14ac:dyDescent="0.2">
       <c r="A25" s="3" t="s">
         <v>31</v>
       </c>
@@ -4327,50 +4906,72 @@
       <c r="T25" s="2" t="s">
         <v>388</v>
       </c>
-      <c r="U25" s="2"/>
-      <c r="V25" s="2"/>
-    </row>
-    <row r="26" spans="1:22" hidden="1" x14ac:dyDescent="0.2">
+      <c r="U25" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="V25" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="W25" s="2" t="s">
+        <v>389</v>
+      </c>
+      <c r="X25" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="Y25" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="Z25" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="AA25" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="AB25" s="2" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="26" spans="1:28" hidden="1" x14ac:dyDescent="0.2">
       <c r="A26" s="3" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="27" spans="1:22" hidden="1" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:28" hidden="1" x14ac:dyDescent="0.2">
       <c r="A27" s="3" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="28" spans="1:22" hidden="1" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:28" hidden="1" x14ac:dyDescent="0.2">
       <c r="A28" s="3" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="29" spans="1:22" hidden="1" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:28" hidden="1" x14ac:dyDescent="0.2">
       <c r="A29" s="3" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="30" spans="1:22" hidden="1" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:28" hidden="1" x14ac:dyDescent="0.2">
       <c r="A30" s="3" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="31" spans="1:22" hidden="1" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:28" hidden="1" x14ac:dyDescent="0.2">
       <c r="A31" s="3" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="32" spans="1:22" hidden="1" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:28" hidden="1" x14ac:dyDescent="0.2">
       <c r="A32" s="3" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="33" spans="1:22" hidden="1" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:28" hidden="1" x14ac:dyDescent="0.2">
       <c r="A33" s="3" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="34" spans="1:22" ht="17" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:28" ht="17" x14ac:dyDescent="0.2">
       <c r="A34" s="3" t="s">
         <v>40</v>
       </c>
@@ -4431,263 +5032,765 @@
       <c r="T34" s="2" t="s">
         <v>392</v>
       </c>
-      <c r="U34" s="2"/>
-      <c r="V34" s="2"/>
-    </row>
-    <row r="35" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="U34" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="V34" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="W34" s="2" t="s">
+        <v>389</v>
+      </c>
+      <c r="X34" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="Y34" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="Z34" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="AA34" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="AB34" s="2" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="35" spans="1:28" ht="51" x14ac:dyDescent="0.2">
       <c r="A35" s="3" t="s">
         <v>41</v>
       </c>
-      <c r="B35" s="2"/>
-      <c r="C35" s="2"/>
-      <c r="D35" s="2"/>
-      <c r="E35" s="2"/>
-      <c r="F35" s="2"/>
-      <c r="G35" s="2"/>
-      <c r="H35" s="2"/>
-      <c r="I35" s="2"/>
-      <c r="J35" s="2"/>
-      <c r="K35" s="2"/>
-      <c r="L35" s="2"/>
-      <c r="M35" s="2"/>
-      <c r="N35" s="2"/>
-      <c r="O35" s="2"/>
-      <c r="P35" s="2"/>
-      <c r="Q35" s="2"/>
-      <c r="R35" s="2"/>
-      <c r="S35" s="2"/>
-      <c r="T35" s="2"/>
-      <c r="U35" s="2"/>
-      <c r="V35" s="2"/>
-    </row>
-    <row r="36" spans="1:22" hidden="1" x14ac:dyDescent="0.2">
+      <c r="B35" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="C35" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="D35" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="E35" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="F35" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="G35" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="H35" s="2" t="s">
+        <v>396</v>
+      </c>
+      <c r="I35" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="J35" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="K35" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="L35" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="M35" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="N35" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="O35" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="P35" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="Q35" s="2" t="s">
+        <v>397</v>
+      </c>
+      <c r="R35" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="S35" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="T35" s="2" t="s">
+        <v>396</v>
+      </c>
+      <c r="U35" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="V35" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="W35" s="2" t="s">
+        <v>389</v>
+      </c>
+      <c r="X35" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="Y35" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="Z35" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="AA35" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="AB35" s="2" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="36" spans="1:28" hidden="1" x14ac:dyDescent="0.2">
       <c r="A36" s="3" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="37" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:28" ht="51" x14ac:dyDescent="0.2">
       <c r="A37" s="3" t="s">
         <v>43</v>
       </c>
-      <c r="B37" s="2"/>
-      <c r="C37" s="2"/>
-      <c r="D37" s="2"/>
-      <c r="E37" s="2"/>
-      <c r="F37" s="2"/>
-      <c r="G37" s="2"/>
-      <c r="H37" s="2"/>
-      <c r="I37" s="2"/>
-      <c r="J37" s="2"/>
-      <c r="K37" s="2"/>
-      <c r="L37" s="2"/>
-      <c r="M37" s="2"/>
-      <c r="N37" s="2"/>
-      <c r="O37" s="2"/>
-      <c r="P37" s="2"/>
-      <c r="Q37" s="2"/>
-      <c r="R37" s="2"/>
-      <c r="S37" s="2"/>
-      <c r="T37" s="2"/>
-      <c r="U37" s="2"/>
-      <c r="V37" s="2"/>
-    </row>
-    <row r="38" spans="1:22" hidden="1" x14ac:dyDescent="0.2">
+      <c r="B37" s="2" t="s">
+        <v>405</v>
+      </c>
+      <c r="C37" s="2" t="s">
+        <v>405</v>
+      </c>
+      <c r="D37" s="2" t="s">
+        <v>405</v>
+      </c>
+      <c r="E37" s="2" t="s">
+        <v>401</v>
+      </c>
+      <c r="F37" s="2" t="s">
+        <v>398</v>
+      </c>
+      <c r="G37" s="2" t="s">
+        <v>408</v>
+      </c>
+      <c r="H37" s="2" t="s">
+        <v>407</v>
+      </c>
+      <c r="I37" s="2" t="s">
+        <v>407</v>
+      </c>
+      <c r="J37" s="2" t="s">
+        <v>402</v>
+      </c>
+      <c r="K37" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="L37" s="2" t="s">
+        <v>398</v>
+      </c>
+      <c r="M37" s="2" t="s">
+        <v>398</v>
+      </c>
+      <c r="N37" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="O37" s="2" t="s">
+        <v>399</v>
+      </c>
+      <c r="P37" s="2" t="s">
+        <v>399</v>
+      </c>
+      <c r="Q37" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="R37" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="S37" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="T37" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="U37" s="2" t="s">
+        <v>399</v>
+      </c>
+      <c r="V37" s="2" t="s">
+        <v>404</v>
+      </c>
+      <c r="W37" s="5" t="s">
+        <v>405</v>
+      </c>
+      <c r="X37" s="5" t="s">
+        <v>413</v>
+      </c>
+      <c r="Y37" s="5" t="s">
+        <v>415</v>
+      </c>
+      <c r="Z37" s="5" t="s">
+        <v>80</v>
+      </c>
+      <c r="AA37" s="5" t="s">
+        <v>80</v>
+      </c>
+      <c r="AB37" s="2" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="38" spans="1:28" hidden="1" x14ac:dyDescent="0.2">
       <c r="A38" s="3" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="39" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:28" ht="34" x14ac:dyDescent="0.2">
       <c r="A39" s="3" t="s">
         <v>45</v>
       </c>
-      <c r="B39" s="2"/>
-      <c r="C39" s="2"/>
-      <c r="D39" s="2"/>
-      <c r="E39" s="2"/>
-      <c r="F39" s="2"/>
-      <c r="G39" s="2"/>
-      <c r="H39" s="2"/>
-      <c r="I39" s="2"/>
-      <c r="J39" s="2"/>
-      <c r="K39" s="2"/>
-      <c r="L39" s="2"/>
-      <c r="M39" s="2"/>
-      <c r="N39" s="2"/>
-      <c r="O39" s="2"/>
-      <c r="P39" s="2"/>
-      <c r="Q39" s="2"/>
-      <c r="R39" s="2"/>
-      <c r="S39" s="2"/>
-      <c r="T39" s="2"/>
-      <c r="U39" s="2"/>
-      <c r="V39" s="2"/>
-    </row>
-    <row r="40" spans="1:22" hidden="1" x14ac:dyDescent="0.2">
+      <c r="B39" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="C39" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="D39" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="E39" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="F39" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="G39" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="H39" s="2" t="s">
+        <v>419</v>
+      </c>
+      <c r="I39" s="2" t="s">
+        <v>419</v>
+      </c>
+      <c r="J39" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="K39" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="L39" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="M39" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="N39" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="O39" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="P39" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="Q39" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="R39" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="S39" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="T39" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="U39" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="V39" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="W39" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="X39" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="Y39" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="Z39" s="5" t="s">
+        <v>419</v>
+      </c>
+      <c r="AA39" s="5" t="s">
+        <v>80</v>
+      </c>
+      <c r="AB39" s="2" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="40" spans="1:28" hidden="1" x14ac:dyDescent="0.2">
       <c r="A40" s="3" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="41" spans="1:22" hidden="1" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:28" hidden="1" x14ac:dyDescent="0.2">
       <c r="A41" s="3" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="42" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:28" ht="34" x14ac:dyDescent="0.2">
       <c r="A42" s="3" t="s">
         <v>48</v>
       </c>
-      <c r="B42" s="2"/>
-      <c r="C42" s="2"/>
-      <c r="D42" s="2"/>
-      <c r="E42" s="2"/>
-      <c r="F42" s="2"/>
-      <c r="G42" s="2"/>
-      <c r="H42" s="2"/>
-      <c r="I42" s="2"/>
-      <c r="J42" s="2"/>
-      <c r="K42" s="2"/>
-      <c r="L42" s="2"/>
-      <c r="M42" s="2"/>
-      <c r="N42" s="2"/>
-      <c r="O42" s="2"/>
-      <c r="P42" s="2"/>
-      <c r="Q42" s="2"/>
-      <c r="R42" s="2"/>
-      <c r="S42" s="2"/>
-      <c r="T42" s="2"/>
-      <c r="U42" s="2"/>
-      <c r="V42" s="2"/>
-    </row>
-    <row r="43" spans="1:22" hidden="1" x14ac:dyDescent="0.2">
+      <c r="B42" s="2" t="s">
+        <v>389</v>
+      </c>
+      <c r="C42" s="2" t="s">
+        <v>389</v>
+      </c>
+      <c r="D42" s="2" t="s">
+        <v>389</v>
+      </c>
+      <c r="E42" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="F42" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="G42" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="H42" s="2" t="s">
+        <v>423</v>
+      </c>
+      <c r="I42" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="J42" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="K42" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="L42" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="M42" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="N42" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="O42" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="P42" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="Q42" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="R42" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="S42" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="T42" s="2" t="s">
+        <v>424</v>
+      </c>
+      <c r="U42" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="V42" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="W42" s="2" t="s">
+        <v>389</v>
+      </c>
+      <c r="X42" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="Y42" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="Z42" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="AA42" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="AB42" s="2" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="43" spans="1:28" hidden="1" x14ac:dyDescent="0.2">
       <c r="A43" s="3" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="44" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:28" ht="51" x14ac:dyDescent="0.2">
       <c r="A44" s="3" t="s">
         <v>50</v>
       </c>
-      <c r="B44" s="2"/>
-      <c r="C44" s="2"/>
-      <c r="D44" s="2"/>
-      <c r="E44" s="2"/>
-      <c r="F44" s="2"/>
-      <c r="G44" s="2"/>
-      <c r="H44" s="2"/>
-      <c r="I44" s="2"/>
-      <c r="J44" s="2"/>
-      <c r="K44" s="2"/>
-      <c r="L44" s="2"/>
-      <c r="M44" s="2"/>
-      <c r="N44" s="2"/>
-      <c r="O44" s="2"/>
-      <c r="P44" s="2"/>
-      <c r="Q44" s="2"/>
-      <c r="R44" s="2"/>
-      <c r="S44" s="2"/>
-      <c r="T44" s="2"/>
-      <c r="U44" s="2"/>
-      <c r="V44" s="2"/>
-    </row>
-    <row r="45" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="B44" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="C44" s="4" t="s">
+        <v>431</v>
+      </c>
+      <c r="D44" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="E44" s="2" t="s">
+        <v>428</v>
+      </c>
+      <c r="F44" s="2" t="s">
+        <v>425</v>
+      </c>
+      <c r="G44" s="2" t="s">
+        <v>426</v>
+      </c>
+      <c r="H44" s="2" t="s">
+        <v>427</v>
+      </c>
+      <c r="I44" s="2" t="s">
+        <v>427</v>
+      </c>
+      <c r="J44" s="2" t="s">
+        <v>428</v>
+      </c>
+      <c r="K44" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="L44" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="M44" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="N44" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="O44" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="P44" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="Q44" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="R44" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="S44" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="T44" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="U44" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="V44" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="W44" s="2" t="s">
+        <v>431</v>
+      </c>
+      <c r="X44" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="Y44" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="Z44" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="AA44" s="2" t="s">
+        <v>430</v>
+      </c>
+      <c r="AB44" s="2" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="45" spans="1:28" ht="51" x14ac:dyDescent="0.2">
       <c r="A45" s="3" t="s">
         <v>51</v>
       </c>
-      <c r="B45" s="2"/>
-      <c r="C45" s="2"/>
-      <c r="D45" s="2"/>
-      <c r="E45" s="2"/>
-      <c r="F45" s="2"/>
-      <c r="G45" s="2"/>
-      <c r="H45" s="2"/>
-      <c r="I45" s="2"/>
-      <c r="J45" s="2"/>
-      <c r="K45" s="2"/>
-      <c r="L45" s="2"/>
-      <c r="M45" s="2"/>
-      <c r="N45" s="2"/>
-      <c r="O45" s="2"/>
-      <c r="P45" s="2"/>
-      <c r="Q45" s="2"/>
-      <c r="R45" s="2"/>
-      <c r="S45" s="2"/>
-      <c r="T45" s="2"/>
-      <c r="U45" s="2"/>
-      <c r="V45" s="2"/>
-    </row>
-    <row r="46" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="B45" s="2" t="s">
+        <v>389</v>
+      </c>
+      <c r="C45" s="2" t="s">
+        <v>389</v>
+      </c>
+      <c r="D45" s="2" t="s">
+        <v>389</v>
+      </c>
+      <c r="E45" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="F45" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="G45" s="2" t="s">
+        <v>436</v>
+      </c>
+      <c r="H45" s="2" t="s">
+        <v>436</v>
+      </c>
+      <c r="I45" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="J45" s="2" t="s">
+        <v>433</v>
+      </c>
+      <c r="K45" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="L45" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="M45" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="N45" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="O45" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="P45" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="Q45" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="R45" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="S45" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="T45" s="2" t="s">
+        <v>437</v>
+      </c>
+      <c r="U45" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="V45" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="W45" s="2" t="s">
+        <v>389</v>
+      </c>
+      <c r="X45" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="Y45" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="Z45" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="AA45" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="AB45" s="2" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="46" spans="1:28" ht="17" x14ac:dyDescent="0.2">
       <c r="A46" s="3" t="s">
         <v>52</v>
       </c>
-      <c r="B46" s="2"/>
-      <c r="C46" s="2"/>
-      <c r="D46" s="2"/>
-      <c r="E46" s="2"/>
-      <c r="F46" s="2"/>
-      <c r="G46" s="2"/>
-      <c r="H46" s="2"/>
-      <c r="I46" s="2"/>
-      <c r="J46" s="2"/>
-      <c r="K46" s="2"/>
-      <c r="L46" s="2"/>
-      <c r="M46" s="2"/>
-      <c r="N46" s="2"/>
-      <c r="O46" s="2"/>
-      <c r="P46" s="2"/>
-      <c r="Q46" s="2"/>
-      <c r="R46" s="2"/>
-      <c r="S46" s="2"/>
-      <c r="T46" s="2"/>
-      <c r="U46" s="2"/>
-      <c r="V46" s="2"/>
-    </row>
-    <row r="47" spans="1:22" hidden="1" x14ac:dyDescent="0.2">
+      <c r="B46" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="C46" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="D46" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="E46" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="F46" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="G46" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="H46" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="I46" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="J46" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="K46" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="L46" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="M46" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="N46" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="O46" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="P46" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="Q46" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="R46" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="S46" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="T46" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="U46" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="V46" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="W46" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="X46" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="Y46" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="Z46" s="2" t="s">
+        <v>440</v>
+      </c>
+      <c r="AA46" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="AB46" s="2" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="47" spans="1:28" hidden="1" x14ac:dyDescent="0.2">
       <c r="A47" s="3" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="48" spans="1:22" hidden="1" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:28" hidden="1" x14ac:dyDescent="0.2">
       <c r="A48" s="3" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="49" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:28" ht="51" x14ac:dyDescent="0.2">
       <c r="A49" s="3" t="s">
         <v>55</v>
       </c>
-      <c r="B49" s="2"/>
-      <c r="C49" s="2"/>
-      <c r="D49" s="2"/>
-      <c r="E49" s="2"/>
-      <c r="F49" s="2"/>
-      <c r="G49" s="2"/>
-      <c r="H49" s="2"/>
-      <c r="I49" s="2"/>
-      <c r="J49" s="2"/>
-      <c r="K49" s="2"/>
-      <c r="L49" s="2"/>
-      <c r="M49" s="2"/>
-      <c r="N49" s="2"/>
-      <c r="O49" s="2"/>
-      <c r="P49" s="2"/>
-      <c r="Q49" s="2"/>
-      <c r="R49" s="2"/>
-      <c r="S49" s="2"/>
-      <c r="T49" s="2"/>
-      <c r="U49" s="2"/>
-      <c r="V49" s="2"/>
-    </row>
-    <row r="50" spans="1:22" hidden="1" x14ac:dyDescent="0.2">
+      <c r="B49" s="2" t="s">
+        <v>389</v>
+      </c>
+      <c r="C49" s="2" t="s">
+        <v>389</v>
+      </c>
+      <c r="D49" s="2" t="s">
+        <v>389</v>
+      </c>
+      <c r="E49" s="2" t="s">
+        <v>443</v>
+      </c>
+      <c r="F49" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="G49" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="H49" s="2" t="s">
+        <v>441</v>
+      </c>
+      <c r="I49" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="J49" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="K49" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="L49" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="M49" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="N49" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="O49" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="P49" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="Q49" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="R49" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="S49" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="T49" s="2" t="s">
+        <v>442</v>
+      </c>
+      <c r="U49" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="V49" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="W49" s="2" t="s">
+        <v>389</v>
+      </c>
+      <c r="X49" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="Y49" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="Z49" s="2" t="s">
+        <v>389</v>
+      </c>
+      <c r="AA49" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="AB49" s="2" t="s">
+        <v>441</v>
+      </c>
+    </row>
+    <row r="50" spans="1:28" hidden="1" x14ac:dyDescent="0.2">
       <c r="A50" s="3" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="51" spans="1:22" hidden="1" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:28" hidden="1" x14ac:dyDescent="0.2">
       <c r="A51" s="3" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="52" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:28" x14ac:dyDescent="0.2">
       <c r="B52" s="2"/>
       <c r="C52" s="2"/>
       <c r="D52" s="2"/>
@@ -4709,8 +5812,10 @@
       <c r="T52" s="2"/>
       <c r="U52" s="2"/>
       <c r="V52" s="2"/>
-    </row>
-    <row r="53" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="X52" s="2"/>
+      <c r="Y52" s="2"/>
+    </row>
+    <row r="53" spans="1:28" x14ac:dyDescent="0.2">
       <c r="B53" s="2"/>
       <c r="C53" s="2"/>
       <c r="D53" s="2"/>
@@ -4732,8 +5837,9 @@
       <c r="T53" s="2"/>
       <c r="U53" s="2"/>
       <c r="V53" s="2"/>
-    </row>
-    <row r="54" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="X53" s="2"/>
+    </row>
+    <row r="54" spans="1:28" x14ac:dyDescent="0.2">
       <c r="B54" s="2"/>
       <c r="C54" s="2"/>
       <c r="D54" s="2"/>
@@ -4755,8 +5861,9 @@
       <c r="T54" s="2"/>
       <c r="U54" s="2"/>
       <c r="V54" s="2"/>
-    </row>
-    <row r="55" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="X54" s="2"/>
+    </row>
+    <row r="55" spans="1:28" x14ac:dyDescent="0.2">
       <c r="B55" s="2"/>
       <c r="C55" s="2"/>
       <c r="D55" s="2"/>
@@ -4778,8 +5885,9 @@
       <c r="T55" s="2"/>
       <c r="U55" s="2"/>
       <c r="V55" s="2"/>
-    </row>
-    <row r="56" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="X55" s="2"/>
+    </row>
+    <row r="56" spans="1:28" x14ac:dyDescent="0.2">
       <c r="B56" s="2"/>
       <c r="C56" s="2"/>
       <c r="D56" s="2"/>
@@ -4802,7 +5910,7 @@
       <c r="U56" s="2"/>
       <c r="V56" s="2"/>
     </row>
-    <row r="57" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:28" x14ac:dyDescent="0.2">
       <c r="B57" s="2"/>
       <c r="C57" s="2"/>
       <c r="D57" s="2"/>
@@ -4825,7 +5933,7 @@
       <c r="U57" s="2"/>
       <c r="V57" s="2"/>
     </row>
-    <row r="58" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:28" x14ac:dyDescent="0.2">
       <c r="B58" s="2"/>
       <c r="C58" s="2"/>
       <c r="D58" s="2"/>
@@ -4848,7 +5956,7 @@
       <c r="U58" s="2"/>
       <c r="V58" s="2"/>
     </row>
-    <row r="59" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:28" x14ac:dyDescent="0.2">
       <c r="B59" s="2"/>
       <c r="C59" s="2"/>
       <c r="D59" s="2"/>
@@ -4871,7 +5979,7 @@
       <c r="U59" s="2"/>
       <c r="V59" s="2"/>
     </row>
-    <row r="60" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:28" x14ac:dyDescent="0.2">
       <c r="B60" s="2"/>
       <c r="C60" s="2"/>
       <c r="D60" s="2"/>
@@ -4894,7 +6002,7 @@
       <c r="U60" s="2"/>
       <c r="V60" s="2"/>
     </row>
-    <row r="61" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:28" x14ac:dyDescent="0.2">
       <c r="B61" s="2"/>
       <c r="C61" s="2"/>
       <c r="D61" s="2"/>
@@ -4917,7 +6025,7 @@
       <c r="U61" s="2"/>
       <c r="V61" s="2"/>
     </row>
-    <row r="62" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:28" x14ac:dyDescent="0.2">
       <c r="B62" s="2"/>
       <c r="C62" s="2"/>
       <c r="D62" s="2"/>
@@ -4940,7 +6048,7 @@
       <c r="U62" s="2"/>
       <c r="V62" s="2"/>
     </row>
-    <row r="63" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:28" x14ac:dyDescent="0.2">
       <c r="B63" s="2"/>
       <c r="C63" s="2"/>
       <c r="D63" s="2"/>
@@ -4963,7 +6071,7 @@
       <c r="U63" s="2"/>
       <c r="V63" s="2"/>
     </row>
-    <row r="64" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:28" x14ac:dyDescent="0.2">
       <c r="B64" s="2"/>
       <c r="C64" s="2"/>
       <c r="D64" s="2"/>
@@ -5045,8 +6153,8 @@
   <dimension ref="A1:Z65"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane xSplit="1" topLeftCell="D1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="I18" sqref="I18"/>
+      <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="K37" sqref="K37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -5095,7 +6203,9 @@
       <c r="J1" s="1" t="s">
         <v>332</v>
       </c>
-      <c r="K1" s="1"/>
+      <c r="K1" s="1" t="s">
+        <v>406</v>
+      </c>
       <c r="L1" s="1"/>
       <c r="M1" s="1"/>
       <c r="N1" s="1"/>
@@ -5143,7 +6253,9 @@
       <c r="J2" s="2" t="s">
         <v>333</v>
       </c>
-      <c r="K2" s="2"/>
+      <c r="K2" s="2" t="s">
+        <v>80</v>
+      </c>
       <c r="L2" s="2"/>
       <c r="M2" s="2"/>
       <c r="N2" s="2"/>
@@ -5457,7 +6569,9 @@
         <v>380</v>
       </c>
       <c r="J18" s="2"/>
-      <c r="K18" s="2"/>
+      <c r="K18" s="2" t="s">
+        <v>80</v>
+      </c>
       <c r="L18" s="2"/>
       <c r="M18" s="2"/>
       <c r="N18" s="2"/>
@@ -5609,7 +6723,7 @@
       <c r="T34" s="2"/>
       <c r="U34" s="2"/>
     </row>
-    <row r="35" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:21" hidden="1" x14ac:dyDescent="0.2">
       <c r="A35" s="3" t="s">
         <v>41</v>
       </c>
@@ -5639,20 +6753,30 @@
         <v>42</v>
       </c>
     </row>
-    <row r="37" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:21" ht="51" x14ac:dyDescent="0.2">
       <c r="A37" s="3" t="s">
         <v>43</v>
       </c>
-      <c r="B37" s="2"/>
-      <c r="C37" s="2"/>
-      <c r="D37" s="2"/>
+      <c r="B37" s="2" t="s">
+        <v>411</v>
+      </c>
+      <c r="C37" s="2" t="s">
+        <v>411</v>
+      </c>
+      <c r="D37" s="2" t="s">
+        <v>410</v>
+      </c>
       <c r="E37" s="2"/>
       <c r="F37" s="2"/>
       <c r="G37" s="2"/>
       <c r="H37" s="2"/>
-      <c r="I37" s="2"/>
+      <c r="I37" s="2" t="s">
+        <v>409</v>
+      </c>
       <c r="J37" s="2"/>
-      <c r="K37" s="2"/>
+      <c r="K37" s="2" t="s">
+        <v>410</v>
+      </c>
       <c r="L37" s="2"/>
       <c r="M37" s="2"/>
       <c r="N37" s="2"/>
@@ -5669,7 +6793,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="39" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:21" hidden="1" x14ac:dyDescent="0.2">
       <c r="A39" s="3" t="s">
         <v>45</v>
       </c>
@@ -5704,7 +6828,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="42" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:21" hidden="1" x14ac:dyDescent="0.2">
       <c r="A42" s="3" t="s">
         <v>48</v>
       </c>
@@ -5734,7 +6858,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="44" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:21" hidden="1" x14ac:dyDescent="0.2">
       <c r="A44" s="3" t="s">
         <v>50</v>
       </c>
@@ -6168,11 +7292,7 @@
       <filters>
         <filter val="Alabama"/>
         <filter val="Kentucky"/>
-        <filter val="North Dakota"/>
         <filter val="Oklahoma"/>
-        <filter val="Pennsylvania"/>
-        <filter val="South Dakota"/>
-        <filter val="Texas"/>
         <filter val="Utah"/>
         <filter val="Vermont"/>
         <filter val="West Virginia"/>
@@ -6188,9 +7308,9 @@
   <sheetPr filterMode="1"/>
   <dimension ref="A1:AB65"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="B16" sqref="B16"/>
+      <selection pane="topRight" activeCell="F49" sqref="F49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -6762,7 +7882,7 @@
       <c r="V34" s="2"/>
       <c r="W34" s="2"/>
     </row>
-    <row r="35" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:23" hidden="1" x14ac:dyDescent="0.2">
       <c r="A35" s="3" t="s">
         <v>41</v>
       </c>
@@ -6794,15 +7914,23 @@
         <v>42</v>
       </c>
     </row>
-    <row r="37" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:23" ht="17" x14ac:dyDescent="0.2">
       <c r="A37" s="3" t="s">
         <v>43</v>
       </c>
-      <c r="B37" s="2"/>
-      <c r="C37" s="2"/>
-      <c r="D37" s="2"/>
+      <c r="B37" s="2" t="s">
+        <v>416</v>
+      </c>
+      <c r="C37" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="D37" s="2" t="s">
+        <v>80</v>
+      </c>
       <c r="E37" s="2"/>
-      <c r="F37" s="2"/>
+      <c r="F37" s="2" t="s">
+        <v>341</v>
+      </c>
       <c r="G37" s="2"/>
       <c r="H37" s="2"/>
       <c r="I37" s="2"/>
@@ -6826,15 +7954,23 @@
         <v>44</v>
       </c>
     </row>
-    <row r="39" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:23" ht="51" x14ac:dyDescent="0.2">
       <c r="A39" s="3" t="s">
         <v>45</v>
       </c>
-      <c r="B39" s="2"/>
-      <c r="C39" s="2"/>
-      <c r="D39" s="2"/>
+      <c r="B39" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="C39" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="D39" s="2" t="s">
+        <v>417</v>
+      </c>
       <c r="E39" s="2"/>
-      <c r="F39" s="2"/>
+      <c r="F39" s="2" t="s">
+        <v>418</v>
+      </c>
       <c r="G39" s="2"/>
       <c r="H39" s="2"/>
       <c r="I39" s="2"/>
@@ -6863,15 +7999,23 @@
         <v>47</v>
       </c>
     </row>
-    <row r="42" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:23" ht="17" x14ac:dyDescent="0.2">
       <c r="A42" s="3" t="s">
         <v>48</v>
       </c>
-      <c r="B42" s="2"/>
-      <c r="C42" s="2"/>
-      <c r="D42" s="2"/>
+      <c r="B42" s="2" t="s">
+        <v>421</v>
+      </c>
+      <c r="C42" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="D42" s="2" t="s">
+        <v>80</v>
+      </c>
       <c r="E42" s="2"/>
-      <c r="F42" s="2"/>
+      <c r="F42" s="2" t="s">
+        <v>341</v>
+      </c>
       <c r="G42" s="2"/>
       <c r="H42" s="2"/>
       <c r="I42" s="2"/>
@@ -6895,15 +8039,23 @@
         <v>49</v>
       </c>
     </row>
-    <row r="44" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:23" ht="17" x14ac:dyDescent="0.2">
       <c r="A44" s="3" t="s">
         <v>50</v>
       </c>
-      <c r="B44" s="2"/>
-      <c r="C44" s="2"/>
-      <c r="D44" s="2"/>
+      <c r="B44" s="2" t="s">
+        <v>432</v>
+      </c>
+      <c r="C44" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="D44" s="2" t="s">
+        <v>80</v>
+      </c>
       <c r="E44" s="2"/>
-      <c r="F44" s="2"/>
+      <c r="F44" s="2" t="s">
+        <v>341</v>
+      </c>
       <c r="G44" s="2"/>
       <c r="H44" s="2"/>
       <c r="I44" s="2"/>
@@ -6922,15 +8074,23 @@
       <c r="V44" s="2"/>
       <c r="W44" s="2"/>
     </row>
-    <row r="45" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:23" ht="17" x14ac:dyDescent="0.2">
       <c r="A45" s="3" t="s">
         <v>51</v>
       </c>
-      <c r="B45" s="2"/>
-      <c r="C45" s="2"/>
-      <c r="D45" s="2"/>
+      <c r="B45" s="2" t="s">
+        <v>435</v>
+      </c>
+      <c r="C45" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="D45" s="2" t="s">
+        <v>80</v>
+      </c>
       <c r="E45" s="2"/>
-      <c r="F45" s="2"/>
+      <c r="F45" s="2" t="s">
+        <v>341</v>
+      </c>
       <c r="G45" s="2"/>
       <c r="H45" s="2"/>
       <c r="I45" s="2"/>
@@ -6949,15 +8109,23 @@
       <c r="V45" s="2"/>
       <c r="W45" s="2"/>
     </row>
-    <row r="46" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:23" ht="17" x14ac:dyDescent="0.2">
       <c r="A46" s="3" t="s">
         <v>52</v>
       </c>
-      <c r="B46" s="2"/>
-      <c r="C46" s="2"/>
-      <c r="D46" s="2"/>
+      <c r="B46" s="2" t="s">
+        <v>439</v>
+      </c>
+      <c r="C46" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="D46" s="2" t="s">
+        <v>80</v>
+      </c>
       <c r="E46" s="2"/>
-      <c r="F46" s="2"/>
+      <c r="F46" s="2" t="s">
+        <v>341</v>
+      </c>
       <c r="G46" s="2"/>
       <c r="H46" s="2"/>
       <c r="I46" s="2"/>
@@ -6986,15 +8154,19 @@
         <v>54</v>
       </c>
     </row>
-    <row r="49" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:23" ht="17" x14ac:dyDescent="0.2">
       <c r="A49" s="3" t="s">
         <v>55</v>
       </c>
-      <c r="B49" s="2"/>
+      <c r="B49" s="2" t="s">
+        <v>445</v>
+      </c>
       <c r="C49" s="2"/>
       <c r="D49" s="2"/>
       <c r="E49" s="2"/>
-      <c r="F49" s="2"/>
+      <c r="F49" s="2" t="s">
+        <v>341</v>
+      </c>
       <c r="G49" s="2"/>
       <c r="H49" s="2"/>
       <c r="I49" s="2"/>
@@ -7369,7 +8541,6 @@
         <filter val="Kansas"/>
         <filter val="Kentucky"/>
         <filter val="Mississippi"/>
-        <filter val="North Dakota"/>
         <filter val="Oklahoma"/>
         <filter val="Pennsylvania"/>
         <filter val="South Dakota"/>

</xml_diff>